<commit_message>
Zeitplan angepasst und fertiggestellt.
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2060" windowWidth="28620" windowHeight="18580"/>
+    <workbookView xWindow="740" yWindow="2160" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>Zusammenfassung Konzept</t>
   </si>
   <si>
-    <t>Vorkenntnisse / Vorarbeiten / Firmenstandards / Meilensteine / Organisaiton des Projekts erfassen</t>
-  </si>
-  <si>
     <t>Vorgehensziele / Systemziele / 
 Anwendungsbereich /  Anforderungen</t>
   </si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>Projektjournal</t>
+  </si>
+  <si>
+    <t>Vorkenntnisse / Vorarbeiten / Firmenstandards / Meilensteine und Organisation der IPA erfassen</t>
   </si>
 </sst>
 </file>
@@ -1061,6 +1061,126 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1073,61 +1193,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1142,24 +1223,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1173,69 +1236,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1768,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1814,50 +1814,50 @@
     </row>
     <row r="2" spans="1:26" ht="23" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="99" t="s">
+      <c r="B2" s="106"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="96"/>
-      <c r="H2" s="99" t="s">
+      <c r="G2" s="124"/>
+      <c r="H2" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="96" t="s">
+      <c r="I2" s="129"/>
+      <c r="J2" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="96"/>
-      <c r="L2" s="99" t="s">
+      <c r="K2" s="124"/>
+      <c r="L2" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="100"/>
-      <c r="N2" s="96" t="s">
+      <c r="M2" s="129"/>
+      <c r="N2" s="124" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="96"/>
-      <c r="P2" s="99" t="s">
+      <c r="O2" s="124"/>
+      <c r="P2" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="96" t="s">
+      <c r="Q2" s="129"/>
+      <c r="R2" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="96"/>
-      <c r="T2" s="99" t="s">
+      <c r="S2" s="124"/>
+      <c r="T2" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="100"/>
-      <c r="V2" s="96" t="s">
+      <c r="U2" s="129"/>
+      <c r="V2" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="96"/>
-      <c r="X2" s="99" t="s">
+      <c r="W2" s="124"/>
+      <c r="X2" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="100"/>
+      <c r="Y2" s="129"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="14" customHeight="1">
@@ -1868,26 +1868,26 @@
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="102"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="101"/>
-      <c r="U3" s="102"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="101"/>
-      <c r="Y3" s="102"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="125"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="125"/>
+      <c r="U3" s="130"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="126"/>
+      <c r="X3" s="125"/>
+      <c r="Y3" s="130"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="14" customHeight="1">
@@ -1898,86 +1898,86 @@
       <c r="C4" s="3"/>
       <c r="D4" s="8"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="97"/>
-      <c r="X4" s="101"/>
-      <c r="Y4" s="102"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="126"/>
+      <c r="O4" s="126"/>
+      <c r="P4" s="125"/>
+      <c r="Q4" s="130"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+      <c r="T4" s="125"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="126"/>
+      <c r="W4" s="126"/>
+      <c r="X4" s="125"/>
+      <c r="Y4" s="130"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="20" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="141"/>
-      <c r="C5" s="142"/>
-      <c r="D5" s="142"/>
-      <c r="E5" s="142"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="140"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="140"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="140"/>
-      <c r="R5" s="98"/>
-      <c r="S5" s="98"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="140"/>
-      <c r="V5" s="98"/>
-      <c r="W5" s="98"/>
-      <c r="X5" s="103"/>
-      <c r="Y5" s="98"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="128"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="131"/>
+      <c r="N5" s="128"/>
+      <c r="O5" s="128"/>
+      <c r="P5" s="127"/>
+      <c r="Q5" s="131"/>
+      <c r="R5" s="128"/>
+      <c r="S5" s="128"/>
+      <c r="T5" s="127"/>
+      <c r="U5" s="131"/>
+      <c r="V5" s="128"/>
+      <c r="W5" s="128"/>
+      <c r="X5" s="127"/>
+      <c r="Y5" s="128"/>
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="10" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="146"/>
-      <c r="D6" s="147"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="110"/>
       <c r="E6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="104"/>
-      <c r="O6" s="105"/>
-      <c r="P6" s="104"/>
-      <c r="Q6" s="105"/>
-      <c r="R6" s="104"/>
-      <c r="S6" s="105"/>
-      <c r="T6" s="104"/>
-      <c r="U6" s="105"/>
-      <c r="V6" s="104"/>
-      <c r="W6" s="105"/>
-      <c r="X6" s="104"/>
-      <c r="Y6" s="105"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="122"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="122"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="122"/>
+      <c r="T6" s="121"/>
+      <c r="U6" s="122"/>
+      <c r="V6" s="121"/>
+      <c r="W6" s="122"/>
+      <c r="X6" s="121"/>
+      <c r="Y6" s="122"/>
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
@@ -2000,11 +2000,11 @@
     </row>
     <row r="8" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="107"/>
-      <c r="D8" s="108"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="114"/>
       <c r="E8" s="14">
         <v>7.5</v>
       </c>
@@ -2033,11 +2033,11 @@
     <row r="9" spans="1:26" ht="10" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="120"/>
-      <c r="E9" s="121"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="100"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
       <c r="H9" s="19"/>
@@ -2063,9 +2063,9 @@
     <row r="10" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A10" s="1"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="123"/>
-      <c r="E10" s="124"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="103"/>
       <c r="F10" s="24"/>
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
@@ -2091,11 +2091,11 @@
     <row r="11" spans="1:26" ht="10" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="119" t="s">
+      <c r="C11" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="121"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="100"/>
       <c r="F11" s="27"/>
       <c r="G11" s="25"/>
       <c r="H11" s="26"/>
@@ -2121,9 +2121,9 @@
     <row r="12" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A12" s="1"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="122"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="124"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="103"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
@@ -2149,11 +2149,11 @@
     <row r="13" spans="1:26" ht="10" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="119" t="s">
+      <c r="C13" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="120"/>
-      <c r="E13" s="121"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="100"/>
       <c r="F13" s="17"/>
       <c r="G13" s="25"/>
       <c r="H13" s="26"/>
@@ -2179,9 +2179,9 @@
     <row r="14" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A14" s="1"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="122"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="124"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
       <c r="H14" s="26"/>
@@ -2207,11 +2207,11 @@
     <row r="15" spans="1:26" ht="10" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="136" t="s">
+      <c r="C15" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="120"/>
-      <c r="E15" s="121"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="100"/>
       <c r="F15" s="17"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
@@ -2237,9 +2237,9 @@
     <row r="16" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="124"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="103"/>
       <c r="F16" s="24"/>
       <c r="G16" s="25"/>
       <c r="H16" s="26"/>
@@ -2265,11 +2265,11 @@
     <row r="17" spans="1:26" ht="10" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="119" t="s">
+      <c r="C17" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="120"/>
-      <c r="E17" s="121"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="100"/>
       <c r="F17" s="27"/>
       <c r="G17" s="25"/>
       <c r="H17" s="26"/>
@@ -2295,9 +2295,9 @@
     <row r="18" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A18" s="1"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="122"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="124"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="103"/>
       <c r="F18" s="24"/>
       <c r="G18" s="28"/>
       <c r="H18" s="26"/>
@@ -2323,11 +2323,11 @@
     <row r="19" spans="1:26" ht="10" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="120"/>
-      <c r="E19" s="121"/>
+      <c r="D19" s="99"/>
+      <c r="E19" s="100"/>
       <c r="F19" s="29"/>
       <c r="G19" s="30"/>
       <c r="H19" s="26"/>
@@ -2353,11 +2353,11 @@
     <row r="20" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A20" s="1"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="122"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="124"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="103"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="25"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="26"/>
       <c r="I20" s="20"/>
       <c r="J20" s="21"/>
@@ -2381,11 +2381,11 @@
     <row r="21" spans="1:26" ht="10" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="136" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="120"/>
-      <c r="E21" s="121"/>
+      <c r="C21" s="111" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="99"/>
+      <c r="E21" s="100"/>
       <c r="F21" s="19"/>
       <c r="G21" s="31"/>
       <c r="H21" s="26"/>
@@ -2411,11 +2411,11 @@
     <row r="22" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A22" s="1"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="122"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="124"/>
+      <c r="C22" s="101"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="103"/>
       <c r="F22" s="29"/>
-      <c r="G22" s="50"/>
+      <c r="G22" s="32"/>
       <c r="H22" s="26"/>
       <c r="I22" s="20"/>
       <c r="J22" s="21"/>
@@ -2438,9 +2438,9 @@
     </row>
     <row r="23" spans="1:26" ht="10" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="112"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="114"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="120"/>
       <c r="E23" s="33">
         <v>8.5</v>
       </c>
@@ -2485,11 +2485,11 @@
     </row>
     <row r="25" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="109" t="s">
+      <c r="B25" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="110"/>
-      <c r="D25" s="111"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="117"/>
       <c r="E25" s="36">
         <v>7.5</v>
       </c>
@@ -2518,11 +2518,11 @@
     <row r="26" spans="1:26" ht="10" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="40"/>
-      <c r="C26" s="119" t="s">
+      <c r="C26" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="120"/>
-      <c r="E26" s="121"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="100"/>
       <c r="F26" s="41"/>
       <c r="G26" s="42"/>
       <c r="H26" s="43"/>
@@ -2548,11 +2548,11 @@
     <row r="27" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A27" s="1"/>
       <c r="B27" s="40"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="124"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="102"/>
+      <c r="E27" s="103"/>
       <c r="F27" s="48"/>
-      <c r="G27" s="50"/>
+      <c r="G27" s="32"/>
       <c r="H27" s="51"/>
       <c r="I27" s="44"/>
       <c r="J27" s="45"/>
@@ -2576,11 +2576,11 @@
     <row r="28" spans="1:26" ht="10" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="40"/>
-      <c r="C28" s="136" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="120"/>
-      <c r="E28" s="121"/>
+      <c r="C28" s="111" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="99"/>
+      <c r="E28" s="100"/>
       <c r="F28" s="48"/>
       <c r="G28" s="50"/>
       <c r="H28" s="43"/>
@@ -2606,9 +2606,9 @@
     <row r="29" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A29" s="1"/>
       <c r="B29" s="40"/>
-      <c r="C29" s="122"/>
-      <c r="D29" s="123"/>
-      <c r="E29" s="124"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="103"/>
       <c r="F29" s="48"/>
       <c r="G29" s="50"/>
       <c r="H29" s="51"/>
@@ -2634,11 +2634,11 @@
     <row r="30" spans="1:26" ht="10" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="40"/>
-      <c r="C30" s="119" t="s">
+      <c r="C30" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="120"/>
-      <c r="E30" s="121"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="100"/>
       <c r="F30" s="47"/>
       <c r="G30" s="18"/>
       <c r="H30" s="43"/>
@@ -2664,9 +2664,9 @@
     <row r="31" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A31" s="1"/>
       <c r="B31" s="40"/>
-      <c r="C31" s="122"/>
-      <c r="D31" s="123"/>
-      <c r="E31" s="124"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="103"/>
       <c r="F31" s="47"/>
       <c r="G31" s="50"/>
       <c r="H31" s="51"/>
@@ -2692,11 +2692,11 @@
     <row r="32" spans="1:26" ht="10" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="40"/>
-      <c r="C32" s="136" t="s">
+      <c r="C32" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="120"/>
-      <c r="E32" s="121"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="100"/>
       <c r="F32" s="47"/>
       <c r="G32" s="18"/>
       <c r="H32" s="19"/>
@@ -2722,9 +2722,9 @@
     <row r="33" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A33" s="1"/>
       <c r="B33" s="40"/>
-      <c r="C33" s="122"/>
-      <c r="D33" s="123"/>
-      <c r="E33" s="124"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="102"/>
+      <c r="E33" s="103"/>
       <c r="F33" s="47"/>
       <c r="G33" s="50"/>
       <c r="H33" s="29"/>
@@ -2750,11 +2750,11 @@
     <row r="34" spans="1:26" ht="10" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="40"/>
-      <c r="C34" s="119" t="s">
+      <c r="C34" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="120"/>
-      <c r="E34" s="121"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="100"/>
       <c r="F34" s="47"/>
       <c r="G34" s="54"/>
       <c r="H34" s="19"/>
@@ -2780,9 +2780,9 @@
     <row r="35" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A35" s="1"/>
       <c r="B35" s="40"/>
-      <c r="C35" s="122"/>
-      <c r="D35" s="123"/>
-      <c r="E35" s="124"/>
+      <c r="C35" s="101"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="103"/>
       <c r="F35" s="47"/>
       <c r="G35" s="55"/>
       <c r="H35" s="29"/>
@@ -2807,9 +2807,9 @@
     </row>
     <row r="36" spans="1:26" ht="10" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="115"/>
-      <c r="C36" s="116"/>
-      <c r="D36" s="117"/>
+      <c r="B36" s="142"/>
+      <c r="C36" s="143"/>
+      <c r="D36" s="144"/>
       <c r="E36" s="56">
         <v>7</v>
       </c>
@@ -2854,11 +2854,11 @@
     </row>
     <row r="38" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="148" t="s">
+      <c r="B38" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="149"/>
-      <c r="D38" s="150"/>
+      <c r="C38" s="140"/>
+      <c r="D38" s="141"/>
       <c r="E38" s="57">
         <v>12</v>
       </c>
@@ -2887,11 +2887,11 @@
     <row r="39" spans="1:26" ht="10" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="61"/>
-      <c r="C39" s="119" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="120"/>
-      <c r="E39" s="121"/>
+      <c r="C39" s="98" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="99"/>
+      <c r="E39" s="100"/>
       <c r="F39" s="47"/>
       <c r="G39" s="62"/>
       <c r="H39" s="47"/>
@@ -2917,9 +2917,9 @@
     <row r="40" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A40" s="1"/>
       <c r="B40" s="61"/>
-      <c r="C40" s="122"/>
-      <c r="D40" s="123"/>
-      <c r="E40" s="124"/>
+      <c r="C40" s="101"/>
+      <c r="D40" s="102"/>
+      <c r="E40" s="103"/>
       <c r="F40" s="47"/>
       <c r="G40" s="62"/>
       <c r="H40" s="47"/>
@@ -2945,11 +2945,11 @@
     <row r="41" spans="1:26" ht="10" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="61"/>
-      <c r="C41" s="119" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="120"/>
-      <c r="E41" s="121"/>
+      <c r="C41" s="98" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="99"/>
+      <c r="E41" s="100"/>
       <c r="F41" s="47"/>
       <c r="G41" s="62"/>
       <c r="H41" s="47"/>
@@ -2975,9 +2975,9 @@
     <row r="42" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A42" s="1"/>
       <c r="B42" s="61"/>
-      <c r="C42" s="122"/>
-      <c r="D42" s="123"/>
-      <c r="E42" s="124"/>
+      <c r="C42" s="101"/>
+      <c r="D42" s="102"/>
+      <c r="E42" s="103"/>
       <c r="F42" s="47"/>
       <c r="G42" s="62"/>
       <c r="H42" s="47"/>
@@ -3003,11 +3003,11 @@
     <row r="43" spans="1:26" ht="10" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="61"/>
-      <c r="C43" s="119" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="120"/>
-      <c r="E43" s="121"/>
+      <c r="C43" s="98" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="99"/>
+      <c r="E43" s="100"/>
       <c r="F43" s="47"/>
       <c r="G43" s="62"/>
       <c r="H43" s="47"/>
@@ -3033,9 +3033,9 @@
     <row r="44" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A44" s="1"/>
       <c r="B44" s="61"/>
-      <c r="C44" s="122"/>
-      <c r="D44" s="123"/>
-      <c r="E44" s="124"/>
+      <c r="C44" s="101"/>
+      <c r="D44" s="102"/>
+      <c r="E44" s="103"/>
       <c r="F44" s="47"/>
       <c r="G44" s="62"/>
       <c r="H44" s="47"/>
@@ -3061,11 +3061,11 @@
     <row r="45" spans="1:26" ht="10" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="61"/>
-      <c r="C45" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" s="120"/>
-      <c r="E45" s="121"/>
+      <c r="C45" s="98" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="99"/>
+      <c r="E45" s="100"/>
       <c r="F45" s="47"/>
       <c r="G45" s="62"/>
       <c r="H45" s="47"/>
@@ -3091,9 +3091,9 @@
     <row r="46" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A46" s="1"/>
       <c r="B46" s="61"/>
-      <c r="C46" s="122"/>
-      <c r="D46" s="123"/>
-      <c r="E46" s="124"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="102"/>
+      <c r="E46" s="103"/>
       <c r="F46" s="47"/>
       <c r="G46" s="62"/>
       <c r="H46" s="47"/>
@@ -3119,11 +3119,11 @@
     <row r="47" spans="1:26" ht="10" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="61"/>
-      <c r="C47" s="119" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="120"/>
-      <c r="E47" s="121"/>
+      <c r="C47" s="98" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="99"/>
+      <c r="E47" s="100"/>
       <c r="F47" s="47"/>
       <c r="G47" s="62"/>
       <c r="H47" s="47"/>
@@ -3149,9 +3149,9 @@
     <row r="48" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A48" s="1"/>
       <c r="B48" s="61"/>
-      <c r="C48" s="122"/>
-      <c r="D48" s="123"/>
-      <c r="E48" s="124"/>
+      <c r="C48" s="101"/>
+      <c r="D48" s="102"/>
+      <c r="E48" s="103"/>
       <c r="F48" s="47"/>
       <c r="G48" s="62"/>
       <c r="H48" s="47"/>
@@ -3177,11 +3177,11 @@
     <row r="49" spans="1:26" ht="10" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="61"/>
-      <c r="C49" s="119" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="120"/>
-      <c r="E49" s="121"/>
+      <c r="C49" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="99"/>
+      <c r="E49" s="100"/>
       <c r="F49" s="47"/>
       <c r="G49" s="62"/>
       <c r="H49" s="47"/>
@@ -3207,9 +3207,9 @@
     <row r="50" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A50" s="1"/>
       <c r="B50" s="61"/>
-      <c r="C50" s="122"/>
-      <c r="D50" s="123"/>
-      <c r="E50" s="124"/>
+      <c r="C50" s="101"/>
+      <c r="D50" s="102"/>
+      <c r="E50" s="103"/>
       <c r="F50" s="47"/>
       <c r="G50" s="62"/>
       <c r="H50" s="47"/>
@@ -3235,11 +3235,11 @@
     <row r="51" spans="1:26" ht="10" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="61"/>
-      <c r="C51" s="119" t="s">
+      <c r="C51" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="D51" s="120"/>
-      <c r="E51" s="121"/>
+      <c r="D51" s="99"/>
+      <c r="E51" s="100"/>
       <c r="F51" s="47"/>
       <c r="G51" s="62"/>
       <c r="H51" s="47"/>
@@ -3265,9 +3265,9 @@
     <row r="52" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A52" s="1"/>
       <c r="B52" s="61"/>
-      <c r="C52" s="122"/>
-      <c r="D52" s="123"/>
-      <c r="E52" s="124"/>
+      <c r="C52" s="101"/>
+      <c r="D52" s="102"/>
+      <c r="E52" s="103"/>
       <c r="F52" s="47"/>
       <c r="G52" s="62"/>
       <c r="H52" s="47"/>
@@ -3293,11 +3293,11 @@
     <row r="53" spans="1:26" ht="10" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="61"/>
-      <c r="C53" s="119" t="s">
+      <c r="C53" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="120"/>
-      <c r="E53" s="121"/>
+      <c r="D53" s="99"/>
+      <c r="E53" s="100"/>
       <c r="F53" s="47"/>
       <c r="G53" s="62"/>
       <c r="H53" s="47"/>
@@ -3323,9 +3323,9 @@
     <row r="54" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A54" s="1"/>
       <c r="B54" s="61"/>
-      <c r="C54" s="122"/>
-      <c r="D54" s="123"/>
-      <c r="E54" s="124"/>
+      <c r="C54" s="101"/>
+      <c r="D54" s="102"/>
+      <c r="E54" s="103"/>
       <c r="F54" s="47"/>
       <c r="G54" s="62"/>
       <c r="H54" s="47"/>
@@ -3351,11 +3351,11 @@
     <row r="55" spans="1:26" ht="10" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="61"/>
-      <c r="C55" s="119" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="120"/>
-      <c r="E55" s="121"/>
+      <c r="C55" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="99"/>
+      <c r="E55" s="100"/>
       <c r="F55" s="47"/>
       <c r="G55" s="62"/>
       <c r="H55" s="47"/>
@@ -3381,9 +3381,9 @@
     <row r="56" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A56" s="1"/>
       <c r="B56" s="61"/>
-      <c r="C56" s="122"/>
-      <c r="D56" s="123"/>
-      <c r="E56" s="124"/>
+      <c r="C56" s="101"/>
+      <c r="D56" s="102"/>
+      <c r="E56" s="103"/>
       <c r="F56" s="47"/>
       <c r="G56" s="62"/>
       <c r="H56" s="47"/>
@@ -3408,9 +3408,9 @@
     </row>
     <row r="57" spans="1:26" ht="10" customHeight="1">
       <c r="A57" s="1"/>
-      <c r="B57" s="133"/>
-      <c r="C57" s="134"/>
-      <c r="D57" s="135"/>
+      <c r="B57" s="136"/>
+      <c r="C57" s="137"/>
+      <c r="D57" s="138"/>
       <c r="E57" s="66"/>
       <c r="F57" s="58"/>
       <c r="G57" s="59"/>
@@ -3486,11 +3486,11 @@
     <row r="60" spans="1:26" ht="10" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="83"/>
-      <c r="C60" s="119" t="s">
+      <c r="C60" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="D60" s="120"/>
-      <c r="E60" s="121"/>
+      <c r="D60" s="99"/>
+      <c r="E60" s="100"/>
       <c r="F60" s="47"/>
       <c r="G60" s="62"/>
       <c r="H60" s="47"/>
@@ -3516,9 +3516,9 @@
     <row r="61" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A61" s="1"/>
       <c r="B61" s="83"/>
-      <c r="C61" s="122"/>
-      <c r="D61" s="123"/>
-      <c r="E61" s="124"/>
+      <c r="C61" s="101"/>
+      <c r="D61" s="102"/>
+      <c r="E61" s="103"/>
       <c r="F61" s="47"/>
       <c r="G61" s="62"/>
       <c r="H61" s="47"/>
@@ -3544,11 +3544,11 @@
     <row r="62" spans="1:26" ht="10" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="83"/>
-      <c r="C62" s="119" t="s">
+      <c r="C62" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="D62" s="120"/>
-      <c r="E62" s="121"/>
+      <c r="D62" s="99"/>
+      <c r="E62" s="100"/>
       <c r="F62" s="47"/>
       <c r="G62" s="62"/>
       <c r="H62" s="47"/>
@@ -3574,9 +3574,9 @@
     <row r="63" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A63" s="1"/>
       <c r="B63" s="83"/>
-      <c r="C63" s="122"/>
-      <c r="D63" s="123"/>
-      <c r="E63" s="124"/>
+      <c r="C63" s="101"/>
+      <c r="D63" s="102"/>
+      <c r="E63" s="103"/>
       <c r="F63" s="47"/>
       <c r="G63" s="62"/>
       <c r="H63" s="47"/>
@@ -3602,11 +3602,11 @@
     <row r="64" spans="1:26" ht="10" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="83"/>
-      <c r="C64" s="119" t="s">
+      <c r="C64" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="120"/>
-      <c r="E64" s="121"/>
+      <c r="D64" s="99"/>
+      <c r="E64" s="100"/>
       <c r="F64" s="47"/>
       <c r="G64" s="62"/>
       <c r="H64" s="47"/>
@@ -3632,9 +3632,9 @@
     <row r="65" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A65" s="1"/>
       <c r="B65" s="83"/>
-      <c r="C65" s="122"/>
-      <c r="D65" s="123"/>
-      <c r="E65" s="124"/>
+      <c r="C65" s="101"/>
+      <c r="D65" s="102"/>
+      <c r="E65" s="103"/>
       <c r="F65" s="47"/>
       <c r="G65" s="62"/>
       <c r="H65" s="47"/>
@@ -3660,11 +3660,11 @@
     <row r="66" spans="1:26" ht="10" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="83"/>
-      <c r="C66" s="119" t="s">
+      <c r="C66" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="D66" s="120"/>
-      <c r="E66" s="121"/>
+      <c r="D66" s="99"/>
+      <c r="E66" s="100"/>
       <c r="F66" s="47"/>
       <c r="G66" s="62"/>
       <c r="H66" s="47"/>
@@ -3690,9 +3690,9 @@
     <row r="67" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A67" s="1"/>
       <c r="B67" s="83"/>
-      <c r="C67" s="122"/>
-      <c r="D67" s="123"/>
-      <c r="E67" s="124"/>
+      <c r="C67" s="101"/>
+      <c r="D67" s="102"/>
+      <c r="E67" s="103"/>
       <c r="F67" s="47"/>
       <c r="G67" s="62"/>
       <c r="H67" s="47"/>
@@ -3718,11 +3718,11 @@
     <row r="68" spans="1:26" ht="10" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="83"/>
-      <c r="C68" s="119" t="s">
+      <c r="C68" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="D68" s="120"/>
-      <c r="E68" s="121"/>
+      <c r="D68" s="99"/>
+      <c r="E68" s="100"/>
       <c r="F68" s="47"/>
       <c r="G68" s="62"/>
       <c r="H68" s="47"/>
@@ -3748,9 +3748,9 @@
     <row r="69" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A69" s="1"/>
       <c r="B69" s="83"/>
-      <c r="C69" s="122"/>
-      <c r="D69" s="123"/>
-      <c r="E69" s="124"/>
+      <c r="C69" s="101"/>
+      <c r="D69" s="102"/>
+      <c r="E69" s="103"/>
       <c r="F69" s="47"/>
       <c r="G69" s="62"/>
       <c r="H69" s="47"/>
@@ -3776,11 +3776,11 @@
     <row r="70" spans="1:26" ht="10" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="83"/>
-      <c r="C70" s="119" t="s">
+      <c r="C70" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="D70" s="120"/>
-      <c r="E70" s="121"/>
+      <c r="D70" s="99"/>
+      <c r="E70" s="100"/>
       <c r="F70" s="47"/>
       <c r="G70" s="62"/>
       <c r="H70" s="47"/>
@@ -3806,9 +3806,9 @@
     <row r="71" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A71" s="1"/>
       <c r="B71" s="83"/>
-      <c r="C71" s="122"/>
-      <c r="D71" s="123"/>
-      <c r="E71" s="124"/>
+      <c r="C71" s="101"/>
+      <c r="D71" s="102"/>
+      <c r="E71" s="103"/>
       <c r="F71" s="47"/>
       <c r="G71" s="62"/>
       <c r="H71" s="47"/>
@@ -3834,11 +3834,11 @@
     <row r="72" spans="1:26" ht="10" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="83"/>
-      <c r="C72" s="119" t="s">
+      <c r="C72" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="D72" s="120"/>
-      <c r="E72" s="121"/>
+      <c r="D72" s="99"/>
+      <c r="E72" s="100"/>
       <c r="F72" s="47"/>
       <c r="G72" s="62"/>
       <c r="H72" s="47"/>
@@ -3864,9 +3864,9 @@
     <row r="73" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A73" s="1"/>
       <c r="B73" s="83"/>
-      <c r="C73" s="122"/>
-      <c r="D73" s="123"/>
-      <c r="E73" s="124"/>
+      <c r="C73" s="101"/>
+      <c r="D73" s="102"/>
+      <c r="E73" s="103"/>
       <c r="F73" s="47"/>
       <c r="G73" s="62"/>
       <c r="H73" s="47"/>
@@ -3892,11 +3892,11 @@
     <row r="74" spans="1:26" ht="10" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="83"/>
-      <c r="C74" s="119" t="s">
-        <v>50</v>
-      </c>
-      <c r="D74" s="120"/>
-      <c r="E74" s="121"/>
+      <c r="C74" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74" s="99"/>
+      <c r="E74" s="100"/>
       <c r="F74" s="47"/>
       <c r="G74" s="62"/>
       <c r="H74" s="47"/>
@@ -3922,9 +3922,9 @@
     <row r="75" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A75" s="1"/>
       <c r="B75" s="83"/>
-      <c r="C75" s="122"/>
-      <c r="D75" s="123"/>
-      <c r="E75" s="124"/>
+      <c r="C75" s="101"/>
+      <c r="D75" s="102"/>
+      <c r="E75" s="103"/>
       <c r="F75" s="47"/>
       <c r="G75" s="62"/>
       <c r="H75" s="47"/>
@@ -3994,11 +3994,11 @@
     </row>
     <row r="78" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A78" s="1"/>
-      <c r="B78" s="125" t="s">
+      <c r="B78" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="C78" s="126"/>
-      <c r="D78" s="127"/>
+      <c r="C78" s="147"/>
+      <c r="D78" s="148"/>
       <c r="E78" s="86">
         <v>12</v>
       </c>
@@ -4027,11 +4027,11 @@
     <row r="79" spans="1:26" ht="10" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="71"/>
-      <c r="C79" s="119" t="s">
+      <c r="C79" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="120"/>
-      <c r="E79" s="121"/>
+      <c r="D79" s="99"/>
+      <c r="E79" s="100"/>
       <c r="F79" s="47"/>
       <c r="G79" s="62"/>
       <c r="H79" s="47"/>
@@ -4057,9 +4057,9 @@
     <row r="80" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A80" s="1"/>
       <c r="B80" s="71"/>
-      <c r="C80" s="122"/>
-      <c r="D80" s="123"/>
-      <c r="E80" s="124"/>
+      <c r="C80" s="101"/>
+      <c r="D80" s="102"/>
+      <c r="E80" s="103"/>
       <c r="F80" s="47"/>
       <c r="G80" s="62"/>
       <c r="H80" s="47"/>
@@ -4085,11 +4085,11 @@
     <row r="81" spans="1:26" ht="10" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="71"/>
-      <c r="C81" s="119" t="s">
+      <c r="C81" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="120"/>
-      <c r="E81" s="121"/>
+      <c r="D81" s="99"/>
+      <c r="E81" s="100"/>
       <c r="F81" s="47"/>
       <c r="G81" s="62"/>
       <c r="H81" s="47"/>
@@ -4115,9 +4115,9 @@
     <row r="82" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A82" s="1"/>
       <c r="B82" s="71"/>
-      <c r="C82" s="122"/>
-      <c r="D82" s="123"/>
-      <c r="E82" s="124"/>
+      <c r="C82" s="101"/>
+      <c r="D82" s="102"/>
+      <c r="E82" s="103"/>
       <c r="F82" s="47"/>
       <c r="G82" s="62"/>
       <c r="H82" s="47"/>
@@ -4142,9 +4142,9 @@
     </row>
     <row r="83" spans="1:26" ht="10" customHeight="1">
       <c r="A83" s="1"/>
-      <c r="B83" s="137"/>
-      <c r="C83" s="138"/>
-      <c r="D83" s="139"/>
+      <c r="B83" s="95"/>
+      <c r="C83" s="96"/>
+      <c r="D83" s="97"/>
       <c r="E83" s="72"/>
       <c r="F83" s="68"/>
       <c r="G83" s="69"/>
@@ -4187,11 +4187,11 @@
     </row>
     <row r="85" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A85" s="1"/>
-      <c r="B85" s="130" t="s">
+      <c r="B85" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="C85" s="131"/>
-      <c r="D85" s="132"/>
+      <c r="C85" s="93"/>
+      <c r="D85" s="94"/>
       <c r="E85" s="87">
         <v>8</v>
       </c>
@@ -4220,11 +4220,11 @@
     <row r="86" spans="1:26" ht="10" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="6"/>
-      <c r="C86" s="119" t="s">
+      <c r="C86" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="D86" s="120"/>
-      <c r="E86" s="121"/>
+      <c r="D86" s="99"/>
+      <c r="E86" s="100"/>
       <c r="F86" s="47"/>
       <c r="G86" s="62"/>
       <c r="H86" s="47"/>
@@ -4250,9 +4250,9 @@
     <row r="87" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A87" s="1"/>
       <c r="B87" s="6"/>
-      <c r="C87" s="122"/>
-      <c r="D87" s="123"/>
-      <c r="E87" s="124"/>
+      <c r="C87" s="101"/>
+      <c r="D87" s="102"/>
+      <c r="E87" s="103"/>
       <c r="F87" s="47"/>
       <c r="G87" s="62"/>
       <c r="H87" s="47"/>
@@ -4278,11 +4278,11 @@
     <row r="88" spans="1:26" ht="10" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="6"/>
-      <c r="C88" s="119" t="s">
+      <c r="C88" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="D88" s="120"/>
-      <c r="E88" s="121"/>
+      <c r="D88" s="99"/>
+      <c r="E88" s="100"/>
       <c r="F88" s="47"/>
       <c r="G88" s="62"/>
       <c r="H88" s="47"/>
@@ -4308,9 +4308,9 @@
     <row r="89" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A89" s="1"/>
       <c r="B89" s="6"/>
-      <c r="C89" s="122"/>
-      <c r="D89" s="123"/>
-      <c r="E89" s="124"/>
+      <c r="C89" s="101"/>
+      <c r="D89" s="102"/>
+      <c r="E89" s="103"/>
       <c r="F89" s="47"/>
       <c r="G89" s="62"/>
       <c r="H89" s="47"/>
@@ -4336,11 +4336,11 @@
     <row r="90" spans="1:26" ht="10" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="6"/>
-      <c r="C90" s="119" t="s">
-        <v>51</v>
-      </c>
-      <c r="D90" s="120"/>
-      <c r="E90" s="121"/>
+      <c r="C90" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="D90" s="99"/>
+      <c r="E90" s="100"/>
       <c r="F90" s="47"/>
       <c r="G90" s="62"/>
       <c r="H90" s="47"/>
@@ -4366,9 +4366,9 @@
     <row r="91" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A91" s="1"/>
       <c r="B91" s="6"/>
-      <c r="C91" s="122"/>
-      <c r="D91" s="123"/>
-      <c r="E91" s="124"/>
+      <c r="C91" s="101"/>
+      <c r="D91" s="102"/>
+      <c r="E91" s="103"/>
       <c r="F91" s="47"/>
       <c r="G91" s="62"/>
       <c r="H91" s="47"/>
@@ -4393,9 +4393,9 @@
     </row>
     <row r="92" spans="1:26" ht="10" customHeight="1">
       <c r="A92" s="1"/>
-      <c r="B92" s="112"/>
-      <c r="C92" s="128"/>
-      <c r="D92" s="129"/>
+      <c r="B92" s="118"/>
+      <c r="C92" s="149"/>
+      <c r="D92" s="150"/>
       <c r="E92" s="22"/>
       <c r="F92" s="15"/>
       <c r="G92" s="16"/>
@@ -4438,11 +4438,11 @@
     </row>
     <row r="94" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A94" s="1"/>
-      <c r="B94" s="130" t="s">
+      <c r="B94" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C94" s="131"/>
-      <c r="D94" s="132"/>
+      <c r="C94" s="93"/>
+      <c r="D94" s="94"/>
       <c r="E94" s="73"/>
       <c r="F94" s="15"/>
       <c r="G94" s="16"/>
@@ -4469,11 +4469,11 @@
     <row r="95" spans="1:26" ht="10" customHeight="1">
       <c r="A95" s="1"/>
       <c r="B95" s="6"/>
-      <c r="C95" s="119" t="s">
+      <c r="C95" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="D95" s="120"/>
-      <c r="E95" s="121"/>
+      <c r="D95" s="99"/>
+      <c r="E95" s="100"/>
       <c r="F95" s="19"/>
       <c r="G95" s="31"/>
       <c r="H95" s="19"/>
@@ -4499,9 +4499,9 @@
     <row r="96" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A96" s="1"/>
       <c r="B96" s="6"/>
-      <c r="C96" s="122"/>
-      <c r="D96" s="123"/>
-      <c r="E96" s="124"/>
+      <c r="C96" s="101"/>
+      <c r="D96" s="102"/>
+      <c r="E96" s="103"/>
       <c r="F96" s="29"/>
       <c r="G96" s="32"/>
       <c r="H96" s="51"/>
@@ -4527,11 +4527,11 @@
     <row r="97" spans="1:26" ht="10" customHeight="1">
       <c r="A97" s="1"/>
       <c r="B97" s="6"/>
-      <c r="C97" s="119" t="s">
-        <v>59</v>
-      </c>
-      <c r="D97" s="120"/>
-      <c r="E97" s="121"/>
+      <c r="C97" s="98" t="s">
+        <v>58</v>
+      </c>
+      <c r="D97" s="99"/>
+      <c r="E97" s="100"/>
       <c r="F97" s="29"/>
       <c r="G97" s="91"/>
       <c r="H97" s="51"/>
@@ -4557,9 +4557,9 @@
     <row r="98" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A98" s="1"/>
       <c r="B98" s="6"/>
-      <c r="C98" s="122"/>
-      <c r="D98" s="123"/>
-      <c r="E98" s="124"/>
+      <c r="C98" s="101"/>
+      <c r="D98" s="102"/>
+      <c r="E98" s="103"/>
       <c r="F98" s="29"/>
       <c r="G98" s="32"/>
       <c r="H98" s="51"/>
@@ -4585,11 +4585,11 @@
     <row r="99" spans="1:26" ht="10" customHeight="1">
       <c r="A99" s="1"/>
       <c r="B99" s="6"/>
-      <c r="C99" s="119" t="s">
+      <c r="C99" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="D99" s="120"/>
-      <c r="E99" s="121"/>
+      <c r="D99" s="99"/>
+      <c r="E99" s="100"/>
       <c r="F99" s="29"/>
       <c r="G99" s="50"/>
       <c r="H99" s="51"/>
@@ -4615,9 +4615,9 @@
     <row r="100" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A100" s="1"/>
       <c r="B100" s="6"/>
-      <c r="C100" s="122"/>
-      <c r="D100" s="123"/>
-      <c r="E100" s="124"/>
+      <c r="C100" s="101"/>
+      <c r="D100" s="102"/>
+      <c r="E100" s="103"/>
       <c r="F100" s="29"/>
       <c r="G100" s="50"/>
       <c r="H100" s="51"/>
@@ -4643,10 +4643,10 @@
     <row r="101" spans="1:26" ht="10" customHeight="1">
       <c r="A101" s="1"/>
       <c r="B101" s="6"/>
-      <c r="C101" s="119" t="s">
-        <v>52</v>
-      </c>
-      <c r="D101" s="120"/>
+      <c r="C101" s="98" t="s">
+        <v>51</v>
+      </c>
+      <c r="D101" s="99"/>
       <c r="E101" s="89">
         <v>5</v>
       </c>
@@ -4675,8 +4675,8 @@
     <row r="102" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A102" s="1"/>
       <c r="B102" s="6"/>
-      <c r="C102" s="122"/>
-      <c r="D102" s="123"/>
+      <c r="C102" s="101"/>
+      <c r="D102" s="102"/>
       <c r="E102" s="67"/>
       <c r="F102" s="49"/>
       <c r="G102" s="78"/>
@@ -4701,9 +4701,9 @@
       <c r="Z102" s="2"/>
     </row>
     <row r="103" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B103" s="112"/>
-      <c r="C103" s="128"/>
-      <c r="D103" s="129"/>
+      <c r="B103" s="118"/>
+      <c r="C103" s="149"/>
+      <c r="D103" s="150"/>
       <c r="E103" s="22"/>
       <c r="F103" s="15"/>
       <c r="G103" s="16"/>
@@ -4728,9 +4728,9 @@
       <c r="Z103" s="2"/>
     </row>
     <row r="104" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
-      <c r="B104" s="118"/>
-      <c r="C104" s="118"/>
-      <c r="D104" s="118"/>
+      <c r="B104" s="145"/>
+      <c r="C104" s="145"/>
+      <c r="D104" s="145"/>
       <c r="E104" s="35"/>
       <c r="F104" s="2"/>
       <c r="H104" s="2"/>
@@ -4745,20 +4745,20 @@
       <c r="Z104" s="2"/>
     </row>
     <row r="105" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B105" s="92" t="s">
+      <c r="B105" s="132" t="s">
         <v>26</v>
       </c>
-      <c r="C105" s="93"/>
-      <c r="D105" s="93"/>
+      <c r="C105" s="133"/>
+      <c r="D105" s="133"/>
       <c r="E105" s="88">
         <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A106" s="1"/>
-      <c r="B106" s="94"/>
-      <c r="C106" s="95"/>
-      <c r="D106" s="95"/>
+      <c r="B106" s="134"/>
+      <c r="C106" s="135"/>
+      <c r="D106" s="135"/>
       <c r="E106" s="79"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -5284,46 +5284,31 @@
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="C45:E46"/>
+    <mergeCell ref="C99:E100"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="C81:E82"/>
+    <mergeCell ref="C86:E87"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="C95:E96"/>
+    <mergeCell ref="C66:E67"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B92:D92"/>
     <mergeCell ref="C88:E89"/>
     <mergeCell ref="B59:D59"/>
     <mergeCell ref="C49:E50"/>
-    <mergeCell ref="C53:E54"/>
-    <mergeCell ref="C74:E75"/>
-    <mergeCell ref="C70:E71"/>
-    <mergeCell ref="C64:E65"/>
-    <mergeCell ref="C62:E63"/>
-    <mergeCell ref="C60:E61"/>
-    <mergeCell ref="C68:E69"/>
-    <mergeCell ref="C72:E73"/>
+    <mergeCell ref="V2:W5"/>
+    <mergeCell ref="X2:Y5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="T2:U5"/>
     <mergeCell ref="R2:S5"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="C28:E29"/>
-    <mergeCell ref="C21:E22"/>
-    <mergeCell ref="P2:Q5"/>
-    <mergeCell ref="C13:E14"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C17:E18"/>
-    <mergeCell ref="C19:E20"/>
-    <mergeCell ref="C9:E10"/>
-    <mergeCell ref="C15:E16"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="T2:U5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="F2:G5"/>
-    <mergeCell ref="H2:I5"/>
-    <mergeCell ref="J2:K5"/>
-    <mergeCell ref="L2:M5"/>
-    <mergeCell ref="N2:O5"/>
+    <mergeCell ref="B105:D106"/>
     <mergeCell ref="C101:D102"/>
     <mergeCell ref="C90:E91"/>
     <mergeCell ref="B57:D57"/>
@@ -5339,28 +5324,43 @@
     <mergeCell ref="C47:E48"/>
     <mergeCell ref="C41:E42"/>
     <mergeCell ref="C97:E98"/>
-    <mergeCell ref="C66:E67"/>
-    <mergeCell ref="C79:E80"/>
-    <mergeCell ref="C81:E82"/>
-    <mergeCell ref="C86:E87"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="C95:E96"/>
-    <mergeCell ref="B105:D106"/>
-    <mergeCell ref="V2:W5"/>
-    <mergeCell ref="X2:Y5"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="F2:G5"/>
+    <mergeCell ref="H2:I5"/>
+    <mergeCell ref="J2:K5"/>
+    <mergeCell ref="L2:M5"/>
+    <mergeCell ref="N2:O5"/>
+    <mergeCell ref="P2:Q5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="C28:E29"/>
+    <mergeCell ref="C21:E22"/>
+    <mergeCell ref="C13:E14"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C17:E18"/>
+    <mergeCell ref="C19:E20"/>
+    <mergeCell ref="C9:E10"/>
+    <mergeCell ref="C15:E16"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="C45:E46"/>
-    <mergeCell ref="C99:E100"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="C79:E80"/>
+    <mergeCell ref="C53:E54"/>
+    <mergeCell ref="C74:E75"/>
+    <mergeCell ref="C70:E71"/>
+    <mergeCell ref="C64:E65"/>
+    <mergeCell ref="C62:E63"/>
+    <mergeCell ref="C60:E61"/>
+    <mergeCell ref="C68:E69"/>
+    <mergeCell ref="C72:E73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Gestern habe ich die Version 0.3 abgeschlossen (erst heute gepusht).
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1240" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="5180" yWindow="6060" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Zeitplan erstellen</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Einführungskonzept</t>
   </si>
   <si>
-    <t>Systemanforderungen</t>
-  </si>
-  <si>
     <t>Projektjournal</t>
   </si>
   <si>
@@ -204,6 +201,12 @@
   </si>
   <si>
     <t>Fazit / Management Summary erfassen</t>
+  </si>
+  <si>
+    <t>Allgemeine Anforderungen</t>
+  </si>
+  <si>
+    <t>Systemarchitektur</t>
   </si>
 </sst>
 </file>
@@ -878,7 +881,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1060,6 +1063,158 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1072,24 +1227,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1099,24 +1236,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1133,126 +1258,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1421,13 +1426,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2197</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>4733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>106567</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1437,8 +1442,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3840817" y="12583099"/>
-          <a:ext cx="104370" cy="124056"/>
+          <a:off x="3851885" y="13173046"/>
+          <a:ext cx="104370" cy="122267"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1765,10 +1770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z205"/>
+  <dimension ref="A1:Z207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="M85" sqref="M85"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="K100" sqref="K100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1779,7 +1784,7 @@
     <col min="4" max="4" width="2.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="10" style="5" customWidth="1"/>
     <col min="6" max="25" width="2.6640625" style="5" customWidth="1"/>
-    <col min="26" max="26" width="2.5" style="5" customWidth="1"/>
+    <col min="26" max="26" width="4.6640625" style="5" customWidth="1"/>
     <col min="27" max="16384" width="9.1640625" style="5"/>
   </cols>
   <sheetData>
@@ -1813,50 +1818,50 @@
     </row>
     <row r="2" spans="1:26" ht="23" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="140"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="119" t="s">
+      <c r="B2" s="107"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="124" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="116"/>
-      <c r="H2" s="119" t="s">
+      <c r="G2" s="125"/>
+      <c r="H2" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="120"/>
-      <c r="J2" s="116" t="s">
+      <c r="I2" s="130"/>
+      <c r="J2" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="116"/>
-      <c r="L2" s="119" t="s">
+      <c r="K2" s="125"/>
+      <c r="L2" s="124" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="120"/>
-      <c r="N2" s="116" t="s">
+      <c r="M2" s="130"/>
+      <c r="N2" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="116"/>
-      <c r="P2" s="119" t="s">
+      <c r="O2" s="125"/>
+      <c r="P2" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="116" t="s">
+      <c r="Q2" s="130"/>
+      <c r="R2" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="116"/>
-      <c r="T2" s="119" t="s">
+      <c r="S2" s="125"/>
+      <c r="T2" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="120"/>
-      <c r="V2" s="116" t="s">
+      <c r="U2" s="130"/>
+      <c r="V2" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="116"/>
-      <c r="X2" s="119" t="s">
+      <c r="W2" s="125"/>
+      <c r="X2" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="120"/>
+      <c r="Y2" s="130"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="14" customHeight="1">
@@ -1867,26 +1872,26 @@
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="121"/>
-      <c r="Q3" s="122"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="121"/>
-      <c r="U3" s="122"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="121"/>
-      <c r="Y3" s="122"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="127"/>
+      <c r="O3" s="127"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="127"/>
+      <c r="S3" s="127"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="131"/>
+      <c r="V3" s="127"/>
+      <c r="W3" s="127"/>
+      <c r="X3" s="126"/>
+      <c r="Y3" s="131"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="14" customHeight="1">
@@ -1897,86 +1902,86 @@
       <c r="C4" s="3"/>
       <c r="D4" s="8"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="122"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
-      <c r="L4" s="121"/>
-      <c r="M4" s="122"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="121"/>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="121"/>
-      <c r="U4" s="122"/>
-      <c r="V4" s="117"/>
-      <c r="W4" s="117"/>
-      <c r="X4" s="121"/>
-      <c r="Y4" s="122"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="127"/>
+      <c r="O4" s="127"/>
+      <c r="P4" s="126"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="127"/>
+      <c r="S4" s="127"/>
+      <c r="T4" s="126"/>
+      <c r="U4" s="131"/>
+      <c r="V4" s="127"/>
+      <c r="W4" s="127"/>
+      <c r="X4" s="126"/>
+      <c r="Y4" s="131"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="20" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="138"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="123"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="123"/>
-      <c r="M5" s="126"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="123"/>
-      <c r="Q5" s="126"/>
-      <c r="R5" s="118"/>
-      <c r="S5" s="118"/>
-      <c r="T5" s="123"/>
-      <c r="U5" s="126"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="118"/>
-      <c r="X5" s="123"/>
-      <c r="Y5" s="118"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="132"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="128"/>
+      <c r="M5" s="132"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="128"/>
+      <c r="Q5" s="132"/>
+      <c r="R5" s="129"/>
+      <c r="S5" s="129"/>
+      <c r="T5" s="128"/>
+      <c r="U5" s="132"/>
+      <c r="V5" s="129"/>
+      <c r="W5" s="129"/>
+      <c r="X5" s="128"/>
+      <c r="Y5" s="129"/>
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="10" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="142" t="s">
+      <c r="B6" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="144"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="111"/>
       <c r="E6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="124"/>
-      <c r="G6" s="125"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="125"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="125"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="125"/>
-      <c r="P6" s="124"/>
-      <c r="Q6" s="125"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="125"/>
-      <c r="T6" s="124"/>
-      <c r="U6" s="125"/>
-      <c r="V6" s="124"/>
-      <c r="W6" s="125"/>
-      <c r="X6" s="124"/>
-      <c r="Y6" s="125"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="123"/>
+      <c r="N6" s="122"/>
+      <c r="O6" s="123"/>
+      <c r="P6" s="122"/>
+      <c r="Q6" s="123"/>
+      <c r="R6" s="122"/>
+      <c r="S6" s="123"/>
+      <c r="T6" s="122"/>
+      <c r="U6" s="123"/>
+      <c r="V6" s="122"/>
+      <c r="W6" s="123"/>
+      <c r="X6" s="122"/>
+      <c r="Y6" s="123"/>
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
@@ -1999,11 +2004,11 @@
     </row>
     <row r="8" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="145" t="s">
+      <c r="B8" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="146"/>
-      <c r="D8" s="147"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="115"/>
       <c r="E8" s="14">
         <v>7.5</v>
       </c>
@@ -2032,11 +2037,11 @@
     <row r="9" spans="1:26" ht="10" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="95"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
       <c r="H9" s="19"/>
@@ -2062,9 +2067,9 @@
     <row r="10" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A10" s="1"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="100"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="98"/>
       <c r="F10" s="24"/>
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
@@ -2090,11 +2095,11 @@
     <row r="11" spans="1:26" ht="10" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="96"/>
-      <c r="E11" s="97"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="95"/>
       <c r="F11" s="27"/>
       <c r="G11" s="25"/>
       <c r="H11" s="26"/>
@@ -2120,9 +2125,9 @@
     <row r="12" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A12" s="1"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="99"/>
-      <c r="E12" s="100"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="98"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
@@ -2148,11 +2153,11 @@
     <row r="13" spans="1:26" ht="10" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="97"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="95"/>
       <c r="F13" s="17"/>
       <c r="G13" s="25"/>
       <c r="H13" s="26"/>
@@ -2178,9 +2183,9 @@
     <row r="14" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A14" s="1"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="100"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="98"/>
       <c r="F14" s="24"/>
       <c r="G14" s="25"/>
       <c r="H14" s="26"/>
@@ -2206,11 +2211,11 @@
     <row r="15" spans="1:26" ht="10" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="137" t="s">
+      <c r="C15" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="97"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="95"/>
       <c r="F15" s="17"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
@@ -2236,9 +2241,9 @@
     <row r="16" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="100"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="98"/>
       <c r="F16" s="24"/>
       <c r="G16" s="25"/>
       <c r="H16" s="26"/>
@@ -2264,11 +2269,11 @@
     <row r="17" spans="1:26" ht="10" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="96"/>
-      <c r="E17" s="97"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="95"/>
       <c r="F17" s="27"/>
       <c r="G17" s="25"/>
       <c r="H17" s="26"/>
@@ -2294,9 +2299,9 @@
     <row r="18" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A18" s="1"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="98"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="100"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="98"/>
       <c r="F18" s="24"/>
       <c r="G18" s="28"/>
       <c r="H18" s="26"/>
@@ -2322,11 +2327,11 @@
     <row r="19" spans="1:26" ht="10" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="96"/>
-      <c r="E19" s="97"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="95"/>
       <c r="F19" s="29"/>
       <c r="G19" s="30"/>
       <c r="H19" s="26"/>
@@ -2352,9 +2357,9 @@
     <row r="20" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A20" s="1"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="98"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="100"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="98"/>
       <c r="F20" s="29"/>
       <c r="G20" s="28"/>
       <c r="H20" s="26"/>
@@ -2380,11 +2385,11 @@
     <row r="21" spans="1:26" ht="10" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="137" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="96"/>
-      <c r="E21" s="97"/>
+      <c r="C21" s="112" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="94"/>
+      <c r="E21" s="95"/>
       <c r="F21" s="19"/>
       <c r="G21" s="31"/>
       <c r="H21" s="26"/>
@@ -2410,9 +2415,9 @@
     <row r="22" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A22" s="1"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="98"/>
-      <c r="D22" s="99"/>
-      <c r="E22" s="100"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="98"/>
       <c r="F22" s="29"/>
       <c r="G22" s="32"/>
       <c r="H22" s="26"/>
@@ -2437,9 +2442,9 @@
     </row>
     <row r="23" spans="1:26" ht="10" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="151"/>
-      <c r="D23" s="152"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="121"/>
       <c r="E23" s="33">
         <v>8.5</v>
       </c>
@@ -2484,11 +2489,11 @@
     </row>
     <row r="25" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="148" t="s">
+      <c r="B25" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="149"/>
-      <c r="D25" s="150"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="118"/>
       <c r="E25" s="36">
         <v>7.5</v>
       </c>
@@ -2517,11 +2522,11 @@
     <row r="26" spans="1:26" ht="10" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="40"/>
-      <c r="C26" s="95" t="s">
+      <c r="C26" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="96"/>
-      <c r="E26" s="97"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="95"/>
       <c r="F26" s="41"/>
       <c r="G26" s="42"/>
       <c r="H26" s="43"/>
@@ -2547,9 +2552,9 @@
     <row r="27" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A27" s="1"/>
       <c r="B27" s="40"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="100"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="98"/>
       <c r="F27" s="48"/>
       <c r="G27" s="32"/>
       <c r="H27" s="49"/>
@@ -2575,15 +2580,15 @@
     <row r="28" spans="1:26" ht="10" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="40"/>
-      <c r="C28" s="137" t="s">
+      <c r="C28" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="96"/>
-      <c r="E28" s="97"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="95"/>
       <c r="F28" s="48"/>
       <c r="G28" s="50"/>
       <c r="H28" s="43"/>
-      <c r="I28" s="52"/>
+      <c r="I28" s="76"/>
       <c r="J28" s="45"/>
       <c r="K28" s="46"/>
       <c r="L28" s="47"/>
@@ -2605,13 +2610,13 @@
     <row r="29" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A29" s="1"/>
       <c r="B29" s="40"/>
-      <c r="C29" s="98"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="100"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="98"/>
       <c r="F29" s="48"/>
       <c r="G29" s="50"/>
       <c r="H29" s="49"/>
-      <c r="I29" s="53"/>
+      <c r="I29" s="76"/>
       <c r="J29" s="45"/>
       <c r="K29" s="46"/>
       <c r="L29" s="47"/>
@@ -2633,11 +2638,11 @@
     <row r="30" spans="1:26" ht="10" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="40"/>
-      <c r="C30" s="95" t="s">
+      <c r="C30" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="96"/>
-      <c r="E30" s="97"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="95"/>
       <c r="F30" s="47"/>
       <c r="G30" s="18"/>
       <c r="H30" s="43"/>
@@ -2663,9 +2668,9 @@
     <row r="31" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A31" s="1"/>
       <c r="B31" s="40"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="100"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="97"/>
+      <c r="E31" s="98"/>
       <c r="F31" s="47"/>
       <c r="G31" s="50"/>
       <c r="H31" s="49"/>
@@ -2691,11 +2696,11 @@
     <row r="32" spans="1:26" ht="10" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="40"/>
-      <c r="C32" s="137" t="s">
+      <c r="C32" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="96"/>
-      <c r="E32" s="97"/>
+      <c r="D32" s="94"/>
+      <c r="E32" s="95"/>
       <c r="F32" s="47"/>
       <c r="G32" s="18"/>
       <c r="H32" s="19"/>
@@ -2721,9 +2726,9 @@
     <row r="33" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A33" s="1"/>
       <c r="B33" s="40"/>
-      <c r="C33" s="98"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="100"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="98"/>
       <c r="F33" s="47"/>
       <c r="G33" s="50"/>
       <c r="H33" s="29"/>
@@ -2749,11 +2754,11 @@
     <row r="34" spans="1:26" ht="10" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="40"/>
-      <c r="C34" s="95" t="s">
+      <c r="C34" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="96"/>
-      <c r="E34" s="97"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="95"/>
       <c r="F34" s="47"/>
       <c r="G34" s="54"/>
       <c r="H34" s="19"/>
@@ -2779,9 +2784,9 @@
     <row r="35" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A35" s="1"/>
       <c r="B35" s="40"/>
-      <c r="C35" s="98"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="100"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="98"/>
       <c r="F35" s="47"/>
       <c r="G35" s="55"/>
       <c r="H35" s="29"/>
@@ -2806,9 +2811,9 @@
     </row>
     <row r="36" spans="1:26" ht="10" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="93"/>
+      <c r="B36" s="143"/>
+      <c r="C36" s="144"/>
+      <c r="D36" s="145"/>
       <c r="E36" s="56">
         <v>7</v>
       </c>
@@ -2853,11 +2858,11 @@
     </row>
     <row r="38" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="134" t="s">
+      <c r="B38" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="135"/>
-      <c r="D38" s="136"/>
+      <c r="C38" s="141"/>
+      <c r="D38" s="142"/>
       <c r="E38" s="57">
         <v>12</v>
       </c>
@@ -2886,11 +2891,11 @@
     <row r="39" spans="1:26" ht="10" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="61"/>
-      <c r="C39" s="95" t="s">
+      <c r="C39" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="96"/>
-      <c r="E39" s="97"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="95"/>
       <c r="F39" s="47"/>
       <c r="G39" s="62"/>
       <c r="H39" s="47"/>
@@ -2916,14 +2921,14 @@
     <row r="40" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A40" s="1"/>
       <c r="B40" s="61"/>
-      <c r="C40" s="98"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="100"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="97"/>
+      <c r="E40" s="98"/>
       <c r="F40" s="47"/>
       <c r="G40" s="62"/>
       <c r="H40" s="47"/>
       <c r="I40" s="44"/>
-      <c r="J40" s="74"/>
+      <c r="J40" s="91"/>
       <c r="K40" s="46"/>
       <c r="L40" s="47"/>
       <c r="M40" s="44"/>
@@ -2944,11 +2949,11 @@
     <row r="41" spans="1:26" ht="10" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="61"/>
-      <c r="C41" s="95" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" s="96"/>
-      <c r="E41" s="97"/>
+      <c r="C41" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="94"/>
+      <c r="E41" s="95"/>
       <c r="F41" s="47"/>
       <c r="G41" s="62"/>
       <c r="H41" s="47"/>
@@ -2974,14 +2979,14 @@
     <row r="42" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A42" s="1"/>
       <c r="B42" s="61"/>
-      <c r="C42" s="98"/>
-      <c r="D42" s="99"/>
-      <c r="E42" s="100"/>
+      <c r="C42" s="96"/>
+      <c r="D42" s="97"/>
+      <c r="E42" s="98"/>
       <c r="F42" s="47"/>
       <c r="G42" s="62"/>
       <c r="H42" s="47"/>
       <c r="I42" s="44"/>
-      <c r="J42" s="74"/>
+      <c r="J42" s="91"/>
       <c r="K42" s="46"/>
       <c r="L42" s="47"/>
       <c r="M42" s="44"/>
@@ -3002,17 +3007,17 @@
     <row r="43" spans="1:26" ht="10" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="61"/>
-      <c r="C43" s="95" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="96"/>
-      <c r="E43" s="97"/>
+      <c r="C43" s="93" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="94"/>
+      <c r="E43" s="95"/>
       <c r="F43" s="47"/>
       <c r="G43" s="62"/>
       <c r="H43" s="47"/>
       <c r="I43" s="44"/>
       <c r="J43" s="63"/>
-      <c r="K43" s="75"/>
+      <c r="K43" s="46"/>
       <c r="L43" s="47"/>
       <c r="M43" s="44"/>
       <c r="N43" s="45"/>
@@ -3032,14 +3037,14 @@
     <row r="44" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A44" s="1"/>
       <c r="B44" s="61"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="99"/>
-      <c r="E44" s="100"/>
+      <c r="C44" s="96"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="98"/>
       <c r="F44" s="47"/>
       <c r="G44" s="62"/>
       <c r="H44" s="47"/>
       <c r="I44" s="44"/>
-      <c r="J44" s="74"/>
+      <c r="J44" s="91"/>
       <c r="K44" s="46"/>
       <c r="L44" s="47"/>
       <c r="M44" s="44"/>
@@ -3060,17 +3065,17 @@
     <row r="45" spans="1:26" ht="10" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="61"/>
-      <c r="C45" s="95" t="s">
-        <v>53</v>
-      </c>
-      <c r="D45" s="96"/>
-      <c r="E45" s="97"/>
+      <c r="C45" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="94"/>
+      <c r="E45" s="95"/>
       <c r="F45" s="47"/>
       <c r="G45" s="62"/>
       <c r="H45" s="47"/>
       <c r="I45" s="44"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="64"/>
+      <c r="J45" s="63"/>
+      <c r="K45" s="75"/>
       <c r="L45" s="47"/>
       <c r="M45" s="44"/>
       <c r="N45" s="45"/>
@@ -3090,15 +3095,15 @@
     <row r="46" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A46" s="1"/>
       <c r="B46" s="61"/>
-      <c r="C46" s="98"/>
-      <c r="D46" s="99"/>
-      <c r="E46" s="100"/>
+      <c r="C46" s="96"/>
+      <c r="D46" s="97"/>
+      <c r="E46" s="98"/>
       <c r="F46" s="47"/>
       <c r="G46" s="62"/>
       <c r="H46" s="47"/>
       <c r="I46" s="44"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="75"/>
+      <c r="J46" s="74"/>
+      <c r="K46" s="92"/>
       <c r="L46" s="47"/>
       <c r="M46" s="44"/>
       <c r="N46" s="45"/>
@@ -3118,18 +3123,18 @@
     <row r="47" spans="1:26" ht="10" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="61"/>
-      <c r="C47" s="95" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="96"/>
-      <c r="E47" s="97"/>
+      <c r="C47" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="94"/>
+      <c r="E47" s="95"/>
       <c r="F47" s="47"/>
       <c r="G47" s="62"/>
       <c r="H47" s="47"/>
       <c r="I47" s="44"/>
       <c r="J47" s="45"/>
-      <c r="K47" s="89"/>
-      <c r="L47" s="43"/>
+      <c r="K47" s="64"/>
+      <c r="L47" s="47"/>
       <c r="M47" s="44"/>
       <c r="N47" s="45"/>
       <c r="O47" s="46"/>
@@ -3148,14 +3153,14 @@
     <row r="48" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A48" s="1"/>
       <c r="B48" s="61"/>
-      <c r="C48" s="98"/>
-      <c r="D48" s="99"/>
-      <c r="E48" s="100"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="97"/>
+      <c r="E48" s="98"/>
       <c r="F48" s="47"/>
       <c r="G48" s="62"/>
       <c r="H48" s="47"/>
       <c r="I48" s="44"/>
-      <c r="J48" s="45"/>
+      <c r="J48" s="91"/>
       <c r="K48" s="75"/>
       <c r="L48" s="47"/>
       <c r="M48" s="44"/>
@@ -3176,19 +3181,19 @@
     <row r="49" spans="1:26" ht="10" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="61"/>
-      <c r="C49" s="95" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="96"/>
-      <c r="E49" s="97"/>
+      <c r="C49" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="94"/>
+      <c r="E49" s="95"/>
       <c r="F49" s="47"/>
       <c r="G49" s="62"/>
       <c r="H49" s="47"/>
       <c r="I49" s="44"/>
       <c r="J49" s="45"/>
-      <c r="K49" s="75"/>
-      <c r="L49" s="51"/>
-      <c r="M49" s="52"/>
+      <c r="K49" s="89"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="44"/>
       <c r="N49" s="45"/>
       <c r="O49" s="46"/>
       <c r="P49" s="47"/>
@@ -3206,9 +3211,9 @@
     <row r="50" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A50" s="1"/>
       <c r="B50" s="61"/>
-      <c r="C50" s="98"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="100"/>
+      <c r="C50" s="96"/>
+      <c r="D50" s="97"/>
+      <c r="E50" s="98"/>
       <c r="F50" s="47"/>
       <c r="G50" s="62"/>
       <c r="H50" s="47"/>
@@ -3234,17 +3239,17 @@
     <row r="51" spans="1:26" ht="10" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="61"/>
-      <c r="C51" s="95" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" s="96"/>
-      <c r="E51" s="97"/>
+      <c r="C51" s="93" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="94"/>
+      <c r="E51" s="95"/>
       <c r="F51" s="47"/>
       <c r="G51" s="62"/>
       <c r="H51" s="47"/>
       <c r="I51" s="44"/>
       <c r="J51" s="45"/>
-      <c r="K51" s="46"/>
+      <c r="K51" s="75"/>
       <c r="L51" s="51"/>
       <c r="M51" s="52"/>
       <c r="N51" s="45"/>
@@ -3264,18 +3269,18 @@
     <row r="52" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A52" s="1"/>
       <c r="B52" s="61"/>
-      <c r="C52" s="98"/>
-      <c r="D52" s="99"/>
-      <c r="E52" s="100"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="97"/>
+      <c r="E52" s="98"/>
       <c r="F52" s="47"/>
       <c r="G52" s="62"/>
       <c r="H52" s="47"/>
       <c r="I52" s="44"/>
       <c r="J52" s="45"/>
-      <c r="K52" s="46"/>
+      <c r="K52" s="75"/>
       <c r="L52" s="47"/>
-      <c r="M52" s="76"/>
-      <c r="N52" s="63"/>
+      <c r="M52" s="44"/>
+      <c r="N52" s="45"/>
       <c r="O52" s="46"/>
       <c r="P52" s="47"/>
       <c r="Q52" s="44"/>
@@ -3292,11 +3297,11 @@
     <row r="53" spans="1:26" ht="10" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="61"/>
-      <c r="C53" s="95" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="96"/>
-      <c r="E53" s="97"/>
+      <c r="C53" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="94"/>
+      <c r="E53" s="95"/>
       <c r="F53" s="47"/>
       <c r="G53" s="62"/>
       <c r="H53" s="47"/>
@@ -3304,8 +3309,8 @@
       <c r="J53" s="45"/>
       <c r="K53" s="46"/>
       <c r="L53" s="51"/>
-      <c r="M53" s="76"/>
-      <c r="N53" s="74"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="45"/>
       <c r="O53" s="46"/>
       <c r="P53" s="47"/>
       <c r="Q53" s="44"/>
@@ -3322,9 +3327,9 @@
     <row r="54" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A54" s="1"/>
       <c r="B54" s="61"/>
-      <c r="C54" s="98"/>
-      <c r="D54" s="99"/>
-      <c r="E54" s="100"/>
+      <c r="C54" s="96"/>
+      <c r="D54" s="97"/>
+      <c r="E54" s="98"/>
       <c r="F54" s="47"/>
       <c r="G54" s="62"/>
       <c r="H54" s="47"/>
@@ -3350,20 +3355,20 @@
     <row r="55" spans="1:26" ht="10" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="61"/>
-      <c r="C55" s="95" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="96"/>
-      <c r="E55" s="97"/>
+      <c r="C55" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="94"/>
+      <c r="E55" s="95"/>
       <c r="F55" s="47"/>
       <c r="G55" s="62"/>
       <c r="H55" s="47"/>
       <c r="I55" s="44"/>
       <c r="J55" s="45"/>
-      <c r="K55" s="64"/>
-      <c r="L55" s="47"/>
-      <c r="M55" s="44"/>
-      <c r="N55" s="45"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="51"/>
+      <c r="M55" s="76"/>
+      <c r="N55" s="74"/>
       <c r="O55" s="46"/>
       <c r="P55" s="47"/>
       <c r="Q55" s="44"/>
@@ -3380,9 +3385,9 @@
     <row r="56" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A56" s="1"/>
       <c r="B56" s="61"/>
-      <c r="C56" s="98"/>
-      <c r="D56" s="99"/>
-      <c r="E56" s="100"/>
+      <c r="C56" s="96"/>
+      <c r="D56" s="97"/>
+      <c r="E56" s="98"/>
       <c r="F56" s="47"/>
       <c r="G56" s="62"/>
       <c r="H56" s="47"/>
@@ -3390,8 +3395,8 @@
       <c r="J56" s="45"/>
       <c r="K56" s="46"/>
       <c r="L56" s="47"/>
-      <c r="M56" s="44"/>
-      <c r="N56" s="45"/>
+      <c r="M56" s="76"/>
+      <c r="N56" s="63"/>
       <c r="O56" s="46"/>
       <c r="P56" s="47"/>
       <c r="Q56" s="44"/>
@@ -3407,147 +3412,147 @@
     </row>
     <row r="57" spans="1:26" ht="10" customHeight="1">
       <c r="A57" s="1"/>
-      <c r="B57" s="131"/>
-      <c r="C57" s="132"/>
-      <c r="D57" s="133"/>
-      <c r="E57" s="65"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="59"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="60"/>
-      <c r="J57" s="58"/>
-      <c r="K57" s="60"/>
-      <c r="L57" s="58"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="58"/>
-      <c r="O57" s="60"/>
-      <c r="P57" s="58"/>
-      <c r="Q57" s="60"/>
-      <c r="R57" s="58"/>
-      <c r="S57" s="60"/>
-      <c r="T57" s="58"/>
-      <c r="U57" s="60"/>
-      <c r="V57" s="58"/>
-      <c r="W57" s="60"/>
-      <c r="X57" s="58"/>
-      <c r="Y57" s="60"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="93" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="94"/>
+      <c r="E57" s="95"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="64"/>
+      <c r="L57" s="47"/>
+      <c r="M57" s="44"/>
+      <c r="N57" s="45"/>
+      <c r="O57" s="46"/>
+      <c r="P57" s="47"/>
+      <c r="Q57" s="44"/>
+      <c r="R57" s="45"/>
+      <c r="S57" s="46"/>
+      <c r="T57" s="47"/>
+      <c r="U57" s="44"/>
+      <c r="V57" s="45"/>
+      <c r="W57" s="46"/>
+      <c r="X57" s="47"/>
+      <c r="Y57" s="44"/>
       <c r="Z57" s="1"/>
     </row>
-    <row r="58" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="4"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="4"/>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="4"/>
-      <c r="T58" s="2"/>
-      <c r="U58" s="4"/>
-      <c r="X58" s="2"/>
-      <c r="Y58" s="4"/>
-    </row>
-    <row r="59" spans="1:26" ht="10" customHeight="1" thickBot="1">
+    <row r="58" spans="1:26" ht="10" customHeight="1" thickBot="1">
+      <c r="A58" s="1"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="96"/>
+      <c r="D58" s="97"/>
+      <c r="E58" s="98"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="62"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="47"/>
+      <c r="M58" s="44"/>
+      <c r="N58" s="45"/>
+      <c r="O58" s="46"/>
+      <c r="P58" s="47"/>
+      <c r="Q58" s="44"/>
+      <c r="R58" s="45"/>
+      <c r="S58" s="46"/>
+      <c r="T58" s="47"/>
+      <c r="U58" s="44"/>
+      <c r="V58" s="45"/>
+      <c r="W58" s="46"/>
+      <c r="X58" s="47"/>
+      <c r="Y58" s="44"/>
+      <c r="Z58" s="1"/>
+    </row>
+    <row r="59" spans="1:26" ht="10" customHeight="1">
       <c r="A59" s="1"/>
-      <c r="B59" s="113" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="114"/>
-      <c r="D59" s="115"/>
-      <c r="E59" s="84">
-        <v>28</v>
-      </c>
-      <c r="F59" s="79"/>
-      <c r="G59" s="80"/>
-      <c r="H59" s="79"/>
-      <c r="I59" s="81"/>
-      <c r="J59" s="79"/>
-      <c r="K59" s="81"/>
-      <c r="L59" s="79"/>
-      <c r="M59" s="81"/>
-      <c r="N59" s="79"/>
-      <c r="O59" s="81"/>
-      <c r="P59" s="79"/>
-      <c r="Q59" s="81"/>
-      <c r="R59" s="79"/>
-      <c r="S59" s="81"/>
-      <c r="T59" s="79"/>
-      <c r="U59" s="81"/>
-      <c r="V59" s="79"/>
-      <c r="W59" s="81"/>
-      <c r="X59" s="79"/>
-      <c r="Y59" s="80"/>
-      <c r="Z59" s="2"/>
-    </row>
-    <row r="60" spans="1:26" ht="10" customHeight="1">
-      <c r="A60" s="1"/>
-      <c r="B60" s="82"/>
-      <c r="C60" s="95" t="s">
-        <v>39</v>
-      </c>
-      <c r="D60" s="96"/>
-      <c r="E60" s="97"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="62"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="44"/>
-      <c r="J60" s="45"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="47"/>
-      <c r="M60" s="76"/>
-      <c r="N60" s="45"/>
-      <c r="O60" s="64"/>
-      <c r="P60" s="47"/>
-      <c r="Q60" s="44"/>
-      <c r="R60" s="45"/>
-      <c r="S60" s="46"/>
-      <c r="T60" s="47"/>
-      <c r="U60" s="44"/>
-      <c r="V60" s="45"/>
-      <c r="W60" s="46"/>
-      <c r="X60" s="47"/>
-      <c r="Y60" s="44"/>
-      <c r="Z60" s="1"/>
+      <c r="B59" s="137"/>
+      <c r="C59" s="138"/>
+      <c r="D59" s="139"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="60"/>
+      <c r="J59" s="58"/>
+      <c r="K59" s="60"/>
+      <c r="L59" s="58"/>
+      <c r="M59" s="60"/>
+      <c r="N59" s="58"/>
+      <c r="O59" s="60"/>
+      <c r="P59" s="58"/>
+      <c r="Q59" s="60"/>
+      <c r="R59" s="58"/>
+      <c r="S59" s="60"/>
+      <c r="T59" s="58"/>
+      <c r="U59" s="60"/>
+      <c r="V59" s="58"/>
+      <c r="W59" s="60"/>
+      <c r="X59" s="58"/>
+      <c r="Y59" s="60"/>
+      <c r="Z59" s="1"/>
+    </row>
+    <row r="60" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="4"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="4"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="4"/>
+      <c r="T60" s="2"/>
+      <c r="U60" s="4"/>
+      <c r="X60" s="2"/>
+      <c r="Y60" s="4"/>
     </row>
     <row r="61" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A61" s="1"/>
-      <c r="B61" s="82"/>
-      <c r="C61" s="98"/>
-      <c r="D61" s="99"/>
-      <c r="E61" s="100"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="62"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="45"/>
-      <c r="K61" s="46"/>
-      <c r="L61" s="47"/>
-      <c r="M61" s="44"/>
-      <c r="N61" s="45"/>
-      <c r="O61" s="46"/>
-      <c r="P61" s="47"/>
-      <c r="Q61" s="44"/>
-      <c r="R61" s="45"/>
-      <c r="S61" s="46"/>
-      <c r="T61" s="47"/>
-      <c r="U61" s="44"/>
-      <c r="V61" s="45"/>
-      <c r="W61" s="46"/>
-      <c r="X61" s="47"/>
-      <c r="Y61" s="44"/>
-      <c r="Z61" s="1"/>
+      <c r="B61" s="155" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="156"/>
+      <c r="D61" s="157"/>
+      <c r="E61" s="84">
+        <v>28</v>
+      </c>
+      <c r="F61" s="79"/>
+      <c r="G61" s="80"/>
+      <c r="H61" s="79"/>
+      <c r="I61" s="81"/>
+      <c r="J61" s="79"/>
+      <c r="K61" s="81"/>
+      <c r="L61" s="79"/>
+      <c r="M61" s="81"/>
+      <c r="N61" s="79"/>
+      <c r="O61" s="81"/>
+      <c r="P61" s="79"/>
+      <c r="Q61" s="81"/>
+      <c r="R61" s="79"/>
+      <c r="S61" s="81"/>
+      <c r="T61" s="79"/>
+      <c r="U61" s="81"/>
+      <c r="V61" s="79"/>
+      <c r="W61" s="81"/>
+      <c r="X61" s="79"/>
+      <c r="Y61" s="80"/>
+      <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="10" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="82"/>
-      <c r="C62" s="95" t="s">
-        <v>40</v>
-      </c>
-      <c r="D62" s="96"/>
-      <c r="E62" s="97"/>
+      <c r="C62" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="94"/>
+      <c r="E62" s="95"/>
       <c r="F62" s="47"/>
       <c r="G62" s="62"/>
       <c r="H62" s="47"/>
@@ -3556,7 +3561,7 @@
       <c r="K62" s="46"/>
       <c r="L62" s="47"/>
       <c r="M62" s="76"/>
-      <c r="N62" s="74"/>
+      <c r="N62" s="45"/>
       <c r="O62" s="64"/>
       <c r="P62" s="47"/>
       <c r="Q62" s="44"/>
@@ -3573,9 +3578,9 @@
     <row r="63" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A63" s="1"/>
       <c r="B63" s="82"/>
-      <c r="C63" s="98"/>
-      <c r="D63" s="99"/>
-      <c r="E63" s="100"/>
+      <c r="C63" s="96"/>
+      <c r="D63" s="97"/>
+      <c r="E63" s="98"/>
       <c r="F63" s="47"/>
       <c r="G63" s="62"/>
       <c r="H63" s="47"/>
@@ -3601,11 +3606,11 @@
     <row r="64" spans="1:26" ht="10" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="82"/>
-      <c r="C64" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="D64" s="96"/>
-      <c r="E64" s="97"/>
+      <c r="C64" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="94"/>
+      <c r="E64" s="95"/>
       <c r="F64" s="47"/>
       <c r="G64" s="62"/>
       <c r="H64" s="47"/>
@@ -3613,13 +3618,13 @@
       <c r="J64" s="45"/>
       <c r="K64" s="46"/>
       <c r="L64" s="47"/>
-      <c r="M64" s="44"/>
+      <c r="M64" s="76"/>
       <c r="N64" s="74"/>
       <c r="O64" s="64"/>
-      <c r="P64" s="43"/>
-      <c r="Q64" s="52"/>
-      <c r="R64" s="63"/>
-      <c r="S64" s="64"/>
+      <c r="P64" s="47"/>
+      <c r="Q64" s="44"/>
+      <c r="R64" s="45"/>
+      <c r="S64" s="46"/>
       <c r="T64" s="47"/>
       <c r="U64" s="44"/>
       <c r="V64" s="45"/>
@@ -3631,9 +3636,9 @@
     <row r="65" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A65" s="1"/>
       <c r="B65" s="82"/>
-      <c r="C65" s="98"/>
-      <c r="D65" s="99"/>
-      <c r="E65" s="100"/>
+      <c r="C65" s="96"/>
+      <c r="D65" s="97"/>
+      <c r="E65" s="98"/>
       <c r="F65" s="47"/>
       <c r="G65" s="62"/>
       <c r="H65" s="47"/>
@@ -3659,11 +3664,11 @@
     <row r="66" spans="1:26" ht="10" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="82"/>
-      <c r="C66" s="95" t="s">
-        <v>42</v>
-      </c>
-      <c r="D66" s="96"/>
-      <c r="E66" s="97"/>
+      <c r="C66" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="94"/>
+      <c r="E66" s="95"/>
       <c r="F66" s="47"/>
       <c r="G66" s="62"/>
       <c r="H66" s="47"/>
@@ -3672,11 +3677,11 @@
       <c r="K66" s="46"/>
       <c r="L66" s="47"/>
       <c r="M66" s="44"/>
-      <c r="N66" s="45"/>
-      <c r="O66" s="46"/>
-      <c r="P66" s="47"/>
-      <c r="Q66" s="44"/>
-      <c r="R66" s="45"/>
+      <c r="N66" s="74"/>
+      <c r="O66" s="64"/>
+      <c r="P66" s="43"/>
+      <c r="Q66" s="52"/>
+      <c r="R66" s="63"/>
       <c r="S66" s="64"/>
       <c r="T66" s="47"/>
       <c r="U66" s="44"/>
@@ -3689,9 +3694,9 @@
     <row r="67" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A67" s="1"/>
       <c r="B67" s="82"/>
-      <c r="C67" s="98"/>
-      <c r="D67" s="99"/>
-      <c r="E67" s="100"/>
+      <c r="C67" s="96"/>
+      <c r="D67" s="97"/>
+      <c r="E67" s="98"/>
       <c r="F67" s="47"/>
       <c r="G67" s="62"/>
       <c r="H67" s="47"/>
@@ -3717,11 +3722,11 @@
     <row r="68" spans="1:26" ht="10" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="82"/>
-      <c r="C68" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="D68" s="96"/>
-      <c r="E68" s="97"/>
+      <c r="C68" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="94"/>
+      <c r="E68" s="95"/>
       <c r="F68" s="47"/>
       <c r="G68" s="62"/>
       <c r="H68" s="47"/>
@@ -3735,8 +3740,8 @@
       <c r="P68" s="47"/>
       <c r="Q68" s="44"/>
       <c r="R68" s="45"/>
-      <c r="S68" s="46"/>
-      <c r="T68" s="43"/>
+      <c r="S68" s="64"/>
+      <c r="T68" s="47"/>
       <c r="U68" s="44"/>
       <c r="V68" s="45"/>
       <c r="W68" s="46"/>
@@ -3747,9 +3752,9 @@
     <row r="69" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A69" s="1"/>
       <c r="B69" s="82"/>
-      <c r="C69" s="98"/>
-      <c r="D69" s="99"/>
-      <c r="E69" s="100"/>
+      <c r="C69" s="96"/>
+      <c r="D69" s="97"/>
+      <c r="E69" s="98"/>
       <c r="F69" s="47"/>
       <c r="G69" s="62"/>
       <c r="H69" s="47"/>
@@ -3775,11 +3780,11 @@
     <row r="70" spans="1:26" ht="10" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="82"/>
-      <c r="C70" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="D70" s="96"/>
-      <c r="E70" s="97"/>
+      <c r="C70" s="93" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="94"/>
+      <c r="E70" s="95"/>
       <c r="F70" s="47"/>
       <c r="G70" s="62"/>
       <c r="H70" s="47"/>
@@ -3795,7 +3800,7 @@
       <c r="R70" s="45"/>
       <c r="S70" s="46"/>
       <c r="T70" s="43"/>
-      <c r="U70" s="52"/>
+      <c r="U70" s="44"/>
       <c r="V70" s="45"/>
       <c r="W70" s="46"/>
       <c r="X70" s="47"/>
@@ -3805,9 +3810,9 @@
     <row r="71" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A71" s="1"/>
       <c r="B71" s="82"/>
-      <c r="C71" s="98"/>
-      <c r="D71" s="99"/>
-      <c r="E71" s="100"/>
+      <c r="C71" s="96"/>
+      <c r="D71" s="97"/>
+      <c r="E71" s="98"/>
       <c r="F71" s="47"/>
       <c r="G71" s="62"/>
       <c r="H71" s="47"/>
@@ -3833,11 +3838,11 @@
     <row r="72" spans="1:26" ht="10" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="82"/>
-      <c r="C72" s="95" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72" s="96"/>
-      <c r="E72" s="97"/>
+      <c r="C72" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="D72" s="94"/>
+      <c r="E72" s="95"/>
       <c r="F72" s="47"/>
       <c r="G72" s="62"/>
       <c r="H72" s="47"/>
@@ -3852,7 +3857,7 @@
       <c r="Q72" s="44"/>
       <c r="R72" s="45"/>
       <c r="S72" s="46"/>
-      <c r="T72" s="47"/>
+      <c r="T72" s="43"/>
       <c r="U72" s="52"/>
       <c r="V72" s="45"/>
       <c r="W72" s="46"/>
@@ -3863,9 +3868,9 @@
     <row r="73" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A73" s="1"/>
       <c r="B73" s="82"/>
-      <c r="C73" s="98"/>
-      <c r="D73" s="99"/>
-      <c r="E73" s="100"/>
+      <c r="C73" s="96"/>
+      <c r="D73" s="97"/>
+      <c r="E73" s="98"/>
       <c r="F73" s="47"/>
       <c r="G73" s="62"/>
       <c r="H73" s="47"/>
@@ -3880,8 +3885,8 @@
       <c r="Q73" s="44"/>
       <c r="R73" s="45"/>
       <c r="S73" s="46"/>
-      <c r="T73" s="51"/>
-      <c r="U73" s="76"/>
+      <c r="T73" s="47"/>
+      <c r="U73" s="44"/>
       <c r="V73" s="45"/>
       <c r="W73" s="46"/>
       <c r="X73" s="47"/>
@@ -3891,11 +3896,11 @@
     <row r="74" spans="1:26" ht="10" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="82"/>
-      <c r="C74" s="95" t="s">
-        <v>48</v>
-      </c>
-      <c r="D74" s="96"/>
-      <c r="E74" s="97"/>
+      <c r="C74" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="94"/>
+      <c r="E74" s="95"/>
       <c r="F74" s="47"/>
       <c r="G74" s="62"/>
       <c r="H74" s="47"/>
@@ -3910,9 +3915,9 @@
       <c r="Q74" s="44"/>
       <c r="R74" s="45"/>
       <c r="S74" s="46"/>
-      <c r="T74" s="51"/>
+      <c r="T74" s="47"/>
       <c r="U74" s="52"/>
-      <c r="V74" s="74"/>
+      <c r="V74" s="45"/>
       <c r="W74" s="46"/>
       <c r="X74" s="47"/>
       <c r="Y74" s="44"/>
@@ -3921,9 +3926,9 @@
     <row r="75" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A75" s="1"/>
       <c r="B75" s="82"/>
-      <c r="C75" s="98"/>
-      <c r="D75" s="99"/>
-      <c r="E75" s="100"/>
+      <c r="C75" s="96"/>
+      <c r="D75" s="97"/>
+      <c r="E75" s="98"/>
       <c r="F75" s="47"/>
       <c r="G75" s="62"/>
       <c r="H75" s="47"/>
@@ -3938,9 +3943,9 @@
       <c r="Q75" s="44"/>
       <c r="R75" s="45"/>
       <c r="S75" s="46"/>
-      <c r="T75" s="47"/>
-      <c r="U75" s="44"/>
-      <c r="V75" s="74"/>
+      <c r="T75" s="51"/>
+      <c r="U75" s="76"/>
+      <c r="V75" s="45"/>
       <c r="W75" s="46"/>
       <c r="X75" s="47"/>
       <c r="Y75" s="44"/>
@@ -3948,147 +3953,147 @@
     </row>
     <row r="76" spans="1:26" ht="10" customHeight="1">
       <c r="A76" s="1"/>
-      <c r="B76" s="110"/>
-      <c r="C76" s="111"/>
-      <c r="D76" s="112"/>
-      <c r="E76" s="83"/>
-      <c r="F76" s="79"/>
-      <c r="G76" s="80"/>
-      <c r="H76" s="79"/>
-      <c r="I76" s="81"/>
-      <c r="J76" s="79"/>
-      <c r="K76" s="81"/>
-      <c r="L76" s="79"/>
-      <c r="M76" s="81"/>
-      <c r="N76" s="79"/>
-      <c r="O76" s="81"/>
-      <c r="P76" s="79"/>
-      <c r="Q76" s="81"/>
-      <c r="R76" s="79"/>
-      <c r="S76" s="81"/>
-      <c r="T76" s="79"/>
-      <c r="U76" s="81"/>
-      <c r="V76" s="79"/>
-      <c r="W76" s="81"/>
-      <c r="X76" s="79"/>
-      <c r="Y76" s="81"/>
+      <c r="B76" s="82"/>
+      <c r="C76" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="D76" s="94"/>
+      <c r="E76" s="95"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="62"/>
+      <c r="H76" s="47"/>
+      <c r="I76" s="44"/>
+      <c r="J76" s="45"/>
+      <c r="K76" s="46"/>
+      <c r="L76" s="47"/>
+      <c r="M76" s="44"/>
+      <c r="N76" s="45"/>
+      <c r="O76" s="46"/>
+      <c r="P76" s="47"/>
+      <c r="Q76" s="44"/>
+      <c r="R76" s="45"/>
+      <c r="S76" s="46"/>
+      <c r="T76" s="51"/>
+      <c r="U76" s="52"/>
+      <c r="V76" s="74"/>
+      <c r="W76" s="46"/>
+      <c r="X76" s="47"/>
+      <c r="Y76" s="44"/>
       <c r="Z76" s="1"/>
     </row>
-    <row r="77" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
-      <c r="B77" s="34"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="4"/>
-      <c r="L77" s="2"/>
-      <c r="M77" s="4"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="4"/>
-      <c r="T77" s="2"/>
-      <c r="U77" s="4"/>
-      <c r="X77" s="2"/>
-      <c r="Y77" s="4"/>
-    </row>
-    <row r="78" spans="1:26" ht="10" customHeight="1" thickBot="1">
+    <row r="77" spans="1:26" ht="10" customHeight="1" thickBot="1">
+      <c r="A77" s="1"/>
+      <c r="B77" s="82"/>
+      <c r="C77" s="96"/>
+      <c r="D77" s="97"/>
+      <c r="E77" s="98"/>
+      <c r="F77" s="47"/>
+      <c r="G77" s="62"/>
+      <c r="H77" s="47"/>
+      <c r="I77" s="44"/>
+      <c r="J77" s="45"/>
+      <c r="K77" s="46"/>
+      <c r="L77" s="47"/>
+      <c r="M77" s="44"/>
+      <c r="N77" s="45"/>
+      <c r="O77" s="46"/>
+      <c r="P77" s="47"/>
+      <c r="Q77" s="44"/>
+      <c r="R77" s="45"/>
+      <c r="S77" s="46"/>
+      <c r="T77" s="47"/>
+      <c r="U77" s="44"/>
+      <c r="V77" s="74"/>
+      <c r="W77" s="46"/>
+      <c r="X77" s="47"/>
+      <c r="Y77" s="44"/>
+      <c r="Z77" s="1"/>
+    </row>
+    <row r="78" spans="1:26" ht="10" customHeight="1">
       <c r="A78" s="1"/>
-      <c r="B78" s="101" t="s">
-        <v>2</v>
-      </c>
-      <c r="C78" s="102"/>
-      <c r="D78" s="103"/>
-      <c r="E78" s="85">
-        <v>12</v>
-      </c>
-      <c r="F78" s="67"/>
-      <c r="G78" s="68"/>
-      <c r="H78" s="67"/>
-      <c r="I78" s="69"/>
-      <c r="J78" s="67"/>
-      <c r="K78" s="69"/>
-      <c r="L78" s="67"/>
-      <c r="M78" s="69"/>
-      <c r="N78" s="67"/>
-      <c r="O78" s="69"/>
-      <c r="P78" s="67"/>
-      <c r="Q78" s="69"/>
-      <c r="R78" s="67"/>
-      <c r="S78" s="69"/>
-      <c r="T78" s="67"/>
-      <c r="U78" s="69"/>
-      <c r="V78" s="67"/>
-      <c r="W78" s="69"/>
-      <c r="X78" s="67"/>
-      <c r="Y78" s="68"/>
-      <c r="Z78" s="2"/>
-    </row>
-    <row r="79" spans="1:26" ht="10" customHeight="1">
-      <c r="A79" s="1"/>
-      <c r="B79" s="70"/>
-      <c r="C79" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="D79" s="96"/>
-      <c r="E79" s="97"/>
-      <c r="F79" s="47"/>
-      <c r="G79" s="62"/>
-      <c r="H79" s="47"/>
-      <c r="I79" s="44"/>
-      <c r="J79" s="45"/>
-      <c r="K79" s="46"/>
-      <c r="L79" s="47"/>
-      <c r="M79" s="44"/>
-      <c r="N79" s="45"/>
-      <c r="O79" s="46"/>
-      <c r="P79" s="47"/>
-      <c r="Q79" s="44"/>
-      <c r="R79" s="45"/>
-      <c r="S79" s="46"/>
-      <c r="T79" s="51"/>
-      <c r="U79" s="52"/>
-      <c r="V79" s="63"/>
-      <c r="W79" s="46"/>
-      <c r="X79" s="47"/>
-      <c r="Y79" s="44"/>
-      <c r="Z79" s="1"/>
+      <c r="B78" s="152"/>
+      <c r="C78" s="153"/>
+      <c r="D78" s="154"/>
+      <c r="E78" s="83"/>
+      <c r="F78" s="79"/>
+      <c r="G78" s="80"/>
+      <c r="H78" s="79"/>
+      <c r="I78" s="81"/>
+      <c r="J78" s="79"/>
+      <c r="K78" s="81"/>
+      <c r="L78" s="79"/>
+      <c r="M78" s="81"/>
+      <c r="N78" s="79"/>
+      <c r="O78" s="81"/>
+      <c r="P78" s="79"/>
+      <c r="Q78" s="81"/>
+      <c r="R78" s="79"/>
+      <c r="S78" s="81"/>
+      <c r="T78" s="79"/>
+      <c r="U78" s="81"/>
+      <c r="V78" s="79"/>
+      <c r="W78" s="81"/>
+      <c r="X78" s="79"/>
+      <c r="Y78" s="81"/>
+      <c r="Z78" s="1"/>
+    </row>
+    <row r="79" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
+      <c r="B79" s="34"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="35"/>
+      <c r="F79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="4"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="4"/>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="4"/>
+      <c r="T79" s="2"/>
+      <c r="U79" s="4"/>
+      <c r="X79" s="2"/>
+      <c r="Y79" s="4"/>
     </row>
     <row r="80" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A80" s="1"/>
-      <c r="B80" s="70"/>
-      <c r="C80" s="98"/>
-      <c r="D80" s="99"/>
-      <c r="E80" s="100"/>
-      <c r="F80" s="47"/>
-      <c r="G80" s="62"/>
-      <c r="H80" s="47"/>
-      <c r="I80" s="44"/>
-      <c r="J80" s="45"/>
-      <c r="K80" s="46"/>
-      <c r="L80" s="47"/>
-      <c r="M80" s="44"/>
-      <c r="N80" s="45"/>
-      <c r="O80" s="46"/>
-      <c r="P80" s="47"/>
-      <c r="Q80" s="44"/>
-      <c r="R80" s="45"/>
-      <c r="S80" s="46"/>
-      <c r="T80" s="47"/>
-      <c r="U80" s="44"/>
-      <c r="V80" s="45"/>
-      <c r="W80" s="46"/>
-      <c r="X80" s="47"/>
-      <c r="Y80" s="44"/>
-      <c r="Z80" s="1"/>
+      <c r="B80" s="147" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="148"/>
+      <c r="D80" s="149"/>
+      <c r="E80" s="85">
+        <v>12</v>
+      </c>
+      <c r="F80" s="67"/>
+      <c r="G80" s="68"/>
+      <c r="H80" s="67"/>
+      <c r="I80" s="69"/>
+      <c r="J80" s="67"/>
+      <c r="K80" s="69"/>
+      <c r="L80" s="67"/>
+      <c r="M80" s="69"/>
+      <c r="N80" s="67"/>
+      <c r="O80" s="69"/>
+      <c r="P80" s="67"/>
+      <c r="Q80" s="69"/>
+      <c r="R80" s="67"/>
+      <c r="S80" s="69"/>
+      <c r="T80" s="67"/>
+      <c r="U80" s="69"/>
+      <c r="V80" s="67"/>
+      <c r="W80" s="69"/>
+      <c r="X80" s="67"/>
+      <c r="Y80" s="68"/>
+      <c r="Z80" s="2"/>
     </row>
     <row r="81" spans="1:26" ht="10" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="70"/>
-      <c r="C81" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="D81" s="96"/>
-      <c r="E81" s="97"/>
+      <c r="C81" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="94"/>
+      <c r="E81" s="95"/>
       <c r="F81" s="47"/>
       <c r="G81" s="62"/>
       <c r="H81" s="47"/>
@@ -4103,10 +4108,10 @@
       <c r="Q81" s="44"/>
       <c r="R81" s="45"/>
       <c r="S81" s="46"/>
-      <c r="T81" s="47"/>
-      <c r="U81" s="44"/>
+      <c r="T81" s="51"/>
+      <c r="U81" s="52"/>
       <c r="V81" s="63"/>
-      <c r="W81" s="64"/>
+      <c r="W81" s="46"/>
       <c r="X81" s="47"/>
       <c r="Y81" s="44"/>
       <c r="Z81" s="1"/>
@@ -4114,9 +4119,9 @@
     <row r="82" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A82" s="1"/>
       <c r="B82" s="70"/>
-      <c r="C82" s="98"/>
-      <c r="D82" s="99"/>
-      <c r="E82" s="100"/>
+      <c r="C82" s="96"/>
+      <c r="D82" s="97"/>
+      <c r="E82" s="98"/>
       <c r="F82" s="47"/>
       <c r="G82" s="62"/>
       <c r="H82" s="47"/>
@@ -4141,147 +4146,147 @@
     </row>
     <row r="83" spans="1:26" ht="10" customHeight="1">
       <c r="A83" s="1"/>
-      <c r="B83" s="153"/>
-      <c r="C83" s="154"/>
-      <c r="D83" s="155"/>
-      <c r="E83" s="71"/>
-      <c r="F83" s="67"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="67"/>
-      <c r="I83" s="69"/>
-      <c r="J83" s="67"/>
-      <c r="K83" s="69"/>
-      <c r="L83" s="67"/>
-      <c r="M83" s="69"/>
-      <c r="N83" s="67"/>
-      <c r="O83" s="69"/>
-      <c r="P83" s="67"/>
-      <c r="Q83" s="69"/>
-      <c r="R83" s="67"/>
-      <c r="S83" s="69"/>
-      <c r="T83" s="67"/>
-      <c r="U83" s="69"/>
-      <c r="V83" s="67"/>
-      <c r="W83" s="69"/>
-      <c r="X83" s="67"/>
-      <c r="Y83" s="69"/>
+      <c r="B83" s="70"/>
+      <c r="C83" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="94"/>
+      <c r="E83" s="95"/>
+      <c r="F83" s="47"/>
+      <c r="G83" s="62"/>
+      <c r="H83" s="47"/>
+      <c r="I83" s="44"/>
+      <c r="J83" s="45"/>
+      <c r="K83" s="46"/>
+      <c r="L83" s="47"/>
+      <c r="M83" s="44"/>
+      <c r="N83" s="45"/>
+      <c r="O83" s="46"/>
+      <c r="P83" s="47"/>
+      <c r="Q83" s="44"/>
+      <c r="R83" s="45"/>
+      <c r="S83" s="46"/>
+      <c r="T83" s="47"/>
+      <c r="U83" s="44"/>
+      <c r="V83" s="63"/>
+      <c r="W83" s="64"/>
+      <c r="X83" s="47"/>
+      <c r="Y83" s="44"/>
       <c r="Z83" s="1"/>
     </row>
-    <row r="84" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
-      <c r="B84" s="34"/>
-      <c r="C84" s="34"/>
-      <c r="D84" s="34"/>
-      <c r="E84" s="35"/>
-      <c r="F84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="4"/>
-      <c r="L84" s="2"/>
-      <c r="M84" s="4"/>
-      <c r="P84" s="2"/>
-      <c r="Q84" s="4"/>
-      <c r="T84" s="2"/>
-      <c r="U84" s="4"/>
-      <c r="X84" s="2"/>
-      <c r="Y84" s="4"/>
-    </row>
-    <row r="85" spans="1:26" ht="10" customHeight="1" thickBot="1">
+    <row r="84" spans="1:26" ht="10" customHeight="1" thickBot="1">
+      <c r="A84" s="1"/>
+      <c r="B84" s="70"/>
+      <c r="C84" s="96"/>
+      <c r="D84" s="97"/>
+      <c r="E84" s="98"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="62"/>
+      <c r="H84" s="47"/>
+      <c r="I84" s="44"/>
+      <c r="J84" s="45"/>
+      <c r="K84" s="46"/>
+      <c r="L84" s="47"/>
+      <c r="M84" s="44"/>
+      <c r="N84" s="45"/>
+      <c r="O84" s="46"/>
+      <c r="P84" s="47"/>
+      <c r="Q84" s="44"/>
+      <c r="R84" s="45"/>
+      <c r="S84" s="46"/>
+      <c r="T84" s="47"/>
+      <c r="U84" s="44"/>
+      <c r="V84" s="45"/>
+      <c r="W84" s="46"/>
+      <c r="X84" s="47"/>
+      <c r="Y84" s="44"/>
+      <c r="Z84" s="1"/>
+    </row>
+    <row r="85" spans="1:26" ht="10" customHeight="1">
       <c r="A85" s="1"/>
-      <c r="B85" s="107" t="s">
-        <v>27</v>
-      </c>
-      <c r="C85" s="108"/>
-      <c r="D85" s="109"/>
-      <c r="E85" s="86">
-        <v>8</v>
-      </c>
-      <c r="F85" s="15"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="15"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="15"/>
-      <c r="K85" s="16"/>
-      <c r="L85" s="15"/>
-      <c r="M85" s="16"/>
-      <c r="N85" s="15"/>
-      <c r="O85" s="16"/>
-      <c r="P85" s="15"/>
-      <c r="Q85" s="16"/>
-      <c r="R85" s="15"/>
-      <c r="S85" s="16"/>
-      <c r="T85" s="15"/>
-      <c r="U85" s="16"/>
-      <c r="V85" s="15"/>
-      <c r="W85" s="16"/>
-      <c r="X85" s="15"/>
-      <c r="Y85" s="73"/>
+      <c r="B85" s="102"/>
+      <c r="C85" s="103"/>
+      <c r="D85" s="104"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="67"/>
+      <c r="G85" s="68"/>
+      <c r="H85" s="67"/>
+      <c r="I85" s="69"/>
+      <c r="J85" s="67"/>
+      <c r="K85" s="69"/>
+      <c r="L85" s="67"/>
+      <c r="M85" s="69"/>
+      <c r="N85" s="67"/>
+      <c r="O85" s="69"/>
+      <c r="P85" s="67"/>
+      <c r="Q85" s="69"/>
+      <c r="R85" s="67"/>
+      <c r="S85" s="69"/>
+      <c r="T85" s="67"/>
+      <c r="U85" s="69"/>
+      <c r="V85" s="67"/>
+      <c r="W85" s="69"/>
+      <c r="X85" s="67"/>
+      <c r="Y85" s="69"/>
       <c r="Z85" s="1"/>
     </row>
-    <row r="86" spans="1:26" ht="10" customHeight="1">
-      <c r="A86" s="1"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="95" t="s">
-        <v>24</v>
-      </c>
-      <c r="D86" s="96"/>
-      <c r="E86" s="97"/>
-      <c r="F86" s="47"/>
-      <c r="G86" s="62"/>
-      <c r="H86" s="47"/>
-      <c r="I86" s="44"/>
-      <c r="J86" s="45"/>
-      <c r="K86" s="46"/>
-      <c r="L86" s="47"/>
-      <c r="M86" s="44"/>
-      <c r="N86" s="45"/>
-      <c r="O86" s="46"/>
-      <c r="P86" s="47"/>
-      <c r="Q86" s="44"/>
-      <c r="R86" s="45"/>
-      <c r="S86" s="46"/>
-      <c r="T86" s="47"/>
-      <c r="U86" s="44"/>
-      <c r="V86" s="45"/>
-      <c r="W86" s="46"/>
-      <c r="X86" s="43"/>
-      <c r="Y86" s="44"/>
-      <c r="Z86" s="1"/>
+    <row r="86" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
+      <c r="B86" s="34"/>
+      <c r="C86" s="34"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="35"/>
+      <c r="F86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="4"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="4"/>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="4"/>
+      <c r="T86" s="2"/>
+      <c r="U86" s="4"/>
+      <c r="X86" s="2"/>
+      <c r="Y86" s="4"/>
     </row>
     <row r="87" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A87" s="1"/>
-      <c r="B87" s="6"/>
-      <c r="C87" s="98"/>
-      <c r="D87" s="99"/>
-      <c r="E87" s="100"/>
-      <c r="F87" s="47"/>
-      <c r="G87" s="62"/>
-      <c r="H87" s="47"/>
-      <c r="I87" s="44"/>
-      <c r="J87" s="45"/>
-      <c r="K87" s="46"/>
-      <c r="L87" s="47"/>
-      <c r="M87" s="44"/>
-      <c r="N87" s="45"/>
-      <c r="O87" s="46"/>
-      <c r="P87" s="47"/>
-      <c r="Q87" s="44"/>
-      <c r="R87" s="45"/>
-      <c r="S87" s="46"/>
-      <c r="T87" s="47"/>
-      <c r="U87" s="44"/>
-      <c r="V87" s="45"/>
-      <c r="W87" s="46"/>
-      <c r="X87" s="47"/>
-      <c r="Y87" s="44"/>
+      <c r="B87" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="C87" s="100"/>
+      <c r="D87" s="101"/>
+      <c r="E87" s="86">
+        <v>8</v>
+      </c>
+      <c r="F87" s="15"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="16"/>
+      <c r="L87" s="15"/>
+      <c r="M87" s="16"/>
+      <c r="N87" s="15"/>
+      <c r="O87" s="16"/>
+      <c r="P87" s="15"/>
+      <c r="Q87" s="16"/>
+      <c r="R87" s="15"/>
+      <c r="S87" s="16"/>
+      <c r="T87" s="15"/>
+      <c r="U87" s="16"/>
+      <c r="V87" s="15"/>
+      <c r="W87" s="16"/>
+      <c r="X87" s="15"/>
+      <c r="Y87" s="73"/>
       <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" ht="10" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="6"/>
-      <c r="C88" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="D88" s="96"/>
-      <c r="E88" s="97"/>
+      <c r="C88" s="93" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" s="94"/>
+      <c r="E88" s="95"/>
       <c r="F88" s="47"/>
       <c r="G88" s="62"/>
       <c r="H88" s="47"/>
@@ -4307,9 +4312,9 @@
     <row r="89" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A89" s="1"/>
       <c r="B89" s="6"/>
-      <c r="C89" s="98"/>
-      <c r="D89" s="99"/>
-      <c r="E89" s="100"/>
+      <c r="C89" s="96"/>
+      <c r="D89" s="97"/>
+      <c r="E89" s="98"/>
       <c r="F89" s="47"/>
       <c r="G89" s="62"/>
       <c r="H89" s="47"/>
@@ -4335,11 +4340,11 @@
     <row r="90" spans="1:26" ht="10" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="6"/>
-      <c r="C90" s="95" t="s">
-        <v>49</v>
-      </c>
-      <c r="D90" s="96"/>
-      <c r="E90" s="97"/>
+      <c r="C90" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="D90" s="94"/>
+      <c r="E90" s="95"/>
       <c r="F90" s="47"/>
       <c r="G90" s="62"/>
       <c r="H90" s="47"/>
@@ -4359,15 +4364,15 @@
       <c r="V90" s="45"/>
       <c r="W90" s="46"/>
       <c r="X90" s="43"/>
-      <c r="Y90" s="52"/>
+      <c r="Y90" s="44"/>
       <c r="Z90" s="1"/>
     </row>
     <row r="91" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A91" s="1"/>
       <c r="B91" s="6"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="99"/>
-      <c r="E91" s="100"/>
+      <c r="C91" s="96"/>
+      <c r="D91" s="97"/>
+      <c r="E91" s="98"/>
       <c r="F91" s="47"/>
       <c r="G91" s="62"/>
       <c r="H91" s="47"/>
@@ -4387,62 +4392,73 @@
       <c r="V91" s="45"/>
       <c r="W91" s="46"/>
       <c r="X91" s="47"/>
-      <c r="Y91" s="46"/>
-      <c r="Z91" s="2"/>
+      <c r="Y91" s="44"/>
+      <c r="Z91" s="1"/>
     </row>
     <row r="92" spans="1:26" ht="10" customHeight="1">
       <c r="A92" s="1"/>
-      <c r="B92" s="104"/>
-      <c r="C92" s="105"/>
-      <c r="D92" s="106"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="15"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="15"/>
-      <c r="I92" s="16"/>
-      <c r="J92" s="15"/>
-      <c r="K92" s="16"/>
-      <c r="L92" s="15"/>
-      <c r="M92" s="16"/>
-      <c r="N92" s="15"/>
-      <c r="O92" s="16"/>
-      <c r="P92" s="15"/>
-      <c r="Q92" s="16"/>
-      <c r="R92" s="15"/>
-      <c r="S92" s="16"/>
-      <c r="T92" s="15"/>
-      <c r="U92" s="16"/>
-      <c r="V92" s="15"/>
-      <c r="W92" s="16"/>
-      <c r="X92" s="15"/>
-      <c r="Y92" s="16"/>
-      <c r="Z92" s="2"/>
-    </row>
-    <row r="93" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
-      <c r="B93" s="34"/>
-      <c r="C93" s="34"/>
-      <c r="D93" s="34"/>
-      <c r="E93" s="35"/>
-      <c r="F93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="4"/>
-      <c r="L93" s="2"/>
-      <c r="M93" s="4"/>
-      <c r="P93" s="2"/>
-      <c r="Q93" s="4"/>
-      <c r="T93" s="2"/>
-      <c r="U93" s="4"/>
-      <c r="X93" s="2"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="93" t="s">
+        <v>49</v>
+      </c>
+      <c r="D92" s="94"/>
+      <c r="E92" s="95"/>
+      <c r="F92" s="47"/>
+      <c r="G92" s="62"/>
+      <c r="H92" s="47"/>
+      <c r="I92" s="44"/>
+      <c r="J92" s="45"/>
+      <c r="K92" s="46"/>
+      <c r="L92" s="47"/>
+      <c r="M92" s="44"/>
+      <c r="N92" s="45"/>
+      <c r="O92" s="46"/>
+      <c r="P92" s="47"/>
+      <c r="Q92" s="44"/>
+      <c r="R92" s="45"/>
+      <c r="S92" s="46"/>
+      <c r="T92" s="47"/>
+      <c r="U92" s="44"/>
+      <c r="V92" s="45"/>
+      <c r="W92" s="46"/>
+      <c r="X92" s="43"/>
+      <c r="Y92" s="52"/>
+      <c r="Z92" s="1"/>
+    </row>
+    <row r="93" spans="1:26" ht="10" customHeight="1" thickBot="1">
+      <c r="A93" s="1"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="96"/>
+      <c r="D93" s="97"/>
+      <c r="E93" s="98"/>
+      <c r="F93" s="47"/>
+      <c r="G93" s="62"/>
+      <c r="H93" s="47"/>
+      <c r="I93" s="44"/>
+      <c r="J93" s="45"/>
+      <c r="K93" s="46"/>
+      <c r="L93" s="47"/>
+      <c r="M93" s="44"/>
+      <c r="N93" s="45"/>
+      <c r="O93" s="46"/>
+      <c r="P93" s="47"/>
+      <c r="Q93" s="44"/>
+      <c r="R93" s="45"/>
+      <c r="S93" s="46"/>
+      <c r="T93" s="47"/>
+      <c r="U93" s="44"/>
+      <c r="V93" s="45"/>
+      <c r="W93" s="46"/>
+      <c r="X93" s="47"/>
+      <c r="Y93" s="46"/>
       <c r="Z93" s="2"/>
     </row>
-    <row r="94" spans="1:26" ht="10" customHeight="1" thickBot="1">
+    <row r="94" spans="1:26" ht="10" customHeight="1">
       <c r="A94" s="1"/>
-      <c r="B94" s="107" t="s">
-        <v>26</v>
-      </c>
-      <c r="C94" s="108"/>
-      <c r="D94" s="109"/>
-      <c r="E94" s="72"/>
+      <c r="B94" s="119"/>
+      <c r="C94" s="150"/>
+      <c r="D94" s="151"/>
+      <c r="E94" s="22"/>
       <c r="F94" s="15"/>
       <c r="G94" s="16"/>
       <c r="H94" s="15"/>
@@ -4465,100 +4481,89 @@
       <c r="Y94" s="16"/>
       <c r="Z94" s="2"/>
     </row>
-    <row r="95" spans="1:26" ht="10" customHeight="1">
-      <c r="A95" s="1"/>
-      <c r="B95" s="6"/>
-      <c r="C95" s="95" t="s">
-        <v>32</v>
-      </c>
-      <c r="D95" s="96"/>
-      <c r="E95" s="97"/>
-      <c r="F95" s="19"/>
-      <c r="G95" s="31"/>
-      <c r="H95" s="19"/>
-      <c r="I95" s="31"/>
-      <c r="J95" s="19"/>
-      <c r="K95" s="31"/>
-      <c r="L95" s="19"/>
-      <c r="M95" s="31"/>
-      <c r="N95" s="19"/>
-      <c r="O95" s="31"/>
-      <c r="P95" s="19"/>
-      <c r="Q95" s="31"/>
-      <c r="R95" s="19"/>
-      <c r="S95" s="31"/>
-      <c r="T95" s="19"/>
-      <c r="U95" s="31"/>
-      <c r="V95" s="19"/>
-      <c r="W95" s="31"/>
-      <c r="X95" s="19"/>
-      <c r="Y95" s="31"/>
+    <row r="95" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
+      <c r="B95" s="34"/>
+      <c r="C95" s="34"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="35"/>
+      <c r="F95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="4"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="4"/>
+      <c r="P95" s="2"/>
+      <c r="Q95" s="4"/>
+      <c r="T95" s="2"/>
+      <c r="U95" s="4"/>
+      <c r="X95" s="2"/>
       <c r="Z95" s="2"/>
     </row>
     <row r="96" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A96" s="1"/>
-      <c r="B96" s="6"/>
-      <c r="C96" s="98"/>
-      <c r="D96" s="99"/>
-      <c r="E96" s="100"/>
-      <c r="F96" s="29"/>
-      <c r="G96" s="32"/>
-      <c r="H96" s="51"/>
-      <c r="I96" s="53"/>
-      <c r="J96" s="74"/>
-      <c r="K96" s="75"/>
-      <c r="L96" s="51"/>
-      <c r="M96" s="76"/>
-      <c r="N96" s="74"/>
-      <c r="O96" s="75"/>
-      <c r="P96" s="51"/>
-      <c r="Q96" s="76"/>
-      <c r="R96" s="74"/>
-      <c r="S96" s="75"/>
-      <c r="T96" s="51"/>
-      <c r="U96" s="76"/>
-      <c r="V96" s="74"/>
-      <c r="W96" s="75"/>
-      <c r="X96" s="51"/>
-      <c r="Y96" s="75"/>
+      <c r="B96" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C96" s="100"/>
+      <c r="D96" s="101"/>
+      <c r="E96" s="72"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="15"/>
+      <c r="M96" s="16"/>
+      <c r="N96" s="15"/>
+      <c r="O96" s="16"/>
+      <c r="P96" s="15"/>
+      <c r="Q96" s="16"/>
+      <c r="R96" s="15"/>
+      <c r="S96" s="16"/>
+      <c r="T96" s="15"/>
+      <c r="U96" s="16"/>
+      <c r="V96" s="15"/>
+      <c r="W96" s="16"/>
+      <c r="X96" s="15"/>
+      <c r="Y96" s="16"/>
       <c r="Z96" s="2"/>
     </row>
     <row r="97" spans="1:26" ht="10" customHeight="1">
       <c r="A97" s="1"/>
       <c r="B97" s="6"/>
-      <c r="C97" s="95" t="s">
-        <v>57</v>
-      </c>
-      <c r="D97" s="96"/>
-      <c r="E97" s="97"/>
-      <c r="F97" s="29"/>
-      <c r="G97" s="90"/>
-      <c r="H97" s="51"/>
-      <c r="I97" s="52"/>
-      <c r="J97" s="74"/>
-      <c r="K97" s="64"/>
-      <c r="L97" s="51"/>
-      <c r="M97" s="52"/>
-      <c r="N97" s="74"/>
-      <c r="O97" s="64"/>
-      <c r="P97" s="51"/>
-      <c r="Q97" s="52"/>
-      <c r="R97" s="74"/>
-      <c r="S97" s="64"/>
-      <c r="T97" s="51"/>
-      <c r="U97" s="52"/>
-      <c r="V97" s="74"/>
-      <c r="W97" s="64"/>
-      <c r="X97" s="51"/>
-      <c r="Y97" s="64"/>
+      <c r="C97" s="93" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97" s="94"/>
+      <c r="E97" s="95"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="31"/>
+      <c r="H97" s="19"/>
+      <c r="I97" s="31"/>
+      <c r="J97" s="19"/>
+      <c r="K97" s="31"/>
+      <c r="L97" s="19"/>
+      <c r="M97" s="31"/>
+      <c r="N97" s="19"/>
+      <c r="O97" s="31"/>
+      <c r="P97" s="19"/>
+      <c r="Q97" s="31"/>
+      <c r="R97" s="19"/>
+      <c r="S97" s="31"/>
+      <c r="T97" s="19"/>
+      <c r="U97" s="31"/>
+      <c r="V97" s="19"/>
+      <c r="W97" s="31"/>
+      <c r="X97" s="19"/>
+      <c r="Y97" s="31"/>
       <c r="Z97" s="2"/>
     </row>
     <row r="98" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A98" s="1"/>
       <c r="B98" s="6"/>
-      <c r="C98" s="98"/>
-      <c r="D98" s="99"/>
-      <c r="E98" s="100"/>
+      <c r="C98" s="96"/>
+      <c r="D98" s="97"/>
+      <c r="E98" s="98"/>
       <c r="F98" s="29"/>
       <c r="G98" s="32"/>
       <c r="H98" s="51"/>
@@ -4584,43 +4589,43 @@
     <row r="99" spans="1:26" ht="10" customHeight="1">
       <c r="A99" s="1"/>
       <c r="B99" s="6"/>
-      <c r="C99" s="95" t="s">
-        <v>33</v>
-      </c>
-      <c r="D99" s="96"/>
-      <c r="E99" s="97"/>
+      <c r="C99" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="D99" s="94"/>
+      <c r="E99" s="95"/>
       <c r="F99" s="29"/>
-      <c r="G99" s="50"/>
+      <c r="G99" s="90"/>
       <c r="H99" s="51"/>
-      <c r="I99" s="76"/>
+      <c r="I99" s="52"/>
       <c r="J99" s="74"/>
       <c r="K99" s="64"/>
       <c r="L99" s="51"/>
-      <c r="M99" s="76"/>
+      <c r="M99" s="52"/>
       <c r="N99" s="74"/>
-      <c r="O99" s="75"/>
+      <c r="O99" s="64"/>
       <c r="P99" s="51"/>
-      <c r="Q99" s="76"/>
+      <c r="Q99" s="52"/>
       <c r="R99" s="74"/>
-      <c r="S99" s="75"/>
+      <c r="S99" s="64"/>
       <c r="T99" s="51"/>
-      <c r="U99" s="76"/>
+      <c r="U99" s="52"/>
       <c r="V99" s="74"/>
-      <c r="W99" s="75"/>
+      <c r="W99" s="64"/>
       <c r="X99" s="51"/>
-      <c r="Y99" s="75"/>
+      <c r="Y99" s="64"/>
       <c r="Z99" s="2"/>
     </row>
     <row r="100" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A100" s="1"/>
       <c r="B100" s="6"/>
-      <c r="C100" s="98"/>
-      <c r="D100" s="99"/>
-      <c r="E100" s="100"/>
+      <c r="C100" s="96"/>
+      <c r="D100" s="97"/>
+      <c r="E100" s="98"/>
       <c r="F100" s="29"/>
-      <c r="G100" s="50"/>
+      <c r="G100" s="32"/>
       <c r="H100" s="51"/>
-      <c r="I100" s="76"/>
+      <c r="I100" s="53"/>
       <c r="J100" s="74"/>
       <c r="K100" s="75"/>
       <c r="L100" s="51"/>
@@ -4642,43 +4647,41 @@
     <row r="101" spans="1:26" ht="10" customHeight="1">
       <c r="A101" s="1"/>
       <c r="B101" s="6"/>
-      <c r="C101" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="D101" s="96"/>
-      <c r="E101" s="88">
-        <v>5</v>
-      </c>
-      <c r="F101" s="43"/>
-      <c r="G101" s="18"/>
-      <c r="H101" s="43"/>
+      <c r="C101" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="D101" s="94"/>
+      <c r="E101" s="95"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="50"/>
+      <c r="H101" s="51"/>
       <c r="I101" s="76"/>
-      <c r="J101" s="63"/>
-      <c r="K101" s="75"/>
-      <c r="L101" s="43"/>
+      <c r="J101" s="74"/>
+      <c r="K101" s="64"/>
+      <c r="L101" s="51"/>
       <c r="M101" s="76"/>
-      <c r="N101" s="63"/>
+      <c r="N101" s="74"/>
       <c r="O101" s="75"/>
-      <c r="P101" s="43"/>
+      <c r="P101" s="51"/>
       <c r="Q101" s="76"/>
-      <c r="R101" s="63"/>
+      <c r="R101" s="74"/>
       <c r="S101" s="75"/>
-      <c r="T101" s="43"/>
+      <c r="T101" s="51"/>
       <c r="U101" s="76"/>
-      <c r="V101" s="63"/>
+      <c r="V101" s="74"/>
       <c r="W101" s="75"/>
-      <c r="X101" s="43"/>
+      <c r="X101" s="51"/>
       <c r="Y101" s="75"/>
       <c r="Z101" s="2"/>
     </row>
     <row r="102" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A102" s="1"/>
       <c r="B102" s="6"/>
-      <c r="C102" s="98"/>
-      <c r="D102" s="99"/>
-      <c r="E102" s="66"/>
-      <c r="F102" s="49"/>
-      <c r="G102" s="77"/>
+      <c r="C102" s="96"/>
+      <c r="D102" s="97"/>
+      <c r="E102" s="98"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="50"/>
       <c r="H102" s="51"/>
       <c r="I102" s="76"/>
       <c r="J102" s="74"/>
@@ -4699,142 +4702,146 @@
       <c r="Y102" s="75"/>
       <c r="Z102" s="2"/>
     </row>
-    <row r="103" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B103" s="104"/>
-      <c r="C103" s="105"/>
-      <c r="D103" s="106"/>
-      <c r="E103" s="22"/>
-      <c r="F103" s="15"/>
-      <c r="G103" s="16"/>
-      <c r="H103" s="15"/>
-      <c r="I103" s="16"/>
-      <c r="J103" s="15"/>
-      <c r="K103" s="16"/>
-      <c r="L103" s="15"/>
-      <c r="M103" s="16"/>
-      <c r="N103" s="15"/>
-      <c r="O103" s="16"/>
-      <c r="P103" s="15"/>
-      <c r="Q103" s="16"/>
-      <c r="R103" s="15"/>
-      <c r="S103" s="16"/>
-      <c r="T103" s="15"/>
-      <c r="U103" s="16"/>
-      <c r="V103" s="15"/>
-      <c r="W103" s="16"/>
-      <c r="X103" s="15"/>
-      <c r="Y103" s="16"/>
+    <row r="103" spans="1:26" ht="10" customHeight="1">
+      <c r="A103" s="1"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="93" t="s">
+        <v>50</v>
+      </c>
+      <c r="D103" s="94"/>
+      <c r="E103" s="88">
+        <v>5</v>
+      </c>
+      <c r="F103" s="43"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="43"/>
+      <c r="I103" s="76"/>
+      <c r="J103" s="63"/>
+      <c r="K103" s="75"/>
+      <c r="L103" s="43"/>
+      <c r="M103" s="76"/>
+      <c r="N103" s="63"/>
+      <c r="O103" s="75"/>
+      <c r="P103" s="43"/>
+      <c r="Q103" s="76"/>
+      <c r="R103" s="63"/>
+      <c r="S103" s="75"/>
+      <c r="T103" s="43"/>
+      <c r="U103" s="76"/>
+      <c r="V103" s="63"/>
+      <c r="W103" s="75"/>
+      <c r="X103" s="43"/>
+      <c r="Y103" s="75"/>
       <c r="Z103" s="2"/>
     </row>
-    <row r="104" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
-      <c r="B104" s="94"/>
-      <c r="C104" s="94"/>
-      <c r="D104" s="94"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="4"/>
-      <c r="L104" s="2"/>
-      <c r="M104" s="4"/>
-      <c r="P104" s="2"/>
-      <c r="Q104" s="4"/>
-      <c r="T104" s="2"/>
-      <c r="U104" s="4"/>
-      <c r="X104" s="2"/>
+    <row r="104" spans="1:26" ht="10" customHeight="1" thickBot="1">
+      <c r="A104" s="1"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="96"/>
+      <c r="D104" s="97"/>
+      <c r="E104" s="66"/>
+      <c r="F104" s="49"/>
+      <c r="G104" s="77"/>
+      <c r="H104" s="51"/>
+      <c r="I104" s="76"/>
+      <c r="J104" s="74"/>
+      <c r="K104" s="75"/>
+      <c r="L104" s="51"/>
+      <c r="M104" s="76"/>
+      <c r="N104" s="74"/>
+      <c r="O104" s="75"/>
+      <c r="P104" s="51"/>
+      <c r="Q104" s="76"/>
+      <c r="R104" s="74"/>
+      <c r="S104" s="75"/>
+      <c r="T104" s="51"/>
+      <c r="U104" s="76"/>
+      <c r="V104" s="74"/>
+      <c r="W104" s="75"/>
+      <c r="X104" s="51"/>
+      <c r="Y104" s="75"/>
       <c r="Z104" s="2"/>
     </row>
     <row r="105" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B105" s="127" t="s">
+      <c r="B105" s="119"/>
+      <c r="C105" s="150"/>
+      <c r="D105" s="151"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="15"/>
+      <c r="G105" s="16"/>
+      <c r="H105" s="15"/>
+      <c r="I105" s="16"/>
+      <c r="J105" s="15"/>
+      <c r="K105" s="16"/>
+      <c r="L105" s="15"/>
+      <c r="M105" s="16"/>
+      <c r="N105" s="15"/>
+      <c r="O105" s="16"/>
+      <c r="P105" s="15"/>
+      <c r="Q105" s="16"/>
+      <c r="R105" s="15"/>
+      <c r="S105" s="16"/>
+      <c r="T105" s="15"/>
+      <c r="U105" s="16"/>
+      <c r="V105" s="15"/>
+      <c r="W105" s="16"/>
+      <c r="X105" s="15"/>
+      <c r="Y105" s="16"/>
+      <c r="Z105" s="2"/>
+    </row>
+    <row r="106" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
+      <c r="B106" s="146"/>
+      <c r="C106" s="146"/>
+      <c r="D106" s="146"/>
+      <c r="E106" s="35"/>
+      <c r="F106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="4"/>
+      <c r="L106" s="2"/>
+      <c r="M106" s="4"/>
+      <c r="P106" s="2"/>
+      <c r="Q106" s="4"/>
+      <c r="T106" s="2"/>
+      <c r="U106" s="4"/>
+      <c r="X106" s="2"/>
+      <c r="Z106" s="2"/>
+    </row>
+    <row r="107" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
+      <c r="B107" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="C105" s="128"/>
-      <c r="D105" s="128"/>
-      <c r="E105" s="87">
+      <c r="C107" s="134"/>
+      <c r="D107" s="134"/>
+      <c r="E107" s="87">
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:26" ht="10" customHeight="1" thickBot="1">
-      <c r="A106" s="1"/>
-      <c r="B106" s="129"/>
-      <c r="C106" s="130"/>
-      <c r="D106" s="130"/>
-      <c r="E106" s="78"/>
-      <c r="F106" s="3"/>
-      <c r="G106" s="3"/>
-      <c r="H106" s="3"/>
-      <c r="I106" s="3"/>
-      <c r="J106" s="3"/>
-      <c r="K106" s="3"/>
-      <c r="L106" s="3"/>
-      <c r="M106" s="3"/>
-      <c r="N106" s="3"/>
-      <c r="O106" s="3"/>
-      <c r="P106" s="3"/>
-      <c r="Q106" s="3"/>
-      <c r="R106" s="3"/>
-      <c r="S106" s="3"/>
-      <c r="T106" s="3"/>
-      <c r="U106" s="3"/>
-      <c r="V106" s="3"/>
-      <c r="W106" s="3"/>
-      <c r="X106" s="3"/>
-      <c r="Y106" s="3"/>
-      <c r="Z106" s="1"/>
-    </row>
-    <row r="107" spans="1:26">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3"/>
-      <c r="I107" s="3"/>
-      <c r="J107" s="3"/>
-      <c r="K107" s="3"/>
-      <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="O107" s="1"/>
-      <c r="P107" s="1"/>
-      <c r="Q107" s="1"/>
-      <c r="R107" s="1"/>
-      <c r="S107" s="1"/>
-      <c r="T107" s="1"/>
-      <c r="U107" s="1"/>
-      <c r="V107" s="1"/>
-      <c r="W107" s="1"/>
-      <c r="X107" s="1"/>
-      <c r="Y107" s="1"/>
-      <c r="Z107" s="1"/>
-    </row>
-    <row r="108" spans="1:26">
+    <row r="108" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="I108" s="1"/>
-      <c r="J108" s="1"/>
-      <c r="K108" s="1"/>
-      <c r="L108" s="1"/>
-      <c r="M108" s="1"/>
-      <c r="N108" s="1"/>
-      <c r="O108" s="1"/>
-      <c r="P108" s="1"/>
-      <c r="Q108" s="1"/>
-      <c r="R108" s="1"/>
-      <c r="S108" s="1"/>
-      <c r="T108" s="1"/>
-      <c r="U108" s="1"/>
-      <c r="V108" s="1"/>
-      <c r="W108" s="1"/>
-      <c r="X108" s="1"/>
-      <c r="Y108" s="1"/>
+      <c r="B108" s="135"/>
+      <c r="C108" s="136"/>
+      <c r="D108" s="136"/>
+      <c r="E108" s="78"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="3"/>
+      <c r="T108" s="3"/>
+      <c r="U108" s="3"/>
+      <c r="V108" s="3"/>
+      <c r="W108" s="3"/>
+      <c r="X108" s="3"/>
+      <c r="Y108" s="3"/>
       <c r="Z108" s="1"/>
     </row>
     <row r="109" spans="1:26">
@@ -4843,15 +4850,15 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="1"/>
-      <c r="J109" s="1"/>
-      <c r="K109" s="1"/>
-      <c r="L109" s="1"/>
-      <c r="M109" s="1"/>
-      <c r="N109" s="1"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
       <c r="O109" s="1"/>
       <c r="P109" s="1"/>
       <c r="Q109" s="1"/>
@@ -4921,55 +4928,103 @@
       <c r="Y111" s="1"/>
       <c r="Z111" s="1"/>
     </row>
-    <row r="116" spans="13:14">
-      <c r="M116" s="1"/>
-      <c r="N116" s="1"/>
-    </row>
-    <row r="117" spans="13:14">
-      <c r="M117" s="1"/>
-      <c r="N117" s="1"/>
-    </row>
-    <row r="118" spans="13:14">
+    <row r="112" spans="1:26">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1"/>
+      <c r="P112" s="1"/>
+      <c r="Q112" s="1"/>
+      <c r="R112" s="1"/>
+      <c r="S112" s="1"/>
+      <c r="T112" s="1"/>
+      <c r="U112" s="1"/>
+      <c r="V112" s="1"/>
+      <c r="W112" s="1"/>
+      <c r="X112" s="1"/>
+      <c r="Y112" s="1"/>
+      <c r="Z112" s="1"/>
+    </row>
+    <row r="113" spans="1:26">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+      <c r="Q113" s="1"/>
+      <c r="R113" s="1"/>
+      <c r="S113" s="1"/>
+      <c r="T113" s="1"/>
+      <c r="U113" s="1"/>
+      <c r="V113" s="1"/>
+      <c r="W113" s="1"/>
+      <c r="X113" s="1"/>
+      <c r="Y113" s="1"/>
+      <c r="Z113" s="1"/>
+    </row>
+    <row r="118" spans="1:26">
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
     </row>
-    <row r="119" spans="13:14">
+    <row r="119" spans="1:26">
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
     </row>
-    <row r="120" spans="13:14">
+    <row r="120" spans="1:26">
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
     </row>
-    <row r="121" spans="13:14">
+    <row r="121" spans="1:26">
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
     </row>
-    <row r="122" spans="13:14">
-      <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
-    </row>
-    <row r="123" spans="13:14">
+    <row r="122" spans="1:26">
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+    </row>
+    <row r="123" spans="1:26">
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
     </row>
-    <row r="124" spans="13:14">
-      <c r="M124" s="1"/>
-      <c r="N124" s="1"/>
-    </row>
-    <row r="125" spans="13:14">
+    <row r="124" spans="1:26">
+      <c r="M124" s="3"/>
+      <c r="N124" s="3"/>
+    </row>
+    <row r="125" spans="1:26">
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
     </row>
-    <row r="126" spans="13:14">
+    <row r="126" spans="1:26">
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
     </row>
-    <row r="127" spans="13:14">
+    <row r="127" spans="1:26">
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
     </row>
-    <row r="128" spans="13:14">
+    <row r="128" spans="1:26">
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
     </row>
@@ -4982,16 +5037,16 @@
       <c r="N130" s="1"/>
     </row>
     <row r="131" spans="13:14">
-      <c r="M131" s="3"/>
-      <c r="N131" s="3"/>
+      <c r="M131" s="1"/>
+      <c r="N131" s="1"/>
     </row>
     <row r="132" spans="13:14">
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
     </row>
     <row r="133" spans="13:14">
-      <c r="M133" s="1"/>
-      <c r="N133" s="1"/>
+      <c r="M133" s="3"/>
+      <c r="N133" s="3"/>
     </row>
     <row r="134" spans="13:14">
       <c r="M134" s="1"/>
@@ -5034,16 +5089,16 @@
       <c r="N143" s="1"/>
     </row>
     <row r="144" spans="13:14">
-      <c r="M144" s="3"/>
-      <c r="N144" s="3"/>
+      <c r="M144" s="1"/>
+      <c r="N144" s="1"/>
     </row>
     <row r="145" spans="13:14">
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
     </row>
     <row r="146" spans="13:14">
-      <c r="M146" s="1"/>
-      <c r="N146" s="1"/>
+      <c r="M146" s="3"/>
+      <c r="N146" s="3"/>
     </row>
     <row r="147" spans="13:14">
       <c r="M147" s="1"/>
@@ -5094,16 +5149,16 @@
       <c r="N158" s="1"/>
     </row>
     <row r="159" spans="13:14">
-      <c r="M159" s="3"/>
-      <c r="N159" s="3"/>
+      <c r="M159" s="1"/>
+      <c r="N159" s="1"/>
     </row>
     <row r="160" spans="13:14">
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
     </row>
     <row r="161" spans="13:14">
-      <c r="M161" s="1"/>
-      <c r="N161" s="1"/>
+      <c r="M161" s="3"/>
+      <c r="N161" s="3"/>
     </row>
     <row r="162" spans="13:14">
       <c r="M162" s="1"/>
@@ -5146,16 +5201,16 @@
       <c r="N171" s="1"/>
     </row>
     <row r="172" spans="13:14">
-      <c r="M172" s="3"/>
-      <c r="N172" s="3"/>
+      <c r="M172" s="1"/>
+      <c r="N172" s="1"/>
     </row>
     <row r="173" spans="13:14">
       <c r="M173" s="1"/>
       <c r="N173" s="1"/>
     </row>
     <row r="174" spans="13:14">
-      <c r="M174" s="1"/>
-      <c r="N174" s="1"/>
+      <c r="M174" s="3"/>
+      <c r="N174" s="3"/>
     </row>
     <row r="175" spans="13:14">
       <c r="M175" s="1"/>
@@ -5174,16 +5229,16 @@
       <c r="N178" s="1"/>
     </row>
     <row r="179" spans="13:14">
-      <c r="M179" s="3"/>
-      <c r="N179" s="3"/>
+      <c r="M179" s="1"/>
+      <c r="N179" s="1"/>
     </row>
     <row r="180" spans="13:14">
       <c r="M180" s="1"/>
       <c r="N180" s="1"/>
     </row>
     <row r="181" spans="13:14">
-      <c r="M181" s="1"/>
-      <c r="N181" s="1"/>
+      <c r="M181" s="3"/>
+      <c r="N181" s="3"/>
     </row>
     <row r="182" spans="13:14">
       <c r="M182" s="1"/>
@@ -5210,16 +5265,16 @@
       <c r="N187" s="1"/>
     </row>
     <row r="188" spans="13:14">
-      <c r="M188" s="3"/>
-      <c r="N188" s="3"/>
+      <c r="M188" s="1"/>
+      <c r="N188" s="1"/>
     </row>
     <row r="189" spans="13:14">
       <c r="M189" s="1"/>
       <c r="N189" s="1"/>
     </row>
     <row r="190" spans="13:14">
-      <c r="M190" s="1"/>
-      <c r="N190" s="1"/>
+      <c r="M190" s="3"/>
+      <c r="N190" s="3"/>
     </row>
     <row r="191" spans="13:14">
       <c r="M191" s="1"/>
@@ -5242,24 +5297,24 @@
       <c r="N195" s="1"/>
     </row>
     <row r="196" spans="13:14">
-      <c r="M196" s="3"/>
-      <c r="N196" s="3"/>
+      <c r="M196" s="1"/>
+      <c r="N196" s="1"/>
     </row>
     <row r="197" spans="13:14">
-      <c r="M197" s="3"/>
-      <c r="N197" s="3"/>
+      <c r="M197" s="1"/>
+      <c r="N197" s="1"/>
     </row>
     <row r="198" spans="13:14">
       <c r="M198" s="3"/>
       <c r="N198" s="3"/>
     </row>
     <row r="199" spans="13:14">
-      <c r="M199" s="1"/>
-      <c r="N199" s="1"/>
+      <c r="M199" s="3"/>
+      <c r="N199" s="3"/>
     </row>
     <row r="200" spans="13:14">
-      <c r="M200" s="1"/>
-      <c r="N200" s="1"/>
+      <c r="M200" s="3"/>
+      <c r="N200" s="3"/>
     </row>
     <row r="201" spans="13:14">
       <c r="M201" s="1"/>
@@ -5281,19 +5336,68 @@
       <c r="M205" s="1"/>
       <c r="N205" s="1"/>
     </row>
+    <row r="206" spans="13:14">
+      <c r="M206" s="1"/>
+      <c r="N206" s="1"/>
+    </row>
+    <row r="207" spans="13:14">
+      <c r="M207" s="1"/>
+      <c r="N207" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="C79:E80"/>
+  <mergeCells count="78">
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="C47:E48"/>
+    <mergeCell ref="C101:E102"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="C83:E84"/>
+    <mergeCell ref="C88:E89"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="C97:E98"/>
+    <mergeCell ref="C68:E69"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="C90:E91"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="C51:E52"/>
+    <mergeCell ref="V2:W5"/>
+    <mergeCell ref="X2:Y5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="T2:U5"/>
+    <mergeCell ref="R2:S5"/>
+    <mergeCell ref="B107:D108"/>
+    <mergeCell ref="C103:D104"/>
+    <mergeCell ref="C92:E93"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="C26:E27"/>
+    <mergeCell ref="C30:E31"/>
+    <mergeCell ref="C57:E58"/>
+    <mergeCell ref="C34:E35"/>
     <mergeCell ref="C53:E54"/>
-    <mergeCell ref="C74:E75"/>
-    <mergeCell ref="C70:E71"/>
-    <mergeCell ref="C64:E65"/>
-    <mergeCell ref="C62:E63"/>
-    <mergeCell ref="C60:E61"/>
-    <mergeCell ref="C68:E69"/>
-    <mergeCell ref="C72:E73"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="C32:E33"/>
+    <mergeCell ref="C39:E40"/>
+    <mergeCell ref="C45:E46"/>
+    <mergeCell ref="C49:E50"/>
+    <mergeCell ref="C41:E42"/>
+    <mergeCell ref="C99:E100"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="F2:G5"/>
+    <mergeCell ref="H2:I5"/>
+    <mergeCell ref="J2:K5"/>
+    <mergeCell ref="L2:M5"/>
+    <mergeCell ref="N2:O5"/>
+    <mergeCell ref="P2:Q5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B6:D6"/>
@@ -5308,58 +5412,18 @@
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="F2:G5"/>
-    <mergeCell ref="H2:I5"/>
-    <mergeCell ref="J2:K5"/>
-    <mergeCell ref="L2:M5"/>
-    <mergeCell ref="N2:O5"/>
-    <mergeCell ref="P2:Q5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="B105:D106"/>
-    <mergeCell ref="C101:D102"/>
-    <mergeCell ref="C90:E91"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="C26:E27"/>
-    <mergeCell ref="C30:E31"/>
+    <mergeCell ref="C43:E44"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="C81:E82"/>
     <mergeCell ref="C55:E56"/>
-    <mergeCell ref="C34:E35"/>
-    <mergeCell ref="C51:E52"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="C32:E33"/>
-    <mergeCell ref="C39:E40"/>
-    <mergeCell ref="C43:E44"/>
-    <mergeCell ref="C47:E48"/>
-    <mergeCell ref="C41:E42"/>
-    <mergeCell ref="C97:E98"/>
-    <mergeCell ref="V2:W5"/>
-    <mergeCell ref="X2:Y5"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="T2:U5"/>
-    <mergeCell ref="R2:S5"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="C45:E46"/>
-    <mergeCell ref="C99:E100"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="C81:E82"/>
-    <mergeCell ref="C86:E87"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="C95:E96"/>
+    <mergeCell ref="C76:E77"/>
+    <mergeCell ref="C72:E73"/>
     <mergeCell ref="C66:E67"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="C88:E89"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="C49:E50"/>
+    <mergeCell ref="C64:E65"/>
+    <mergeCell ref="C62:E63"/>
+    <mergeCell ref="C70:E71"/>
+    <mergeCell ref="C74:E75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Dokumentation 0.5 teilweise überarbeitet, Bild der Struktur hinzugefügt, Zeitplan aktualisiert.
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="1140" windowWidth="31380" windowHeight="19780"/>
+    <workbookView xWindow="41860" yWindow="6780" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Zeitplan erstellen</t>
   </si>
@@ -173,9 +173,6 @@
     <t>Reserve: 0.5 pro Tag</t>
   </si>
   <si>
-    <t>Situationsanalyse</t>
-  </si>
-  <si>
     <t>Zugriffskonzept</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
   </si>
   <si>
     <t>Allgemeine Anforderungen</t>
-  </si>
-  <si>
-    <t>Systemarchitektur</t>
   </si>
   <si>
     <r>
@@ -263,17 +257,6 @@
     <t>Unterbruch der IPA</t>
   </si>
   <si>
-    <t>Installationsskript erstellen als 
-Branch des Pakets "eGov buildout"</t>
-  </si>
-  <si>
-    <t>Runskript erarbeiten als Branch
- des Pakets "eGov core"</t>
-  </si>
-  <si>
-    <t>Profil definieren im Paket "eGov Core"</t>
-  </si>
-  <si>
     <t>Meilensteine</t>
   </si>
   <si>
@@ -301,12 +284,25 @@
       <t>xx</t>
     </r>
   </si>
+  <si>
+    <t>Systemstruktur</t>
+  </si>
+  <si>
+    <t>Profil definieren in einem Branch des Pakest "eGov"</t>
+  </si>
+  <si>
+    <t>Installationsskript erstellen</t>
+  </si>
+  <si>
+    <t>Runskript erarbeiten in einem Branch
+ des Pakets "teamraum-buildout"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +374,12 @@
       <color theme="1"/>
       <name val="Wingdings"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1067,7 +1069,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1278,58 +1280,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1341,15 +1297,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1362,28 +1309,103 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1404,48 +1426,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1458,52 +1438,76 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1846,13 +1850,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>231775</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>49212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1902,13 +1906,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>214313</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>301625</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>79375</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1958,13 +1962,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>261938</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>79376</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2300,10 +2304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE212"/>
+  <dimension ref="A1:AE210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="J114" sqref="J114"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -2313,7 +2317,7 @@
     <col min="3" max="3" width="26.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="4.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="5" customWidth="1"/>
-    <col min="6" max="25" width="2.6640625" style="5" customWidth="1"/>
+    <col min="6" max="25" width="3.83203125" style="5" customWidth="1"/>
     <col min="26" max="26" width="4.6640625" style="5" customWidth="1"/>
     <col min="27" max="16384" width="9.1640625" style="5"/>
   </cols>
@@ -2348,50 +2352,50 @@
     </row>
     <row r="2" spans="1:31" ht="16" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="166"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="153" t="s">
+      <c r="B2" s="160"/>
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="154"/>
-      <c r="H2" s="153" t="s">
+      <c r="G2" s="152"/>
+      <c r="H2" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="159"/>
-      <c r="J2" s="154" t="s">
+      <c r="I2" s="138"/>
+      <c r="J2" s="152" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="154"/>
-      <c r="L2" s="153" t="s">
+      <c r="K2" s="152"/>
+      <c r="L2" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="154"/>
-      <c r="N2" s="162" t="s">
+      <c r="M2" s="152"/>
+      <c r="N2" s="137" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="159"/>
-      <c r="P2" s="153" t="s">
+      <c r="O2" s="138"/>
+      <c r="P2" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="159"/>
-      <c r="R2" s="154" t="s">
+      <c r="Q2" s="138"/>
+      <c r="R2" s="152" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="154"/>
-      <c r="T2" s="153" t="s">
+      <c r="S2" s="152"/>
+      <c r="T2" s="143" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="154"/>
-      <c r="V2" s="162" t="s">
+      <c r="U2" s="152"/>
+      <c r="V2" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="159"/>
-      <c r="X2" s="153" t="s">
+      <c r="W2" s="138"/>
+      <c r="X2" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="159"/>
+      <c r="Y2" s="138"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:31" ht="14" customHeight="1">
@@ -2401,27 +2405,27 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="155"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="155"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="163"/>
-      <c r="O3" s="160"/>
-      <c r="P3" s="155"/>
-      <c r="Q3" s="160"/>
-      <c r="R3" s="156"/>
-      <c r="S3" s="156"/>
-      <c r="T3" s="155"/>
-      <c r="U3" s="156"/>
-      <c r="V3" s="163"/>
-      <c r="W3" s="160"/>
-      <c r="X3" s="155"/>
-      <c r="Y3" s="160"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="145"/>
+      <c r="K3" s="145"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="145"/>
+      <c r="N3" s="139"/>
+      <c r="O3" s="140"/>
+      <c r="P3" s="144"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="145"/>
+      <c r="S3" s="145"/>
+      <c r="T3" s="144"/>
+      <c r="U3" s="145"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="140"/>
+      <c r="X3" s="144"/>
+      <c r="Y3" s="140"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:31" ht="14" customHeight="1">
@@ -2431,143 +2435,143 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="160"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="155"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="163"/>
-      <c r="O4" s="160"/>
-      <c r="P4" s="155"/>
-      <c r="Q4" s="160"/>
-      <c r="R4" s="156"/>
-      <c r="S4" s="156"/>
-      <c r="T4" s="155"/>
-      <c r="U4" s="156"/>
-      <c r="V4" s="163"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="160"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="144"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="145"/>
+      <c r="K4" s="145"/>
+      <c r="L4" s="144"/>
+      <c r="M4" s="145"/>
+      <c r="N4" s="139"/>
+      <c r="O4" s="140"/>
+      <c r="P4" s="144"/>
+      <c r="Q4" s="140"/>
+      <c r="R4" s="145"/>
+      <c r="S4" s="145"/>
+      <c r="T4" s="144"/>
+      <c r="U4" s="145"/>
+      <c r="V4" s="139"/>
+      <c r="W4" s="140"/>
+      <c r="X4" s="144"/>
+      <c r="Y4" s="140"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:31" ht="7" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="150" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="151"/>
+      <c r="B5" s="158" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="159"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="168"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="156"/>
-      <c r="H5" s="155"/>
-      <c r="I5" s="160"/>
-      <c r="J5" s="156"/>
-      <c r="K5" s="156"/>
-      <c r="L5" s="155"/>
-      <c r="M5" s="156"/>
-      <c r="N5" s="163"/>
-      <c r="O5" s="160"/>
-      <c r="P5" s="155"/>
-      <c r="Q5" s="160"/>
-      <c r="R5" s="156"/>
-      <c r="S5" s="156"/>
-      <c r="T5" s="155"/>
-      <c r="U5" s="156"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="160"/>
-      <c r="X5" s="155"/>
-      <c r="Y5" s="156"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="144"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="140"/>
+      <c r="J5" s="145"/>
+      <c r="K5" s="145"/>
+      <c r="L5" s="144"/>
+      <c r="M5" s="145"/>
+      <c r="N5" s="139"/>
+      <c r="O5" s="140"/>
+      <c r="P5" s="144"/>
+      <c r="Q5" s="140"/>
+      <c r="R5" s="145"/>
+      <c r="S5" s="145"/>
+      <c r="T5" s="144"/>
+      <c r="U5" s="145"/>
+      <c r="V5" s="139"/>
+      <c r="W5" s="140"/>
+      <c r="X5" s="144"/>
+      <c r="Y5" s="145"/>
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:31" ht="7" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="150"/>
-      <c r="C6" s="151"/>
+      <c r="B6" s="158"/>
+      <c r="C6" s="159"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="168"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="156"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="160"/>
-      <c r="J6" s="156"/>
-      <c r="K6" s="156"/>
-      <c r="L6" s="155"/>
-      <c r="M6" s="156"/>
-      <c r="N6" s="163"/>
-      <c r="O6" s="160"/>
-      <c r="P6" s="155"/>
-      <c r="Q6" s="160"/>
-      <c r="R6" s="156"/>
-      <c r="S6" s="156"/>
-      <c r="T6" s="155"/>
-      <c r="U6" s="156"/>
-      <c r="V6" s="163"/>
-      <c r="W6" s="160"/>
-      <c r="X6" s="155"/>
-      <c r="Y6" s="156"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="144"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="145"/>
+      <c r="L6" s="144"/>
+      <c r="M6" s="145"/>
+      <c r="N6" s="139"/>
+      <c r="O6" s="140"/>
+      <c r="P6" s="144"/>
+      <c r="Q6" s="140"/>
+      <c r="R6" s="145"/>
+      <c r="S6" s="145"/>
+      <c r="T6" s="144"/>
+      <c r="U6" s="145"/>
+      <c r="V6" s="139"/>
+      <c r="W6" s="140"/>
+      <c r="X6" s="144"/>
+      <c r="Y6" s="145"/>
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:31" ht="7" customHeight="1" thickBot="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="146" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="147"/>
+      <c r="B7" s="154" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="155"/>
       <c r="D7" s="108"/>
-      <c r="E7" s="168"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="156"/>
-      <c r="H7" s="155"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="156"/>
-      <c r="K7" s="156"/>
-      <c r="L7" s="155"/>
-      <c r="M7" s="156"/>
-      <c r="N7" s="163"/>
-      <c r="O7" s="160"/>
-      <c r="P7" s="155"/>
-      <c r="Q7" s="160"/>
-      <c r="R7" s="156"/>
-      <c r="S7" s="156"/>
-      <c r="T7" s="155"/>
-      <c r="U7" s="156"/>
-      <c r="V7" s="163"/>
-      <c r="W7" s="160"/>
-      <c r="X7" s="155"/>
-      <c r="Y7" s="156"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="144"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="145"/>
+      <c r="L7" s="144"/>
+      <c r="M7" s="145"/>
+      <c r="N7" s="139"/>
+      <c r="O7" s="140"/>
+      <c r="P7" s="144"/>
+      <c r="Q7" s="140"/>
+      <c r="R7" s="145"/>
+      <c r="S7" s="145"/>
+      <c r="T7" s="144"/>
+      <c r="U7" s="145"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="140"/>
+      <c r="X7" s="144"/>
+      <c r="Y7" s="145"/>
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:31" ht="7" customHeight="1" thickTop="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="148"/>
-      <c r="C8" s="149"/>
+      <c r="B8" s="156"/>
+      <c r="C8" s="157"/>
       <c r="D8" s="107"/>
-      <c r="E8" s="169"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="158"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="161"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="158"/>
-      <c r="L8" s="157"/>
-      <c r="M8" s="158"/>
-      <c r="N8" s="164"/>
-      <c r="O8" s="161"/>
-      <c r="P8" s="157"/>
-      <c r="Q8" s="161"/>
-      <c r="R8" s="158"/>
-      <c r="S8" s="158"/>
-      <c r="T8" s="157"/>
-      <c r="U8" s="158"/>
-      <c r="V8" s="164"/>
-      <c r="W8" s="161"/>
-      <c r="X8" s="157"/>
-      <c r="Y8" s="158"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="147"/>
+      <c r="K8" s="147"/>
+      <c r="L8" s="146"/>
+      <c r="M8" s="147"/>
+      <c r="N8" s="141"/>
+      <c r="O8" s="142"/>
+      <c r="P8" s="146"/>
+      <c r="Q8" s="142"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="146"/>
+      <c r="U8" s="147"/>
+      <c r="V8" s="141"/>
+      <c r="W8" s="142"/>
+      <c r="X8" s="146"/>
+      <c r="Y8" s="147"/>
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:31" ht="10" customHeight="1">
@@ -2576,30 +2580,30 @@
         <v>13</v>
       </c>
       <c r="C9" s="81"/>
-      <c r="D9" s="138" t="s">
+      <c r="D9" s="150" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="139"/>
-      <c r="F9" s="152"/>
-      <c r="G9" s="139"/>
-      <c r="H9" s="152"/>
-      <c r="I9" s="139"/>
-      <c r="J9" s="152"/>
-      <c r="K9" s="139"/>
-      <c r="L9" s="152"/>
-      <c r="M9" s="138"/>
-      <c r="N9" s="165"/>
-      <c r="O9" s="139"/>
-      <c r="P9" s="152"/>
-      <c r="Q9" s="139"/>
-      <c r="R9" s="152"/>
-      <c r="S9" s="139"/>
-      <c r="T9" s="152"/>
-      <c r="U9" s="138"/>
-      <c r="V9" s="165"/>
-      <c r="W9" s="139"/>
-      <c r="X9" s="152"/>
-      <c r="Y9" s="139"/>
+      <c r="E9" s="149"/>
+      <c r="F9" s="148"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="149"/>
+      <c r="J9" s="148"/>
+      <c r="K9" s="149"/>
+      <c r="L9" s="148"/>
+      <c r="M9" s="150"/>
+      <c r="N9" s="151"/>
+      <c r="O9" s="149"/>
+      <c r="P9" s="148"/>
+      <c r="Q9" s="149"/>
+      <c r="R9" s="148"/>
+      <c r="S9" s="149"/>
+      <c r="T9" s="148"/>
+      <c r="U9" s="150"/>
+      <c r="V9" s="151"/>
+      <c r="W9" s="149"/>
+      <c r="X9" s="148"/>
+      <c r="Y9" s="149"/>
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:31" s="3" customFormat="1" ht="7" customHeight="1">
@@ -2628,10 +2632,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="83"/>
-      <c r="D11" s="142" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="143"/>
+      <c r="D11" s="168" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="169"/>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
       <c r="H11" s="13"/>
@@ -2657,11 +2661,11 @@
     <row r="12" spans="1:31" ht="10" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="137" t="s">
+      <c r="C12" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="129"/>
-      <c r="E12" s="130"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="116"/>
       <c r="F12" s="15"/>
       <c r="G12" s="16"/>
       <c r="H12" s="17"/>
@@ -2687,9 +2691,9 @@
     <row r="13" spans="1:31" ht="10" customHeight="1" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="135"/>
-      <c r="E13" s="136"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="119"/>
       <c r="F13" s="22"/>
       <c r="G13" s="23"/>
       <c r="H13" s="24"/>
@@ -2715,11 +2719,11 @@
     <row r="14" spans="1:31" ht="10" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="137" t="s">
+      <c r="C14" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="129"/>
-      <c r="E14" s="130"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="116"/>
       <c r="F14" s="25"/>
       <c r="G14" s="23"/>
       <c r="H14" s="24"/>
@@ -2745,9 +2749,9 @@
     <row r="15" spans="1:31" ht="10" customHeight="1" thickBot="1">
       <c r="A15" s="1"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="136"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="119"/>
       <c r="F15" s="22"/>
       <c r="G15" s="23"/>
       <c r="H15" s="24"/>
@@ -2774,11 +2778,11 @@
     <row r="16" spans="1:31" ht="10" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="137" t="s">
+      <c r="C16" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="129"/>
-      <c r="E16" s="130"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="116"/>
       <c r="F16" s="15"/>
       <c r="G16" s="23"/>
       <c r="H16" s="24"/>
@@ -2804,9 +2808,9 @@
     <row r="17" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="135"/>
-      <c r="E17" s="136"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="119"/>
       <c r="F17" s="22"/>
       <c r="G17" s="23"/>
       <c r="H17" s="24"/>
@@ -2832,11 +2836,11 @@
     <row r="18" spans="1:26" ht="10" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="128" t="s">
+      <c r="C18" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="129"/>
-      <c r="E18" s="130"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="116"/>
       <c r="F18" s="15"/>
       <c r="G18" s="23"/>
       <c r="H18" s="24"/>
@@ -2862,9 +2866,9 @@
     <row r="19" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A19" s="1"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="136"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="119"/>
       <c r="F19" s="22"/>
       <c r="G19" s="23"/>
       <c r="H19" s="24"/>
@@ -2890,11 +2894,11 @@
     <row r="20" spans="1:26" ht="10" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="137" t="s">
+      <c r="C20" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="129"/>
-      <c r="E20" s="130"/>
+      <c r="D20" s="115"/>
+      <c r="E20" s="116"/>
       <c r="F20" s="25"/>
       <c r="G20" s="23"/>
       <c r="H20" s="24"/>
@@ -2920,9 +2924,9 @@
     <row r="21" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A21" s="1"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="136"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="22"/>
       <c r="G21" s="26"/>
       <c r="H21" s="24"/>
@@ -2948,11 +2952,11 @@
     <row r="22" spans="1:26" ht="10" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="137" t="s">
+      <c r="C22" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="116"/>
       <c r="F22" s="27"/>
       <c r="G22" s="28"/>
       <c r="H22" s="24"/>
@@ -2978,9 +2982,9 @@
     <row r="23" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A23" s="1"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="134"/>
-      <c r="D23" s="135"/>
-      <c r="E23" s="136"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="119"/>
       <c r="F23" s="27"/>
       <c r="G23" s="26"/>
       <c r="H23" s="24"/>
@@ -3006,11 +3010,11 @@
     <row r="24" spans="1:26" ht="10" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="128" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="129"/>
-      <c r="E24" s="130"/>
+      <c r="C24" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="115"/>
+      <c r="E24" s="116"/>
       <c r="F24" s="17"/>
       <c r="G24" s="29"/>
       <c r="H24" s="24"/>
@@ -3036,9 +3040,9 @@
     <row r="25" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A25" s="1"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="135"/>
-      <c r="E25" s="136"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="119"/>
       <c r="F25" s="27"/>
       <c r="G25" s="30"/>
       <c r="H25" s="24"/>
@@ -3065,8 +3069,8 @@
       <c r="A26" s="1"/>
       <c r="B26" s="78"/>
       <c r="C26" s="79"/>
-      <c r="D26" s="140"/>
-      <c r="E26" s="141"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="167"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
       <c r="H26" s="13"/>
@@ -3114,10 +3118,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="85"/>
-      <c r="D28" s="144" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="145"/>
+      <c r="D28" s="164" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="165"/>
       <c r="F28" s="33"/>
       <c r="G28" s="34"/>
       <c r="H28" s="33"/>
@@ -3143,11 +3147,11 @@
     <row r="29" spans="1:26" ht="10" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="36"/>
-      <c r="C29" s="137" t="s">
+      <c r="C29" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="129"/>
-      <c r="E29" s="130"/>
+      <c r="D29" s="115"/>
+      <c r="E29" s="116"/>
       <c r="F29" s="37"/>
       <c r="G29" s="38"/>
       <c r="H29" s="39"/>
@@ -3173,9 +3177,9 @@
     <row r="30" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A30" s="1"/>
       <c r="B30" s="36"/>
-      <c r="C30" s="134"/>
-      <c r="D30" s="135"/>
-      <c r="E30" s="136"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="119"/>
       <c r="F30" s="44"/>
       <c r="G30" s="30"/>
       <c r="H30" s="45"/>
@@ -3201,11 +3205,11 @@
     <row r="31" spans="1:26" ht="10" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="36"/>
-      <c r="C31" s="128" t="s">
+      <c r="C31" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="129"/>
-      <c r="E31" s="130"/>
+      <c r="D31" s="115"/>
+      <c r="E31" s="116"/>
       <c r="F31" s="44"/>
       <c r="G31" s="46"/>
       <c r="H31" s="39"/>
@@ -3231,9 +3235,9 @@
     <row r="32" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A32" s="1"/>
       <c r="B32" s="36"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="135"/>
-      <c r="E32" s="136"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="119"/>
       <c r="F32" s="44"/>
       <c r="G32" s="46"/>
       <c r="H32" s="45"/>
@@ -3259,11 +3263,11 @@
     <row r="33" spans="1:26" ht="10" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="36"/>
-      <c r="C33" s="137" t="s">
+      <c r="C33" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="129"/>
-      <c r="E33" s="130"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="116"/>
       <c r="F33" s="43"/>
       <c r="G33" s="16"/>
       <c r="H33" s="39"/>
@@ -3289,9 +3293,9 @@
     <row r="34" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A34" s="1"/>
       <c r="B34" s="36"/>
-      <c r="C34" s="134"/>
-      <c r="D34" s="135"/>
-      <c r="E34" s="136"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="119"/>
       <c r="F34" s="43"/>
       <c r="G34" s="46"/>
       <c r="H34" s="45"/>
@@ -3317,11 +3321,11 @@
     <row r="35" spans="1:26" ht="10" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="36"/>
-      <c r="C35" s="128" t="s">
+      <c r="C35" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="129"/>
-      <c r="E35" s="130"/>
+      <c r="D35" s="115"/>
+      <c r="E35" s="116"/>
       <c r="F35" s="43"/>
       <c r="G35" s="16"/>
       <c r="H35" s="17"/>
@@ -3347,9 +3351,9 @@
     <row r="36" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A36" s="1"/>
       <c r="B36" s="36"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="135"/>
-      <c r="E36" s="136"/>
+      <c r="C36" s="117"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="119"/>
       <c r="F36" s="43"/>
       <c r="G36" s="46"/>
       <c r="H36" s="27"/>
@@ -3375,11 +3379,11 @@
     <row r="37" spans="1:26" ht="10" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="36"/>
-      <c r="C37" s="137" t="s">
+      <c r="C37" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="129"/>
-      <c r="E37" s="130"/>
+      <c r="D37" s="115"/>
+      <c r="E37" s="116"/>
       <c r="F37" s="43"/>
       <c r="G37" s="50"/>
       <c r="H37" s="17"/>
@@ -3405,9 +3409,9 @@
     <row r="38" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A38" s="1"/>
       <c r="B38" s="36"/>
-      <c r="C38" s="134"/>
-      <c r="D38" s="135"/>
-      <c r="E38" s="136"/>
+      <c r="C38" s="117"/>
+      <c r="D38" s="118"/>
+      <c r="E38" s="119"/>
       <c r="F38" s="43"/>
       <c r="G38" s="51"/>
       <c r="H38" s="27"/>
@@ -3432,10 +3436,10 @@
     </row>
     <row r="39" spans="1:26" ht="10" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="115"/>
-      <c r="C39" s="116"/>
-      <c r="D39" s="116"/>
-      <c r="E39" s="117"/>
+      <c r="B39" s="172"/>
+      <c r="C39" s="173"/>
+      <c r="D39" s="173"/>
+      <c r="E39" s="174"/>
       <c r="F39" s="33"/>
       <c r="G39" s="34"/>
       <c r="H39" s="33"/>
@@ -3483,10 +3487,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="87"/>
-      <c r="D41" s="118">
+      <c r="D41" s="175">
         <v>12</v>
       </c>
-      <c r="E41" s="119"/>
+      <c r="E41" s="176"/>
       <c r="F41" s="52"/>
       <c r="G41" s="53"/>
       <c r="H41" s="52"/>
@@ -3512,11 +3516,11 @@
     <row r="42" spans="1:26" ht="10" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="55"/>
-      <c r="C42" s="137" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="129"/>
-      <c r="E42" s="130"/>
+      <c r="C42" s="120" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="115"/>
+      <c r="E42" s="116"/>
       <c r="F42" s="43"/>
       <c r="G42" s="56"/>
       <c r="H42" s="43"/>
@@ -3542,9 +3546,9 @@
     <row r="43" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A43" s="1"/>
       <c r="B43" s="55"/>
-      <c r="C43" s="134"/>
-      <c r="D43" s="135"/>
-      <c r="E43" s="136"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="118"/>
+      <c r="E43" s="119"/>
       <c r="F43" s="43"/>
       <c r="G43" s="56"/>
       <c r="H43" s="43"/>
@@ -3570,11 +3574,11 @@
     <row r="44" spans="1:26" ht="10" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="55"/>
-      <c r="C44" s="137" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" s="129"/>
-      <c r="E44" s="130"/>
+      <c r="C44" s="120" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="115"/>
+      <c r="E44" s="116"/>
       <c r="F44" s="43"/>
       <c r="G44" s="56"/>
       <c r="H44" s="43"/>
@@ -3600,9 +3604,9 @@
     <row r="45" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A45" s="1"/>
       <c r="B45" s="55"/>
-      <c r="C45" s="134"/>
-      <c r="D45" s="135"/>
-      <c r="E45" s="136"/>
+      <c r="C45" s="117"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="119"/>
       <c r="F45" s="43"/>
       <c r="G45" s="56"/>
       <c r="H45" s="43"/>
@@ -3628,17 +3632,17 @@
     <row r="46" spans="1:26" ht="10" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="55"/>
-      <c r="C46" s="137" t="s">
-        <v>57</v>
-      </c>
-      <c r="D46" s="129"/>
-      <c r="E46" s="130"/>
+      <c r="C46" s="120" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="115"/>
+      <c r="E46" s="116"/>
       <c r="F46" s="43"/>
       <c r="G46" s="56"/>
       <c r="H46" s="43"/>
       <c r="I46" s="40"/>
       <c r="J46" s="57"/>
-      <c r="K46" s="42"/>
+      <c r="K46" s="66"/>
       <c r="L46" s="43"/>
       <c r="M46" s="42"/>
       <c r="N46" s="100"/>
@@ -3658,16 +3662,16 @@
     <row r="47" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A47" s="1"/>
       <c r="B47" s="55"/>
-      <c r="C47" s="134"/>
-      <c r="D47" s="135"/>
-      <c r="E47" s="136"/>
+      <c r="C47" s="117"/>
+      <c r="D47" s="118"/>
+      <c r="E47" s="119"/>
       <c r="F47" s="43"/>
       <c r="G47" s="56"/>
       <c r="H47" s="43"/>
       <c r="I47" s="40"/>
-      <c r="J47" s="76"/>
-      <c r="K47" s="42"/>
-      <c r="L47" s="43"/>
+      <c r="J47" s="65"/>
+      <c r="K47" s="77"/>
+      <c r="L47" s="45"/>
       <c r="M47" s="42"/>
       <c r="N47" s="100"/>
       <c r="O47" s="40"/>
@@ -3686,17 +3690,17 @@
     <row r="48" spans="1:26" ht="10" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="55"/>
-      <c r="C48" s="137" t="s">
+      <c r="C48" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="129"/>
-      <c r="E48" s="130"/>
+      <c r="D48" s="115"/>
+      <c r="E48" s="116"/>
       <c r="F48" s="43"/>
       <c r="G48" s="56"/>
       <c r="H48" s="43"/>
       <c r="I48" s="40"/>
-      <c r="J48" s="57"/>
-      <c r="K48" s="66"/>
+      <c r="J48" s="41"/>
+      <c r="K48" s="58"/>
       <c r="L48" s="43"/>
       <c r="M48" s="42"/>
       <c r="N48" s="100"/>
@@ -3716,16 +3720,16 @@
     <row r="49" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A49" s="1"/>
       <c r="B49" s="55"/>
-      <c r="C49" s="134"/>
-      <c r="D49" s="135"/>
-      <c r="E49" s="136"/>
+      <c r="C49" s="117"/>
+      <c r="D49" s="118"/>
+      <c r="E49" s="119"/>
       <c r="F49" s="43"/>
       <c r="G49" s="56"/>
       <c r="H49" s="43"/>
       <c r="I49" s="40"/>
-      <c r="J49" s="65"/>
-      <c r="K49" s="77"/>
-      <c r="L49" s="43"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="66"/>
+      <c r="L49" s="47"/>
       <c r="M49" s="42"/>
       <c r="N49" s="100"/>
       <c r="O49" s="40"/>
@@ -3744,18 +3748,18 @@
     <row r="50" spans="1:26" ht="10" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="55"/>
-      <c r="C50" s="137" t="s">
+      <c r="C50" s="120" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="129"/>
-      <c r="E50" s="130"/>
+      <c r="D50" s="115"/>
+      <c r="E50" s="116"/>
       <c r="F50" s="43"/>
       <c r="G50" s="56"/>
       <c r="H50" s="43"/>
       <c r="I50" s="40"/>
       <c r="J50" s="41"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="43"/>
+      <c r="K50" s="74"/>
+      <c r="L50" s="39"/>
       <c r="M50" s="42"/>
       <c r="N50" s="100"/>
       <c r="O50" s="40"/>
@@ -3774,14 +3778,14 @@
     <row r="51" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A51" s="1"/>
       <c r="B51" s="55"/>
-      <c r="C51" s="134"/>
-      <c r="D51" s="135"/>
-      <c r="E51" s="136"/>
+      <c r="C51" s="117"/>
+      <c r="D51" s="118"/>
+      <c r="E51" s="119"/>
       <c r="F51" s="43"/>
       <c r="G51" s="56"/>
       <c r="H51" s="43"/>
       <c r="I51" s="40"/>
-      <c r="J51" s="76"/>
+      <c r="J51" s="41"/>
       <c r="K51" s="66"/>
       <c r="L51" s="45"/>
       <c r="M51" s="42"/>
@@ -3802,19 +3806,19 @@
     <row r="52" spans="1:26" ht="10" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="55"/>
-      <c r="C52" s="137" t="s">
+      <c r="C52" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="129"/>
-      <c r="E52" s="130"/>
+      <c r="D52" s="115"/>
+      <c r="E52" s="116"/>
       <c r="F52" s="43"/>
       <c r="G52" s="56"/>
       <c r="H52" s="43"/>
       <c r="I52" s="40"/>
       <c r="J52" s="41"/>
-      <c r="K52" s="74"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="42"/>
+      <c r="K52" s="66"/>
+      <c r="L52" s="47"/>
+      <c r="M52" s="58"/>
       <c r="N52" s="100"/>
       <c r="O52" s="40"/>
       <c r="P52" s="43"/>
@@ -3832,17 +3836,17 @@
     <row r="53" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A53" s="1"/>
       <c r="B53" s="55"/>
-      <c r="C53" s="134"/>
-      <c r="D53" s="135"/>
-      <c r="E53" s="136"/>
+      <c r="C53" s="117"/>
+      <c r="D53" s="118"/>
+      <c r="E53" s="119"/>
       <c r="F53" s="43"/>
       <c r="G53" s="56"/>
       <c r="H53" s="43"/>
       <c r="I53" s="40"/>
       <c r="J53" s="41"/>
       <c r="K53" s="66"/>
-      <c r="L53" s="45"/>
-      <c r="M53" s="42"/>
+      <c r="L53" s="43"/>
+      <c r="M53" s="77"/>
       <c r="N53" s="100"/>
       <c r="O53" s="40"/>
       <c r="P53" s="43"/>
@@ -3860,20 +3864,20 @@
     <row r="54" spans="1:26" ht="10" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="55"/>
-      <c r="C54" s="137" t="s">
-        <v>53</v>
-      </c>
-      <c r="D54" s="129"/>
-      <c r="E54" s="130"/>
+      <c r="C54" s="120" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="115"/>
+      <c r="E54" s="116"/>
       <c r="F54" s="43"/>
       <c r="G54" s="56"/>
       <c r="H54" s="43"/>
       <c r="I54" s="40"/>
       <c r="J54" s="41"/>
-      <c r="K54" s="66"/>
+      <c r="K54" s="42"/>
       <c r="L54" s="47"/>
       <c r="M54" s="58"/>
-      <c r="N54" s="100"/>
+      <c r="N54" s="102"/>
       <c r="O54" s="40"/>
       <c r="P54" s="43"/>
       <c r="Q54" s="40"/>
@@ -3890,18 +3894,18 @@
     <row r="55" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A55" s="1"/>
       <c r="B55" s="55"/>
-      <c r="C55" s="134"/>
-      <c r="D55" s="135"/>
-      <c r="E55" s="136"/>
+      <c r="C55" s="117"/>
+      <c r="D55" s="118"/>
+      <c r="E55" s="119"/>
       <c r="F55" s="43"/>
       <c r="G55" s="56"/>
       <c r="H55" s="43"/>
       <c r="I55" s="40"/>
       <c r="J55" s="41"/>
-      <c r="K55" s="66"/>
+      <c r="K55" s="42"/>
       <c r="L55" s="43"/>
-      <c r="M55" s="77"/>
-      <c r="N55" s="100"/>
+      <c r="M55" s="94"/>
+      <c r="N55" s="102"/>
       <c r="O55" s="40"/>
       <c r="P55" s="43"/>
       <c r="Q55" s="40"/>
@@ -3918,11 +3922,11 @@
     <row r="56" spans="1:26" ht="10" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="55"/>
-      <c r="C56" s="137" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" s="129"/>
-      <c r="E56" s="130"/>
+      <c r="C56" s="120" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="115"/>
+      <c r="E56" s="116"/>
       <c r="F56" s="43"/>
       <c r="G56" s="56"/>
       <c r="H56" s="43"/>
@@ -3930,8 +3934,8 @@
       <c r="J56" s="41"/>
       <c r="K56" s="42"/>
       <c r="L56" s="47"/>
-      <c r="M56" s="58"/>
-      <c r="N56" s="102"/>
+      <c r="M56" s="66"/>
+      <c r="N56" s="103"/>
       <c r="O56" s="40"/>
       <c r="P56" s="43"/>
       <c r="Q56" s="40"/>
@@ -3948,9 +3952,9 @@
     <row r="57" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A57" s="1"/>
       <c r="B57" s="55"/>
-      <c r="C57" s="134"/>
-      <c r="D57" s="135"/>
-      <c r="E57" s="136"/>
+      <c r="C57" s="117"/>
+      <c r="D57" s="118"/>
+      <c r="E57" s="119"/>
       <c r="F57" s="43"/>
       <c r="G57" s="56"/>
       <c r="H57" s="43"/>
@@ -3958,8 +3962,8 @@
       <c r="J57" s="41"/>
       <c r="K57" s="42"/>
       <c r="L57" s="43"/>
-      <c r="M57" s="94"/>
-      <c r="N57" s="102"/>
+      <c r="M57" s="66"/>
+      <c r="N57" s="110"/>
       <c r="O57" s="40"/>
       <c r="P57" s="43"/>
       <c r="Q57" s="40"/>
@@ -3976,20 +3980,20 @@
     <row r="58" spans="1:26" ht="10" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="55"/>
-      <c r="C58" s="137" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="129"/>
-      <c r="E58" s="130"/>
+      <c r="C58" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="D58" s="115"/>
+      <c r="E58" s="116"/>
       <c r="F58" s="43"/>
       <c r="G58" s="56"/>
       <c r="H58" s="43"/>
       <c r="I58" s="40"/>
       <c r="J58" s="41"/>
-      <c r="K58" s="42"/>
-      <c r="L58" s="47"/>
-      <c r="M58" s="66"/>
-      <c r="N58" s="103"/>
+      <c r="K58" s="58"/>
+      <c r="L58" s="43"/>
+      <c r="M58" s="42"/>
+      <c r="N58" s="100"/>
       <c r="O58" s="40"/>
       <c r="P58" s="43"/>
       <c r="Q58" s="40"/>
@@ -4006,18 +4010,18 @@
     <row r="59" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A59" s="1"/>
       <c r="B59" s="55"/>
-      <c r="C59" s="134"/>
-      <c r="D59" s="135"/>
-      <c r="E59" s="136"/>
+      <c r="C59" s="117"/>
+      <c r="D59" s="118"/>
+      <c r="E59" s="119"/>
       <c r="F59" s="43"/>
       <c r="G59" s="56"/>
       <c r="H59" s="43"/>
       <c r="I59" s="40"/>
       <c r="J59" s="41"/>
-      <c r="K59" s="42"/>
+      <c r="K59" s="77"/>
       <c r="L59" s="43"/>
-      <c r="M59" s="66"/>
-      <c r="N59" s="102"/>
+      <c r="M59" s="42"/>
+      <c r="N59" s="100"/>
       <c r="O59" s="40"/>
       <c r="P59" s="43"/>
       <c r="Q59" s="40"/>
@@ -4033,149 +4037,149 @@
     </row>
     <row r="60" spans="1:26" ht="10" customHeight="1">
       <c r="A60" s="1"/>
-      <c r="B60" s="55"/>
-      <c r="C60" s="137" t="s">
-        <v>45</v>
-      </c>
-      <c r="D60" s="129"/>
-      <c r="E60" s="130"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="43"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="58"/>
-      <c r="L60" s="43"/>
-      <c r="M60" s="42"/>
-      <c r="N60" s="100"/>
-      <c r="O60" s="40"/>
-      <c r="P60" s="43"/>
-      <c r="Q60" s="40"/>
-      <c r="R60" s="41"/>
-      <c r="S60" s="42"/>
-      <c r="T60" s="43"/>
-      <c r="U60" s="42"/>
-      <c r="V60" s="100"/>
-      <c r="W60" s="40"/>
-      <c r="X60" s="43"/>
-      <c r="Y60" s="40"/>
+      <c r="B60" s="177"/>
+      <c r="C60" s="178"/>
+      <c r="D60" s="178"/>
+      <c r="E60" s="179"/>
+      <c r="F60" s="52"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="54"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="54"/>
+      <c r="L60" s="52"/>
+      <c r="M60" s="53"/>
+      <c r="N60" s="101"/>
+      <c r="O60" s="54"/>
+      <c r="P60" s="52"/>
+      <c r="Q60" s="54"/>
+      <c r="R60" s="52"/>
+      <c r="S60" s="54"/>
+      <c r="T60" s="52"/>
+      <c r="U60" s="53"/>
+      <c r="V60" s="101"/>
+      <c r="W60" s="54"/>
+      <c r="X60" s="52"/>
+      <c r="Y60" s="54"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="61" spans="1:26" ht="10" customHeight="1" thickBot="1">
-      <c r="A61" s="1"/>
-      <c r="B61" s="55"/>
-      <c r="C61" s="134"/>
-      <c r="D61" s="135"/>
-      <c r="E61" s="136"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="40"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="77"/>
-      <c r="L61" s="43"/>
-      <c r="M61" s="42"/>
-      <c r="N61" s="100"/>
-      <c r="O61" s="40"/>
-      <c r="P61" s="43"/>
-      <c r="Q61" s="40"/>
-      <c r="R61" s="41"/>
-      <c r="S61" s="42"/>
-      <c r="T61" s="43"/>
-      <c r="U61" s="42"/>
-      <c r="V61" s="100"/>
-      <c r="W61" s="40"/>
-      <c r="X61" s="43"/>
-      <c r="Y61" s="40"/>
-      <c r="Z61" s="1"/>
-    </row>
-    <row r="62" spans="1:26" ht="10" customHeight="1">
+    <row r="61" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="4"/>
+      <c r="L61" s="2"/>
+      <c r="N61" s="96"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="4"/>
+      <c r="T61" s="2"/>
+      <c r="V61" s="96"/>
+      <c r="W61" s="4"/>
+      <c r="X61" s="2"/>
+      <c r="Y61" s="4"/>
+    </row>
+    <row r="62" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A62" s="1"/>
-      <c r="B62" s="120"/>
-      <c r="C62" s="121"/>
-      <c r="D62" s="121"/>
-      <c r="E62" s="122"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="53"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="54"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="54"/>
-      <c r="L62" s="52"/>
-      <c r="M62" s="53"/>
-      <c r="N62" s="101"/>
-      <c r="O62" s="54"/>
-      <c r="P62" s="52"/>
-      <c r="Q62" s="54"/>
-      <c r="R62" s="52"/>
-      <c r="S62" s="54"/>
-      <c r="T62" s="52"/>
-      <c r="U62" s="53"/>
-      <c r="V62" s="101"/>
-      <c r="W62" s="54"/>
-      <c r="X62" s="52"/>
-      <c r="Y62" s="54"/>
-      <c r="Z62" s="1"/>
-    </row>
-    <row r="63" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="4"/>
-      <c r="L63" s="2"/>
-      <c r="N63" s="96"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="4"/>
-      <c r="T63" s="2"/>
-      <c r="V63" s="96"/>
-      <c r="W63" s="4"/>
-      <c r="X63" s="2"/>
-      <c r="Y63" s="4"/>
+      <c r="B62" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="89"/>
+      <c r="D62" s="180">
+        <v>28</v>
+      </c>
+      <c r="E62" s="181"/>
+      <c r="F62" s="69"/>
+      <c r="G62" s="70"/>
+      <c r="H62" s="69"/>
+      <c r="I62" s="71"/>
+      <c r="J62" s="69"/>
+      <c r="K62" s="71"/>
+      <c r="L62" s="69"/>
+      <c r="M62" s="70"/>
+      <c r="N62" s="104"/>
+      <c r="O62" s="71"/>
+      <c r="P62" s="69"/>
+      <c r="Q62" s="71"/>
+      <c r="R62" s="69"/>
+      <c r="S62" s="71"/>
+      <c r="T62" s="69"/>
+      <c r="U62" s="70"/>
+      <c r="V62" s="104"/>
+      <c r="W62" s="71"/>
+      <c r="X62" s="69"/>
+      <c r="Y62" s="70"/>
+      <c r="Z62" s="2"/>
+    </row>
+    <row r="63" spans="1:26" ht="10" customHeight="1">
+      <c r="A63" s="1"/>
+      <c r="B63" s="72"/>
+      <c r="C63" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" s="115"/>
+      <c r="E63" s="116"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="40"/>
+      <c r="J63" s="41"/>
+      <c r="K63" s="42"/>
+      <c r="L63" s="43"/>
+      <c r="M63" s="66"/>
+      <c r="N63" s="111"/>
+      <c r="O63" s="48"/>
+      <c r="P63" s="43"/>
+      <c r="Q63" s="40"/>
+      <c r="R63" s="41"/>
+      <c r="S63" s="42"/>
+      <c r="T63" s="43"/>
+      <c r="U63" s="42"/>
+      <c r="V63" s="100"/>
+      <c r="W63" s="40"/>
+      <c r="X63" s="43"/>
+      <c r="Y63" s="40"/>
+      <c r="Z63" s="1"/>
     </row>
     <row r="64" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A64" s="1"/>
-      <c r="B64" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="89"/>
-      <c r="D64" s="123">
-        <v>28</v>
-      </c>
-      <c r="E64" s="124"/>
-      <c r="F64" s="69"/>
-      <c r="G64" s="70"/>
-      <c r="H64" s="69"/>
-      <c r="I64" s="71"/>
-      <c r="J64" s="69"/>
-      <c r="K64" s="71"/>
-      <c r="L64" s="69"/>
-      <c r="M64" s="70"/>
-      <c r="N64" s="104"/>
-      <c r="O64" s="71"/>
-      <c r="P64" s="69"/>
-      <c r="Q64" s="71"/>
-      <c r="R64" s="69"/>
-      <c r="S64" s="71"/>
-      <c r="T64" s="69"/>
-      <c r="U64" s="70"/>
-      <c r="V64" s="104"/>
-      <c r="W64" s="71"/>
-      <c r="X64" s="69"/>
-      <c r="Y64" s="70"/>
-      <c r="Z64" s="2"/>
+      <c r="B64" s="72"/>
+      <c r="C64" s="117"/>
+      <c r="D64" s="118"/>
+      <c r="E64" s="119"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="56"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="40"/>
+      <c r="J64" s="41"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="43"/>
+      <c r="M64" s="42"/>
+      <c r="N64" s="110"/>
+      <c r="O64" s="40"/>
+      <c r="P64" s="43"/>
+      <c r="Q64" s="40"/>
+      <c r="R64" s="41"/>
+      <c r="S64" s="42"/>
+      <c r="T64" s="43"/>
+      <c r="U64" s="42"/>
+      <c r="V64" s="100"/>
+      <c r="W64" s="40"/>
+      <c r="X64" s="43"/>
+      <c r="Y64" s="40"/>
+      <c r="Z64" s="1"/>
     </row>
     <row r="65" spans="1:26" ht="10" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="72"/>
-      <c r="C65" s="137" t="s">
-        <v>38</v>
-      </c>
-      <c r="D65" s="129"/>
-      <c r="E65" s="130"/>
+      <c r="C65" s="120" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" s="115"/>
+      <c r="E65" s="116"/>
       <c r="F65" s="43"/>
       <c r="G65" s="56"/>
       <c r="H65" s="43"/>
@@ -4201,9 +4205,9 @@
     <row r="66" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A66" s="1"/>
       <c r="B66" s="72"/>
-      <c r="C66" s="134"/>
-      <c r="D66" s="135"/>
-      <c r="E66" s="136"/>
+      <c r="C66" s="117"/>
+      <c r="D66" s="118"/>
+      <c r="E66" s="119"/>
       <c r="F66" s="43"/>
       <c r="G66" s="56"/>
       <c r="H66" s="43"/>
@@ -4212,8 +4216,8 @@
       <c r="K66" s="42"/>
       <c r="L66" s="43"/>
       <c r="M66" s="42"/>
-      <c r="N66" s="100"/>
-      <c r="O66" s="40"/>
+      <c r="N66" s="110"/>
+      <c r="O66" s="67"/>
       <c r="P66" s="43"/>
       <c r="Q66" s="40"/>
       <c r="R66" s="41"/>
@@ -4229,11 +4233,11 @@
     <row r="67" spans="1:26" ht="10" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="72"/>
-      <c r="C67" s="137" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" s="129"/>
-      <c r="E67" s="130"/>
+      <c r="C67" s="114" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" s="115"/>
+      <c r="E67" s="116"/>
       <c r="F67" s="43"/>
       <c r="G67" s="56"/>
       <c r="H67" s="43"/>
@@ -4241,11 +4245,11 @@
       <c r="J67" s="41"/>
       <c r="K67" s="42"/>
       <c r="L67" s="43"/>
-      <c r="M67" s="66"/>
-      <c r="N67" s="102"/>
+      <c r="M67" s="42"/>
+      <c r="N67" s="100"/>
       <c r="O67" s="48"/>
-      <c r="P67" s="43"/>
-      <c r="Q67" s="40"/>
+      <c r="P67" s="39"/>
+      <c r="Q67" s="48"/>
       <c r="R67" s="41"/>
       <c r="S67" s="42"/>
       <c r="T67" s="43"/>
@@ -4259,9 +4263,9 @@
     <row r="68" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A68" s="1"/>
       <c r="B68" s="72"/>
-      <c r="C68" s="134"/>
-      <c r="D68" s="135"/>
-      <c r="E68" s="136"/>
+      <c r="C68" s="185"/>
+      <c r="D68" s="186"/>
+      <c r="E68" s="187"/>
       <c r="F68" s="43"/>
       <c r="G68" s="56"/>
       <c r="H68" s="43"/>
@@ -4270,8 +4274,8 @@
       <c r="K68" s="42"/>
       <c r="L68" s="43"/>
       <c r="M68" s="42"/>
-      <c r="N68" s="100"/>
-      <c r="O68" s="40"/>
+      <c r="N68" s="102"/>
+      <c r="O68" s="67"/>
       <c r="P68" s="43"/>
       <c r="Q68" s="40"/>
       <c r="R68" s="41"/>
@@ -4287,11 +4291,11 @@
     <row r="69" spans="1:26" ht="10" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="72"/>
-      <c r="C69" s="128" t="s">
-        <v>61</v>
-      </c>
-      <c r="D69" s="129"/>
-      <c r="E69" s="130"/>
+      <c r="C69" s="114" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" s="115"/>
+      <c r="E69" s="116"/>
       <c r="F69" s="43"/>
       <c r="G69" s="56"/>
       <c r="H69" s="43"/>
@@ -4301,10 +4305,10 @@
       <c r="L69" s="43"/>
       <c r="M69" s="42"/>
       <c r="N69" s="100"/>
-      <c r="O69" s="48"/>
-      <c r="P69" s="39"/>
-      <c r="Q69" s="48"/>
-      <c r="R69" s="41"/>
+      <c r="O69" s="40"/>
+      <c r="P69" s="43"/>
+      <c r="Q69" s="40"/>
+      <c r="R69" s="57"/>
       <c r="S69" s="42"/>
       <c r="T69" s="43"/>
       <c r="U69" s="42"/>
@@ -4317,9 +4321,9 @@
     <row r="70" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A70" s="1"/>
       <c r="B70" s="72"/>
-      <c r="C70" s="131"/>
-      <c r="D70" s="132"/>
-      <c r="E70" s="133"/>
+      <c r="C70" s="117"/>
+      <c r="D70" s="118"/>
+      <c r="E70" s="119"/>
       <c r="F70" s="43"/>
       <c r="G70" s="56"/>
       <c r="H70" s="43"/>
@@ -4345,11 +4349,11 @@
     <row r="71" spans="1:26" ht="10" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="72"/>
-      <c r="C71" s="128" t="s">
-        <v>63</v>
-      </c>
-      <c r="D71" s="129"/>
-      <c r="E71" s="130"/>
+      <c r="C71" s="114" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="115"/>
+      <c r="E71" s="116"/>
       <c r="F71" s="43"/>
       <c r="G71" s="56"/>
       <c r="H71" s="43"/>
@@ -4358,12 +4362,12 @@
       <c r="K71" s="42"/>
       <c r="L71" s="43"/>
       <c r="M71" s="42"/>
-      <c r="N71" s="100"/>
-      <c r="O71" s="40"/>
-      <c r="P71" s="43"/>
-      <c r="Q71" s="40"/>
+      <c r="N71" s="102"/>
+      <c r="O71" s="67"/>
+      <c r="P71" s="47"/>
+      <c r="Q71" s="67"/>
       <c r="R71" s="57"/>
-      <c r="S71" s="42"/>
+      <c r="S71" s="58"/>
       <c r="T71" s="43"/>
       <c r="U71" s="42"/>
       <c r="V71" s="100"/>
@@ -4375,9 +4379,9 @@
     <row r="72" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A72" s="1"/>
       <c r="B72" s="72"/>
-      <c r="C72" s="134"/>
-      <c r="D72" s="135"/>
-      <c r="E72" s="136"/>
+      <c r="C72" s="117"/>
+      <c r="D72" s="118"/>
+      <c r="E72" s="119"/>
       <c r="F72" s="43"/>
       <c r="G72" s="56"/>
       <c r="H72" s="43"/>
@@ -4403,11 +4407,11 @@
     <row r="73" spans="1:26" ht="10" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="72"/>
-      <c r="C73" s="128" t="s">
-        <v>62</v>
-      </c>
-      <c r="D73" s="129"/>
-      <c r="E73" s="130"/>
+      <c r="C73" s="120" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="115"/>
+      <c r="E73" s="116"/>
       <c r="F73" s="43"/>
       <c r="G73" s="56"/>
       <c r="H73" s="43"/>
@@ -4416,11 +4420,11 @@
       <c r="K73" s="42"/>
       <c r="L73" s="43"/>
       <c r="M73" s="42"/>
-      <c r="N73" s="102"/>
-      <c r="O73" s="67"/>
-      <c r="P73" s="47"/>
-      <c r="Q73" s="67"/>
-      <c r="R73" s="57"/>
+      <c r="N73" s="100"/>
+      <c r="O73" s="40"/>
+      <c r="P73" s="43"/>
+      <c r="Q73" s="40"/>
+      <c r="R73" s="41"/>
       <c r="S73" s="58"/>
       <c r="T73" s="43"/>
       <c r="U73" s="42"/>
@@ -4433,9 +4437,9 @@
     <row r="74" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A74" s="1"/>
       <c r="B74" s="72"/>
-      <c r="C74" s="134"/>
-      <c r="D74" s="135"/>
-      <c r="E74" s="136"/>
+      <c r="C74" s="117"/>
+      <c r="D74" s="118"/>
+      <c r="E74" s="119"/>
       <c r="F74" s="43"/>
       <c r="G74" s="56"/>
       <c r="H74" s="43"/>
@@ -4461,11 +4465,11 @@
     <row r="75" spans="1:26" ht="10" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="72"/>
-      <c r="C75" s="137" t="s">
-        <v>40</v>
-      </c>
-      <c r="D75" s="129"/>
-      <c r="E75" s="130"/>
+      <c r="C75" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="D75" s="115"/>
+      <c r="E75" s="116"/>
       <c r="F75" s="43"/>
       <c r="G75" s="56"/>
       <c r="H75" s="43"/>
@@ -4479,8 +4483,8 @@
       <c r="P75" s="43"/>
       <c r="Q75" s="40"/>
       <c r="R75" s="41"/>
-      <c r="S75" s="58"/>
-      <c r="T75" s="43"/>
+      <c r="S75" s="42"/>
+      <c r="T75" s="39"/>
       <c r="U75" s="42"/>
       <c r="V75" s="100"/>
       <c r="W75" s="40"/>
@@ -4491,9 +4495,9 @@
     <row r="76" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A76" s="1"/>
       <c r="B76" s="72"/>
-      <c r="C76" s="134"/>
-      <c r="D76" s="135"/>
-      <c r="E76" s="136"/>
+      <c r="C76" s="117"/>
+      <c r="D76" s="118"/>
+      <c r="E76" s="119"/>
       <c r="F76" s="43"/>
       <c r="G76" s="56"/>
       <c r="H76" s="43"/>
@@ -4519,11 +4523,11 @@
     <row r="77" spans="1:26" ht="10" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="72"/>
-      <c r="C77" s="137" t="s">
-        <v>41</v>
-      </c>
-      <c r="D77" s="129"/>
-      <c r="E77" s="130"/>
+      <c r="C77" s="120" t="s">
+        <v>42</v>
+      </c>
+      <c r="D77" s="115"/>
+      <c r="E77" s="116"/>
       <c r="F77" s="43"/>
       <c r="G77" s="56"/>
       <c r="H77" s="43"/>
@@ -4539,7 +4543,7 @@
       <c r="R77" s="41"/>
       <c r="S77" s="42"/>
       <c r="T77" s="39"/>
-      <c r="U77" s="42"/>
+      <c r="U77" s="58"/>
       <c r="V77" s="100"/>
       <c r="W77" s="40"/>
       <c r="X77" s="43"/>
@@ -4549,9 +4553,9 @@
     <row r="78" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A78" s="1"/>
       <c r="B78" s="72"/>
-      <c r="C78" s="134"/>
-      <c r="D78" s="135"/>
-      <c r="E78" s="136"/>
+      <c r="C78" s="117"/>
+      <c r="D78" s="118"/>
+      <c r="E78" s="119"/>
       <c r="F78" s="43"/>
       <c r="G78" s="56"/>
       <c r="H78" s="43"/>
@@ -4577,11 +4581,11 @@
     <row r="79" spans="1:26" ht="10" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="72"/>
-      <c r="C79" s="137" t="s">
-        <v>42</v>
-      </c>
-      <c r="D79" s="129"/>
-      <c r="E79" s="130"/>
+      <c r="C79" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="115"/>
+      <c r="E79" s="116"/>
       <c r="F79" s="43"/>
       <c r="G79" s="56"/>
       <c r="H79" s="43"/>
@@ -4596,7 +4600,7 @@
       <c r="Q79" s="40"/>
       <c r="R79" s="41"/>
       <c r="S79" s="42"/>
-      <c r="T79" s="39"/>
+      <c r="T79" s="43"/>
       <c r="U79" s="58"/>
       <c r="V79" s="100"/>
       <c r="W79" s="40"/>
@@ -4607,9 +4611,9 @@
     <row r="80" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A80" s="1"/>
       <c r="B80" s="72"/>
-      <c r="C80" s="134"/>
-      <c r="D80" s="135"/>
-      <c r="E80" s="136"/>
+      <c r="C80" s="117"/>
+      <c r="D80" s="118"/>
+      <c r="E80" s="119"/>
       <c r="F80" s="43"/>
       <c r="G80" s="56"/>
       <c r="H80" s="43"/>
@@ -4624,8 +4628,8 @@
       <c r="Q80" s="40"/>
       <c r="R80" s="41"/>
       <c r="S80" s="42"/>
-      <c r="T80" s="43"/>
-      <c r="U80" s="42"/>
+      <c r="T80" s="47"/>
+      <c r="U80" s="66"/>
       <c r="V80" s="100"/>
       <c r="W80" s="40"/>
       <c r="X80" s="43"/>
@@ -4635,11 +4639,11 @@
     <row r="81" spans="1:26" ht="10" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="72"/>
-      <c r="C81" s="137" t="s">
-        <v>9</v>
-      </c>
-      <c r="D81" s="129"/>
-      <c r="E81" s="130"/>
+      <c r="C81" s="120" t="s">
+        <v>46</v>
+      </c>
+      <c r="D81" s="115"/>
+      <c r="E81" s="116"/>
       <c r="F81" s="43"/>
       <c r="G81" s="56"/>
       <c r="H81" s="43"/>
@@ -4654,9 +4658,9 @@
       <c r="Q81" s="40"/>
       <c r="R81" s="41"/>
       <c r="S81" s="42"/>
-      <c r="T81" s="43"/>
-      <c r="U81" s="58"/>
-      <c r="V81" s="100"/>
+      <c r="T81" s="39"/>
+      <c r="U81" s="66"/>
+      <c r="V81" s="102"/>
       <c r="W81" s="40"/>
       <c r="X81" s="43"/>
       <c r="Y81" s="40"/>
@@ -4665,9 +4669,9 @@
     <row r="82" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A82" s="1"/>
       <c r="B82" s="72"/>
-      <c r="C82" s="134"/>
-      <c r="D82" s="135"/>
-      <c r="E82" s="136"/>
+      <c r="C82" s="117"/>
+      <c r="D82" s="118"/>
+      <c r="E82" s="119"/>
       <c r="F82" s="43"/>
       <c r="G82" s="56"/>
       <c r="H82" s="43"/>
@@ -4682,9 +4686,9 @@
       <c r="Q82" s="40"/>
       <c r="R82" s="41"/>
       <c r="S82" s="42"/>
-      <c r="T82" s="47"/>
-      <c r="U82" s="66"/>
-      <c r="V82" s="100"/>
+      <c r="T82" s="43"/>
+      <c r="U82" s="42"/>
+      <c r="V82" s="102"/>
       <c r="W82" s="40"/>
       <c r="X82" s="43"/>
       <c r="Y82" s="40"/>
@@ -4692,149 +4696,149 @@
     </row>
     <row r="83" spans="1:26" ht="10" customHeight="1">
       <c r="A83" s="1"/>
-      <c r="B83" s="72"/>
-      <c r="C83" s="137" t="s">
-        <v>46</v>
-      </c>
-      <c r="D83" s="129"/>
-      <c r="E83" s="130"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="56"/>
-      <c r="H83" s="43"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="41"/>
-      <c r="K83" s="42"/>
-      <c r="L83" s="43"/>
-      <c r="M83" s="42"/>
-      <c r="N83" s="100"/>
-      <c r="O83" s="40"/>
-      <c r="P83" s="43"/>
-      <c r="Q83" s="40"/>
-      <c r="R83" s="41"/>
-      <c r="S83" s="42"/>
-      <c r="T83" s="47"/>
-      <c r="U83" s="58"/>
-      <c r="V83" s="102"/>
-      <c r="W83" s="40"/>
-      <c r="X83" s="43"/>
-      <c r="Y83" s="40"/>
+      <c r="B83" s="182"/>
+      <c r="C83" s="183"/>
+      <c r="D83" s="183"/>
+      <c r="E83" s="184"/>
+      <c r="F83" s="69"/>
+      <c r="G83" s="70"/>
+      <c r="H83" s="69"/>
+      <c r="I83" s="71"/>
+      <c r="J83" s="69"/>
+      <c r="K83" s="71"/>
+      <c r="L83" s="69"/>
+      <c r="M83" s="70"/>
+      <c r="N83" s="104"/>
+      <c r="O83" s="71"/>
+      <c r="P83" s="69"/>
+      <c r="Q83" s="71"/>
+      <c r="R83" s="69"/>
+      <c r="S83" s="71"/>
+      <c r="T83" s="69"/>
+      <c r="U83" s="70"/>
+      <c r="V83" s="104"/>
+      <c r="W83" s="71"/>
+      <c r="X83" s="69"/>
+      <c r="Y83" s="71"/>
       <c r="Z83" s="1"/>
     </row>
-    <row r="84" spans="1:26" ht="10" customHeight="1" thickBot="1">
-      <c r="A84" s="1"/>
-      <c r="B84" s="72"/>
-      <c r="C84" s="134"/>
-      <c r="D84" s="135"/>
-      <c r="E84" s="136"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="56"/>
-      <c r="H84" s="43"/>
-      <c r="I84" s="40"/>
-      <c r="J84" s="41"/>
-      <c r="K84" s="42"/>
-      <c r="L84" s="43"/>
-      <c r="M84" s="42"/>
-      <c r="N84" s="100"/>
-      <c r="O84" s="40"/>
-      <c r="P84" s="43"/>
-      <c r="Q84" s="40"/>
-      <c r="R84" s="41"/>
-      <c r="S84" s="42"/>
-      <c r="T84" s="43"/>
-      <c r="U84" s="42"/>
-      <c r="V84" s="102"/>
-      <c r="W84" s="40"/>
-      <c r="X84" s="43"/>
-      <c r="Y84" s="40"/>
-      <c r="Z84" s="1"/>
-    </row>
-    <row r="85" spans="1:26" ht="10" customHeight="1">
+    <row r="84" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
+      <c r="B84" s="31"/>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="4"/>
+      <c r="L84" s="2"/>
+      <c r="N84" s="96"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="4"/>
+      <c r="T84" s="2"/>
+      <c r="V84" s="96"/>
+      <c r="W84" s="4"/>
+      <c r="X84" s="2"/>
+      <c r="Y84" s="4"/>
+    </row>
+    <row r="85" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A85" s="1"/>
-      <c r="B85" s="125"/>
-      <c r="C85" s="126"/>
-      <c r="D85" s="126"/>
+      <c r="B85" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C85" s="91"/>
+      <c r="D85" s="126">
+        <v>12</v>
+      </c>
       <c r="E85" s="127"/>
-      <c r="F85" s="69"/>
-      <c r="G85" s="70"/>
-      <c r="H85" s="69"/>
-      <c r="I85" s="71"/>
-      <c r="J85" s="69"/>
-      <c r="K85" s="71"/>
-      <c r="L85" s="69"/>
-      <c r="M85" s="70"/>
-      <c r="N85" s="104"/>
-      <c r="O85" s="71"/>
-      <c r="P85" s="69"/>
-      <c r="Q85" s="71"/>
-      <c r="R85" s="69"/>
-      <c r="S85" s="71"/>
-      <c r="T85" s="69"/>
-      <c r="U85" s="70"/>
-      <c r="V85" s="104"/>
-      <c r="W85" s="71"/>
-      <c r="X85" s="69"/>
-      <c r="Y85" s="71"/>
-      <c r="Z85" s="1"/>
-    </row>
-    <row r="86" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
-      <c r="B86" s="31"/>
-      <c r="C86" s="31"/>
-      <c r="D86" s="31"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="4"/>
-      <c r="L86" s="2"/>
-      <c r="N86" s="96"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="2"/>
-      <c r="Q86" s="4"/>
-      <c r="T86" s="2"/>
-      <c r="V86" s="96"/>
-      <c r="W86" s="4"/>
-      <c r="X86" s="2"/>
-      <c r="Y86" s="4"/>
+      <c r="F85" s="60"/>
+      <c r="G85" s="61"/>
+      <c r="H85" s="60"/>
+      <c r="I85" s="62"/>
+      <c r="J85" s="60"/>
+      <c r="K85" s="62"/>
+      <c r="L85" s="60"/>
+      <c r="M85" s="61"/>
+      <c r="N85" s="105"/>
+      <c r="O85" s="62"/>
+      <c r="P85" s="60"/>
+      <c r="Q85" s="62"/>
+      <c r="R85" s="60"/>
+      <c r="S85" s="62"/>
+      <c r="T85" s="60"/>
+      <c r="U85" s="61"/>
+      <c r="V85" s="105"/>
+      <c r="W85" s="62"/>
+      <c r="X85" s="60"/>
+      <c r="Y85" s="61"/>
+      <c r="Z85" s="2"/>
+    </row>
+    <row r="86" spans="1:26" ht="10" customHeight="1">
+      <c r="A86" s="1"/>
+      <c r="B86" s="63"/>
+      <c r="C86" s="120" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86" s="115"/>
+      <c r="E86" s="116"/>
+      <c r="F86" s="43"/>
+      <c r="G86" s="56"/>
+      <c r="H86" s="43"/>
+      <c r="I86" s="40"/>
+      <c r="J86" s="41"/>
+      <c r="K86" s="42"/>
+      <c r="L86" s="43"/>
+      <c r="M86" s="42"/>
+      <c r="N86" s="100"/>
+      <c r="O86" s="40"/>
+      <c r="P86" s="43"/>
+      <c r="Q86" s="40"/>
+      <c r="R86" s="41"/>
+      <c r="S86" s="42"/>
+      <c r="T86" s="47"/>
+      <c r="U86" s="58"/>
+      <c r="V86" s="103"/>
+      <c r="W86" s="40"/>
+      <c r="X86" s="43"/>
+      <c r="Y86" s="40"/>
+      <c r="Z86" s="1"/>
     </row>
     <row r="87" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A87" s="1"/>
-      <c r="B87" s="90" t="s">
-        <v>2</v>
-      </c>
-      <c r="C87" s="91"/>
-      <c r="D87" s="178">
-        <v>12</v>
-      </c>
-      <c r="E87" s="179"/>
-      <c r="F87" s="60"/>
-      <c r="G87" s="61"/>
-      <c r="H87" s="60"/>
-      <c r="I87" s="62"/>
-      <c r="J87" s="60"/>
-      <c r="K87" s="62"/>
-      <c r="L87" s="60"/>
-      <c r="M87" s="61"/>
-      <c r="N87" s="105"/>
-      <c r="O87" s="62"/>
-      <c r="P87" s="60"/>
-      <c r="Q87" s="62"/>
-      <c r="R87" s="60"/>
-      <c r="S87" s="62"/>
-      <c r="T87" s="60"/>
-      <c r="U87" s="61"/>
-      <c r="V87" s="105"/>
-      <c r="W87" s="62"/>
-      <c r="X87" s="60"/>
-      <c r="Y87" s="61"/>
-      <c r="Z87" s="2"/>
+      <c r="B87" s="63"/>
+      <c r="C87" s="117"/>
+      <c r="D87" s="118"/>
+      <c r="E87" s="119"/>
+      <c r="F87" s="43"/>
+      <c r="G87" s="56"/>
+      <c r="H87" s="43"/>
+      <c r="I87" s="40"/>
+      <c r="J87" s="41"/>
+      <c r="K87" s="42"/>
+      <c r="L87" s="43"/>
+      <c r="M87" s="42"/>
+      <c r="N87" s="100"/>
+      <c r="O87" s="40"/>
+      <c r="P87" s="43"/>
+      <c r="Q87" s="40"/>
+      <c r="R87" s="41"/>
+      <c r="S87" s="42"/>
+      <c r="T87" s="43"/>
+      <c r="U87" s="42"/>
+      <c r="V87" s="100"/>
+      <c r="W87" s="40"/>
+      <c r="X87" s="43"/>
+      <c r="Y87" s="40"/>
+      <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" ht="10" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="63"/>
-      <c r="C88" s="137" t="s">
-        <v>3</v>
-      </c>
-      <c r="D88" s="129"/>
-      <c r="E88" s="130"/>
+      <c r="C88" s="120" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88" s="115"/>
+      <c r="E88" s="116"/>
       <c r="F88" s="43"/>
       <c r="G88" s="56"/>
       <c r="H88" s="43"/>
@@ -4849,10 +4853,10 @@
       <c r="Q88" s="40"/>
       <c r="R88" s="41"/>
       <c r="S88" s="42"/>
-      <c r="T88" s="47"/>
-      <c r="U88" s="58"/>
+      <c r="T88" s="43"/>
+      <c r="U88" s="42"/>
       <c r="V88" s="103"/>
-      <c r="W88" s="40"/>
+      <c r="W88" s="48"/>
       <c r="X88" s="43"/>
       <c r="Y88" s="40"/>
       <c r="Z88" s="1"/>
@@ -4860,9 +4864,9 @@
     <row r="89" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A89" s="1"/>
       <c r="B89" s="63"/>
-      <c r="C89" s="134"/>
-      <c r="D89" s="135"/>
-      <c r="E89" s="136"/>
+      <c r="C89" s="117"/>
+      <c r="D89" s="118"/>
+      <c r="E89" s="119"/>
       <c r="F89" s="43"/>
       <c r="G89" s="56"/>
       <c r="H89" s="43"/>
@@ -4887,149 +4891,149 @@
     </row>
     <row r="90" spans="1:26" ht="10" customHeight="1">
       <c r="A90" s="1"/>
-      <c r="B90" s="63"/>
-      <c r="C90" s="137" t="s">
-        <v>10</v>
-      </c>
-      <c r="D90" s="129"/>
-      <c r="E90" s="130"/>
-      <c r="F90" s="43"/>
-      <c r="G90" s="56"/>
-      <c r="H90" s="43"/>
-      <c r="I90" s="40"/>
-      <c r="J90" s="41"/>
-      <c r="K90" s="42"/>
-      <c r="L90" s="43"/>
-      <c r="M90" s="42"/>
-      <c r="N90" s="100"/>
-      <c r="O90" s="40"/>
-      <c r="P90" s="43"/>
-      <c r="Q90" s="40"/>
-      <c r="R90" s="41"/>
-      <c r="S90" s="42"/>
-      <c r="T90" s="43"/>
-      <c r="U90" s="42"/>
-      <c r="V90" s="103"/>
-      <c r="W90" s="48"/>
-      <c r="X90" s="43"/>
-      <c r="Y90" s="40"/>
+      <c r="B90" s="123"/>
+      <c r="C90" s="124"/>
+      <c r="D90" s="124"/>
+      <c r="E90" s="125"/>
+      <c r="F90" s="60"/>
+      <c r="G90" s="61"/>
+      <c r="H90" s="60"/>
+      <c r="I90" s="62"/>
+      <c r="J90" s="60"/>
+      <c r="K90" s="62"/>
+      <c r="L90" s="60"/>
+      <c r="M90" s="61"/>
+      <c r="N90" s="105"/>
+      <c r="O90" s="62"/>
+      <c r="P90" s="60"/>
+      <c r="Q90" s="62"/>
+      <c r="R90" s="60"/>
+      <c r="S90" s="62"/>
+      <c r="T90" s="60"/>
+      <c r="U90" s="61"/>
+      <c r="V90" s="105"/>
+      <c r="W90" s="62"/>
+      <c r="X90" s="60"/>
+      <c r="Y90" s="62"/>
       <c r="Z90" s="1"/>
     </row>
-    <row r="91" spans="1:26" ht="10" customHeight="1" thickBot="1">
-      <c r="A91" s="1"/>
-      <c r="B91" s="63"/>
-      <c r="C91" s="134"/>
-      <c r="D91" s="135"/>
-      <c r="E91" s="136"/>
-      <c r="F91" s="43"/>
-      <c r="G91" s="56"/>
-      <c r="H91" s="43"/>
-      <c r="I91" s="40"/>
-      <c r="J91" s="41"/>
-      <c r="K91" s="42"/>
-      <c r="L91" s="43"/>
-      <c r="M91" s="42"/>
-      <c r="N91" s="100"/>
-      <c r="O91" s="40"/>
-      <c r="P91" s="43"/>
-      <c r="Q91" s="40"/>
-      <c r="R91" s="41"/>
-      <c r="S91" s="42"/>
-      <c r="T91" s="43"/>
-      <c r="U91" s="42"/>
-      <c r="V91" s="100"/>
-      <c r="W91" s="40"/>
-      <c r="X91" s="43"/>
-      <c r="Y91" s="40"/>
-      <c r="Z91" s="1"/>
-    </row>
-    <row r="92" spans="1:26" ht="10" customHeight="1">
+    <row r="91" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
+      <c r="B91" s="31"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="4"/>
+      <c r="L91" s="2"/>
+      <c r="N91" s="96"/>
+      <c r="O91" s="4"/>
+      <c r="P91" s="2"/>
+      <c r="Q91" s="4"/>
+      <c r="T91" s="2"/>
+      <c r="V91" s="96"/>
+      <c r="W91" s="4"/>
+      <c r="X91" s="2"/>
+      <c r="Y91" s="4"/>
+    </row>
+    <row r="92" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A92" s="1"/>
-      <c r="B92" s="175"/>
-      <c r="C92" s="176"/>
-      <c r="D92" s="176"/>
-      <c r="E92" s="177"/>
-      <c r="F92" s="60"/>
-      <c r="G92" s="61"/>
-      <c r="H92" s="60"/>
-      <c r="I92" s="62"/>
-      <c r="J92" s="60"/>
-      <c r="K92" s="62"/>
-      <c r="L92" s="60"/>
-      <c r="M92" s="61"/>
-      <c r="N92" s="105"/>
-      <c r="O92" s="62"/>
-      <c r="P92" s="60"/>
-      <c r="Q92" s="62"/>
-      <c r="R92" s="60"/>
-      <c r="S92" s="62"/>
-      <c r="T92" s="60"/>
-      <c r="U92" s="61"/>
-      <c r="V92" s="105"/>
-      <c r="W92" s="62"/>
-      <c r="X92" s="60"/>
-      <c r="Y92" s="62"/>
+      <c r="B92" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92" s="93"/>
+      <c r="D92" s="121">
+        <v>8</v>
+      </c>
+      <c r="E92" s="122"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="13"/>
+      <c r="M92" s="14"/>
+      <c r="N92" s="97"/>
+      <c r="O92" s="64"/>
+      <c r="P92" s="13"/>
+      <c r="Q92" s="14"/>
+      <c r="R92" s="13"/>
+      <c r="S92" s="14"/>
+      <c r="T92" s="13"/>
+      <c r="U92" s="14"/>
+      <c r="V92" s="97"/>
+      <c r="W92" s="64"/>
+      <c r="X92" s="13"/>
+      <c r="Y92" s="64"/>
       <c r="Z92" s="1"/>
     </row>
-    <row r="93" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
-      <c r="B93" s="31"/>
-      <c r="C93" s="31"/>
-      <c r="D93" s="31"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="4"/>
-      <c r="L93" s="2"/>
-      <c r="N93" s="96"/>
-      <c r="O93" s="4"/>
-      <c r="P93" s="2"/>
-      <c r="Q93" s="4"/>
-      <c r="T93" s="2"/>
-      <c r="V93" s="96"/>
-      <c r="W93" s="4"/>
-      <c r="X93" s="2"/>
-      <c r="Y93" s="4"/>
+    <row r="93" spans="1:26" ht="10" customHeight="1">
+      <c r="A93" s="1"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="120" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="115"/>
+      <c r="E93" s="116"/>
+      <c r="F93" s="43"/>
+      <c r="G93" s="56"/>
+      <c r="H93" s="43"/>
+      <c r="I93" s="40"/>
+      <c r="J93" s="41"/>
+      <c r="K93" s="42"/>
+      <c r="L93" s="43"/>
+      <c r="M93" s="42"/>
+      <c r="N93" s="100"/>
+      <c r="O93" s="40"/>
+      <c r="P93" s="43"/>
+      <c r="Q93" s="40"/>
+      <c r="R93" s="41"/>
+      <c r="S93" s="42"/>
+      <c r="T93" s="43"/>
+      <c r="U93" s="42"/>
+      <c r="V93" s="100"/>
+      <c r="W93" s="40"/>
+      <c r="X93" s="39"/>
+      <c r="Y93" s="40"/>
+      <c r="Z93" s="1"/>
     </row>
     <row r="94" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A94" s="1"/>
-      <c r="B94" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="C94" s="93"/>
-      <c r="D94" s="180">
-        <v>8</v>
-      </c>
-      <c r="E94" s="181"/>
-      <c r="F94" s="13"/>
-      <c r="G94" s="14"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="14"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="14"/>
-      <c r="L94" s="13"/>
-      <c r="M94" s="14"/>
-      <c r="N94" s="97"/>
-      <c r="O94" s="64"/>
-      <c r="P94" s="13"/>
-      <c r="Q94" s="14"/>
-      <c r="R94" s="13"/>
-      <c r="S94" s="14"/>
-      <c r="T94" s="13"/>
-      <c r="U94" s="14"/>
-      <c r="V94" s="97"/>
-      <c r="W94" s="64"/>
-      <c r="X94" s="13"/>
-      <c r="Y94" s="64"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="117"/>
+      <c r="D94" s="118"/>
+      <c r="E94" s="119"/>
+      <c r="F94" s="43"/>
+      <c r="G94" s="56"/>
+      <c r="H94" s="43"/>
+      <c r="I94" s="40"/>
+      <c r="J94" s="41"/>
+      <c r="K94" s="42"/>
+      <c r="L94" s="45"/>
+      <c r="M94" s="42"/>
+      <c r="N94" s="110"/>
+      <c r="O94" s="40"/>
+      <c r="P94" s="43"/>
+      <c r="Q94" s="40"/>
+      <c r="R94" s="41"/>
+      <c r="S94" s="42"/>
+      <c r="T94" s="43"/>
+      <c r="U94" s="42"/>
+      <c r="V94" s="100"/>
+      <c r="W94" s="40"/>
+      <c r="X94" s="43"/>
+      <c r="Y94" s="40"/>
       <c r="Z94" s="1"/>
     </row>
     <row r="95" spans="1:26" ht="10" customHeight="1">
       <c r="A95" s="1"/>
       <c r="B95" s="6"/>
-      <c r="C95" s="137" t="s">
-        <v>24</v>
-      </c>
-      <c r="D95" s="129"/>
-      <c r="E95" s="130"/>
+      <c r="C95" s="120" t="s">
+        <v>54</v>
+      </c>
+      <c r="D95" s="115"/>
+      <c r="E95" s="116"/>
       <c r="F95" s="43"/>
       <c r="G95" s="56"/>
       <c r="H95" s="43"/>
@@ -5055,9 +5059,9 @@
     <row r="96" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A96" s="1"/>
       <c r="B96" s="6"/>
-      <c r="C96" s="134"/>
-      <c r="D96" s="135"/>
-      <c r="E96" s="136"/>
+      <c r="C96" s="117"/>
+      <c r="D96" s="118"/>
+      <c r="E96" s="119"/>
       <c r="F96" s="43"/>
       <c r="G96" s="56"/>
       <c r="H96" s="43"/>
@@ -5083,11 +5087,11 @@
     <row r="97" spans="1:26" ht="10" customHeight="1">
       <c r="A97" s="1"/>
       <c r="B97" s="6"/>
-      <c r="C97" s="137" t="s">
-        <v>55</v>
-      </c>
-      <c r="D97" s="129"/>
-      <c r="E97" s="130"/>
+      <c r="C97" s="120" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" s="115"/>
+      <c r="E97" s="116"/>
       <c r="F97" s="43"/>
       <c r="G97" s="56"/>
       <c r="H97" s="43"/>
@@ -5107,15 +5111,15 @@
       <c r="V97" s="100"/>
       <c r="W97" s="40"/>
       <c r="X97" s="39"/>
-      <c r="Y97" s="40"/>
+      <c r="Y97" s="48"/>
       <c r="Z97" s="1"/>
     </row>
     <row r="98" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A98" s="1"/>
       <c r="B98" s="6"/>
-      <c r="C98" s="134"/>
-      <c r="D98" s="135"/>
-      <c r="E98" s="136"/>
+      <c r="C98" s="117"/>
+      <c r="D98" s="118"/>
+      <c r="E98" s="119"/>
       <c r="F98" s="43"/>
       <c r="G98" s="56"/>
       <c r="H98" s="43"/>
@@ -5135,73 +5139,64 @@
       <c r="V98" s="100"/>
       <c r="W98" s="40"/>
       <c r="X98" s="43"/>
-      <c r="Y98" s="40"/>
-      <c r="Z98" s="1"/>
+      <c r="Y98" s="42"/>
+      <c r="Z98" s="2"/>
     </row>
     <row r="99" spans="1:26" ht="10" customHeight="1">
       <c r="A99" s="1"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="137" t="s">
-        <v>47</v>
-      </c>
-      <c r="D99" s="129"/>
-      <c r="E99" s="130"/>
-      <c r="F99" s="43"/>
-      <c r="G99" s="56"/>
-      <c r="H99" s="43"/>
-      <c r="I99" s="40"/>
-      <c r="J99" s="41"/>
-      <c r="K99" s="42"/>
-      <c r="L99" s="43"/>
-      <c r="M99" s="42"/>
-      <c r="N99" s="100"/>
-      <c r="O99" s="40"/>
-      <c r="P99" s="43"/>
-      <c r="Q99" s="40"/>
-      <c r="R99" s="41"/>
-      <c r="S99" s="42"/>
-      <c r="T99" s="43"/>
-      <c r="U99" s="42"/>
-      <c r="V99" s="100"/>
-      <c r="W99" s="40"/>
-      <c r="X99" s="39"/>
-      <c r="Y99" s="48"/>
-      <c r="Z99" s="1"/>
-    </row>
-    <row r="100" spans="1:26" ht="10" customHeight="1" thickBot="1">
-      <c r="A100" s="1"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="134"/>
-      <c r="D100" s="135"/>
-      <c r="E100" s="136"/>
-      <c r="F100" s="43"/>
-      <c r="G100" s="56"/>
-      <c r="H100" s="43"/>
-      <c r="I100" s="40"/>
-      <c r="J100" s="41"/>
-      <c r="K100" s="42"/>
-      <c r="L100" s="43"/>
-      <c r="M100" s="42"/>
-      <c r="N100" s="100"/>
-      <c r="O100" s="40"/>
-      <c r="P100" s="43"/>
-      <c r="Q100" s="40"/>
-      <c r="R100" s="41"/>
-      <c r="S100" s="42"/>
-      <c r="T100" s="43"/>
-      <c r="U100" s="42"/>
-      <c r="V100" s="100"/>
-      <c r="W100" s="40"/>
-      <c r="X100" s="43"/>
-      <c r="Y100" s="42"/>
+      <c r="B99" s="134"/>
+      <c r="C99" s="135"/>
+      <c r="D99" s="135"/>
+      <c r="E99" s="136"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="14"/>
+      <c r="J99" s="13"/>
+      <c r="K99" s="14"/>
+      <c r="L99" s="13"/>
+      <c r="M99" s="14"/>
+      <c r="N99" s="97"/>
+      <c r="O99" s="64"/>
+      <c r="P99" s="13"/>
+      <c r="Q99" s="14"/>
+      <c r="R99" s="13"/>
+      <c r="S99" s="14"/>
+      <c r="T99" s="13"/>
+      <c r="U99" s="14"/>
+      <c r="V99" s="97"/>
+      <c r="W99" s="64"/>
+      <c r="X99" s="13"/>
+      <c r="Y99" s="14"/>
+      <c r="Z99" s="2"/>
+    </row>
+    <row r="100" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
+      <c r="B100" s="31"/>
+      <c r="C100" s="31"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="32"/>
+      <c r="F100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="4"/>
+      <c r="L100" s="2"/>
+      <c r="N100" s="96"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="2"/>
+      <c r="Q100" s="4"/>
+      <c r="T100" s="2"/>
+      <c r="V100" s="96"/>
+      <c r="W100" s="4"/>
+      <c r="X100" s="2"/>
       <c r="Z100" s="2"/>
     </row>
-    <row r="101" spans="1:26" ht="10" customHeight="1">
+    <row r="101" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A101" s="1"/>
-      <c r="B101" s="110"/>
-      <c r="C101" s="111"/>
-      <c r="D101" s="111"/>
-      <c r="E101" s="112"/>
+      <c r="B101" s="92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C101" s="93"/>
+      <c r="D101" s="170"/>
+      <c r="E101" s="171"/>
       <c r="F101" s="13"/>
       <c r="G101" s="14"/>
       <c r="H101" s="13"/>
@@ -5224,91 +5219,100 @@
       <c r="Y101" s="14"/>
       <c r="Z101" s="2"/>
     </row>
-    <row r="102" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1">
-      <c r="B102" s="31"/>
-      <c r="C102" s="31"/>
-      <c r="D102" s="31"/>
-      <c r="E102" s="32"/>
-      <c r="F102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="4"/>
-      <c r="L102" s="2"/>
-      <c r="N102" s="96"/>
-      <c r="O102" s="4"/>
-      <c r="P102" s="2"/>
-      <c r="Q102" s="4"/>
-      <c r="T102" s="2"/>
-      <c r="V102" s="96"/>
-      <c r="W102" s="4"/>
-      <c r="X102" s="2"/>
+    <row r="102" spans="1:26" ht="10" customHeight="1">
+      <c r="A102" s="1"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="120" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102" s="115"/>
+      <c r="E102" s="116"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="29"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="29"/>
+      <c r="J102" s="17"/>
+      <c r="K102" s="29"/>
+      <c r="L102" s="17"/>
+      <c r="M102" s="29"/>
+      <c r="N102" s="106"/>
+      <c r="O102" s="95"/>
+      <c r="P102" s="17"/>
+      <c r="Q102" s="29"/>
+      <c r="R102" s="17"/>
+      <c r="S102" s="29"/>
+      <c r="T102" s="17"/>
+      <c r="U102" s="29"/>
+      <c r="V102" s="106"/>
+      <c r="W102" s="95"/>
+      <c r="X102" s="17"/>
+      <c r="Y102" s="29"/>
       <c r="Z102" s="2"/>
     </row>
     <row r="103" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A103" s="1"/>
-      <c r="B103" s="92" t="s">
-        <v>26</v>
-      </c>
-      <c r="C103" s="93"/>
-      <c r="D103" s="113"/>
-      <c r="E103" s="114"/>
-      <c r="F103" s="13"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="13"/>
-      <c r="I103" s="14"/>
-      <c r="J103" s="13"/>
-      <c r="K103" s="14"/>
-      <c r="L103" s="13"/>
-      <c r="M103" s="14"/>
-      <c r="N103" s="97"/>
-      <c r="O103" s="64"/>
-      <c r="P103" s="13"/>
-      <c r="Q103" s="14"/>
-      <c r="R103" s="13"/>
-      <c r="S103" s="14"/>
-      <c r="T103" s="13"/>
-      <c r="U103" s="14"/>
-      <c r="V103" s="97"/>
-      <c r="W103" s="64"/>
-      <c r="X103" s="13"/>
-      <c r="Y103" s="14"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="117"/>
+      <c r="D103" s="118"/>
+      <c r="E103" s="119"/>
+      <c r="F103" s="27"/>
+      <c r="G103" s="30"/>
+      <c r="H103" s="47"/>
+      <c r="I103" s="49"/>
+      <c r="J103" s="65"/>
+      <c r="K103" s="77"/>
+      <c r="L103" s="47"/>
+      <c r="M103" s="77"/>
+      <c r="N103" s="102"/>
+      <c r="O103" s="67"/>
+      <c r="P103" s="47"/>
+      <c r="Q103" s="67"/>
+      <c r="R103" s="65"/>
+      <c r="S103" s="66"/>
+      <c r="T103" s="47"/>
+      <c r="U103" s="66"/>
+      <c r="V103" s="102"/>
+      <c r="W103" s="67"/>
+      <c r="X103" s="47"/>
+      <c r="Y103" s="66"/>
       <c r="Z103" s="2"/>
     </row>
     <row r="104" spans="1:26" ht="10" customHeight="1">
       <c r="A104" s="1"/>
       <c r="B104" s="6"/>
-      <c r="C104" s="137" t="s">
-        <v>32</v>
-      </c>
-      <c r="D104" s="129"/>
-      <c r="E104" s="130"/>
-      <c r="F104" s="17"/>
-      <c r="G104" s="29"/>
-      <c r="H104" s="17"/>
-      <c r="I104" s="29"/>
-      <c r="J104" s="17"/>
-      <c r="K104" s="29"/>
-      <c r="L104" s="17"/>
-      <c r="M104" s="29"/>
-      <c r="N104" s="106"/>
-      <c r="O104" s="95"/>
-      <c r="P104" s="17"/>
-      <c r="Q104" s="29"/>
-      <c r="R104" s="17"/>
-      <c r="S104" s="29"/>
-      <c r="T104" s="17"/>
-      <c r="U104" s="29"/>
-      <c r="V104" s="106"/>
-      <c r="W104" s="95"/>
-      <c r="X104" s="17"/>
-      <c r="Y104" s="29"/>
+      <c r="C104" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104" s="115"/>
+      <c r="E104" s="116"/>
+      <c r="F104" s="27"/>
+      <c r="G104" s="75"/>
+      <c r="H104" s="47"/>
+      <c r="I104" s="48"/>
+      <c r="J104" s="65"/>
+      <c r="K104" s="58"/>
+      <c r="L104" s="47"/>
+      <c r="M104" s="58"/>
+      <c r="N104" s="102"/>
+      <c r="O104" s="48"/>
+      <c r="P104" s="47"/>
+      <c r="Q104" s="48"/>
+      <c r="R104" s="65"/>
+      <c r="S104" s="58"/>
+      <c r="T104" s="47"/>
+      <c r="U104" s="58"/>
+      <c r="V104" s="102"/>
+      <c r="W104" s="48"/>
+      <c r="X104" s="47"/>
+      <c r="Y104" s="58"/>
       <c r="Z104" s="2"/>
     </row>
     <row r="105" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A105" s="1"/>
       <c r="B105" s="6"/>
-      <c r="C105" s="134"/>
-      <c r="D105" s="135"/>
-      <c r="E105" s="136"/>
+      <c r="C105" s="117"/>
+      <c r="D105" s="118"/>
+      <c r="E105" s="119"/>
       <c r="F105" s="27"/>
       <c r="G105" s="30"/>
       <c r="H105" s="47"/>
@@ -5334,47 +5338,49 @@
     <row r="106" spans="1:26" ht="10" customHeight="1">
       <c r="A106" s="1"/>
       <c r="B106" s="6"/>
-      <c r="C106" s="137" t="s">
-        <v>65</v>
-      </c>
-      <c r="D106" s="129"/>
-      <c r="E106" s="130"/>
-      <c r="F106" s="27"/>
-      <c r="G106" s="75"/>
-      <c r="H106" s="47"/>
-      <c r="I106" s="48"/>
-      <c r="J106" s="65"/>
-      <c r="K106" s="58"/>
-      <c r="L106" s="47"/>
-      <c r="M106" s="58"/>
-      <c r="N106" s="102"/>
-      <c r="O106" s="48"/>
-      <c r="P106" s="47"/>
-      <c r="Q106" s="48"/>
-      <c r="R106" s="65"/>
-      <c r="S106" s="58"/>
-      <c r="T106" s="47"/>
-      <c r="U106" s="58"/>
-      <c r="V106" s="102"/>
-      <c r="W106" s="48"/>
-      <c r="X106" s="47"/>
-      <c r="Y106" s="58"/>
+      <c r="C106" s="120" t="s">
+        <v>48</v>
+      </c>
+      <c r="D106" s="115"/>
+      <c r="E106" s="73">
+        <v>5</v>
+      </c>
+      <c r="F106" s="39"/>
+      <c r="G106" s="16"/>
+      <c r="H106" s="39"/>
+      <c r="I106" s="67"/>
+      <c r="J106" s="57"/>
+      <c r="K106" s="66"/>
+      <c r="L106" s="39"/>
+      <c r="M106" s="66"/>
+      <c r="N106" s="103"/>
+      <c r="O106" s="67"/>
+      <c r="P106" s="39"/>
+      <c r="Q106" s="67"/>
+      <c r="R106" s="57"/>
+      <c r="S106" s="66"/>
+      <c r="T106" s="39"/>
+      <c r="U106" s="66"/>
+      <c r="V106" s="103"/>
+      <c r="W106" s="67"/>
+      <c r="X106" s="39"/>
+      <c r="Y106" s="66"/>
       <c r="Z106" s="2"/>
     </row>
     <row r="107" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A107" s="1"/>
       <c r="B107" s="6"/>
-      <c r="C107" s="134"/>
-      <c r="D107" s="135"/>
-      <c r="E107" s="136"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="30"/>
+      <c r="C107" s="117"/>
+      <c r="D107" s="118"/>
+      <c r="E107" s="59"/>
+      <c r="F107" s="45"/>
+      <c r="G107" s="68"/>
       <c r="H107" s="47"/>
-      <c r="I107" s="49"/>
+      <c r="I107" s="67"/>
       <c r="J107" s="65"/>
-      <c r="K107" s="77"/>
+      <c r="K107" s="66"/>
       <c r="L107" s="47"/>
-      <c r="M107" s="77"/>
+      <c r="M107" s="66"/>
       <c r="N107" s="102"/>
       <c r="O107" s="67"/>
       <c r="P107" s="47"/>
@@ -5389,148 +5395,144 @@
       <c r="Y107" s="66"/>
       <c r="Z107" s="2"/>
     </row>
-    <row r="108" spans="1:26" ht="10" customHeight="1">
-      <c r="A108" s="1"/>
-      <c r="B108" s="6"/>
-      <c r="C108" s="137" t="s">
-        <v>48</v>
-      </c>
-      <c r="D108" s="129"/>
-      <c r="E108" s="73">
-        <v>5</v>
-      </c>
-      <c r="F108" s="39"/>
-      <c r="G108" s="16"/>
-      <c r="H108" s="39"/>
-      <c r="I108" s="67"/>
-      <c r="J108" s="57"/>
-      <c r="K108" s="66"/>
-      <c r="L108" s="39"/>
-      <c r="M108" s="66"/>
-      <c r="N108" s="103"/>
-      <c r="O108" s="67"/>
-      <c r="P108" s="39"/>
-      <c r="Q108" s="67"/>
-      <c r="R108" s="57"/>
-      <c r="S108" s="66"/>
-      <c r="T108" s="39"/>
-      <c r="U108" s="66"/>
-      <c r="V108" s="103"/>
-      <c r="W108" s="67"/>
-      <c r="X108" s="39"/>
-      <c r="Y108" s="66"/>
+    <row r="108" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
+      <c r="B108" s="134"/>
+      <c r="C108" s="135"/>
+      <c r="D108" s="135"/>
+      <c r="E108" s="136"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="13"/>
+      <c r="K108" s="14"/>
+      <c r="L108" s="13"/>
+      <c r="M108" s="14"/>
+      <c r="N108" s="97"/>
+      <c r="O108" s="64"/>
+      <c r="P108" s="13"/>
+      <c r="Q108" s="14"/>
+      <c r="R108" s="13"/>
+      <c r="S108" s="14"/>
+      <c r="T108" s="13"/>
+      <c r="U108" s="14"/>
+      <c r="V108" s="97"/>
+      <c r="W108" s="64"/>
+      <c r="X108" s="13"/>
+      <c r="Y108" s="14"/>
       <c r="Z108" s="2"/>
     </row>
-    <row r="109" spans="1:26" ht="10" customHeight="1" thickBot="1">
-      <c r="A109" s="1"/>
-      <c r="B109" s="6"/>
-      <c r="C109" s="134"/>
-      <c r="D109" s="135"/>
-      <c r="E109" s="59"/>
-      <c r="F109" s="45"/>
-      <c r="G109" s="68"/>
-      <c r="H109" s="47"/>
-      <c r="I109" s="67"/>
-      <c r="J109" s="65"/>
-      <c r="K109" s="66"/>
-      <c r="L109" s="47"/>
-      <c r="M109" s="66"/>
-      <c r="N109" s="102"/>
-      <c r="O109" s="67"/>
-      <c r="P109" s="47"/>
-      <c r="Q109" s="67"/>
-      <c r="R109" s="65"/>
-      <c r="S109" s="66"/>
-      <c r="T109" s="47"/>
-      <c r="U109" s="66"/>
-      <c r="V109" s="102"/>
-      <c r="W109" s="67"/>
-      <c r="X109" s="47"/>
-      <c r="Y109" s="66"/>
+    <row r="109" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
+      <c r="B109" s="153"/>
+      <c r="C109" s="153"/>
+      <c r="D109" s="153"/>
+      <c r="E109" s="32"/>
+      <c r="F109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="4"/>
+      <c r="L109" s="2"/>
+      <c r="N109" s="96"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="2"/>
+      <c r="Q109" s="4"/>
+      <c r="T109" s="2"/>
+      <c r="V109" s="96"/>
+      <c r="W109" s="4"/>
+      <c r="X109" s="2"/>
       <c r="Z109" s="2"/>
     </row>
     <row r="110" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B110" s="110"/>
-      <c r="C110" s="111"/>
-      <c r="D110" s="111"/>
-      <c r="E110" s="112"/>
-      <c r="F110" s="13"/>
-      <c r="G110" s="14"/>
-      <c r="H110" s="13"/>
-      <c r="I110" s="14"/>
-      <c r="J110" s="13"/>
-      <c r="K110" s="14"/>
-      <c r="L110" s="13"/>
-      <c r="M110" s="14"/>
-      <c r="N110" s="97"/>
-      <c r="O110" s="64"/>
-      <c r="P110" s="13"/>
-      <c r="Q110" s="14"/>
-      <c r="R110" s="13"/>
-      <c r="S110" s="14"/>
-      <c r="T110" s="13"/>
-      <c r="U110" s="14"/>
-      <c r="V110" s="97"/>
-      <c r="W110" s="64"/>
-      <c r="X110" s="13"/>
-      <c r="Y110" s="14"/>
-      <c r="Z110" s="2"/>
-    </row>
-    <row r="111" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
-      <c r="B111" s="174"/>
-      <c r="C111" s="174"/>
-      <c r="D111" s="174"/>
-      <c r="E111" s="32"/>
-      <c r="F111" s="2"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="4"/>
-      <c r="L111" s="2"/>
-      <c r="N111" s="96"/>
-      <c r="O111" s="4"/>
-      <c r="P111" s="2"/>
-      <c r="Q111" s="4"/>
-      <c r="T111" s="2"/>
-      <c r="V111" s="96"/>
-      <c r="W111" s="4"/>
-      <c r="X111" s="2"/>
-      <c r="Z111" s="2"/>
-    </row>
-    <row r="112" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B112" s="170" t="s">
+      <c r="B110" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="C112" s="171"/>
-      <c r="D112" s="182"/>
-      <c r="E112" s="184" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="113" spans="1:26" ht="10" customHeight="1" thickBot="1">
+      <c r="C110" s="129"/>
+      <c r="D110" s="130"/>
+      <c r="E110" s="112" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="111" spans="1:26" ht="10" customHeight="1" thickBot="1">
+      <c r="A111" s="1"/>
+      <c r="B111" s="131"/>
+      <c r="C111" s="132"/>
+      <c r="D111" s="133"/>
+      <c r="E111" s="113"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="3"/>
+      <c r="M111" s="3"/>
+      <c r="N111" s="3"/>
+      <c r="O111" s="3"/>
+      <c r="P111" s="3"/>
+      <c r="Q111" s="3"/>
+      <c r="R111" s="3"/>
+      <c r="S111" s="3"/>
+      <c r="T111" s="3"/>
+      <c r="U111" s="3"/>
+      <c r="V111" s="3"/>
+      <c r="W111" s="3"/>
+      <c r="X111" s="3"/>
+      <c r="Y111" s="3"/>
+      <c r="Z111" s="1"/>
+    </row>
+    <row r="112" spans="1:26">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
+      <c r="M112" s="3"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="1"/>
+      <c r="P112" s="1"/>
+      <c r="Q112" s="1"/>
+      <c r="R112" s="1"/>
+      <c r="S112" s="1"/>
+      <c r="T112" s="1"/>
+      <c r="U112" s="1"/>
+      <c r="V112" s="1"/>
+      <c r="W112" s="1"/>
+      <c r="X112" s="1"/>
+      <c r="Y112" s="1"/>
+      <c r="Z112" s="1"/>
+    </row>
+    <row r="113" spans="1:26">
       <c r="A113" s="1"/>
-      <c r="B113" s="172"/>
-      <c r="C113" s="173"/>
-      <c r="D113" s="183"/>
-      <c r="E113" s="185"/>
-      <c r="F113" s="3"/>
-      <c r="G113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="3"/>
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-      <c r="L113" s="3"/>
-      <c r="M113" s="3"/>
-      <c r="N113" s="3"/>
-      <c r="O113" s="3"/>
-      <c r="P113" s="3"/>
-      <c r="Q113" s="3"/>
-      <c r="R113" s="3"/>
-      <c r="S113" s="3"/>
-      <c r="T113" s="3"/>
-      <c r="U113" s="3"/>
-      <c r="V113" s="3"/>
-      <c r="W113" s="3"/>
-      <c r="X113" s="3"/>
-      <c r="Y113" s="3"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+      <c r="Q113" s="1"/>
+      <c r="R113" s="1"/>
+      <c r="S113" s="1"/>
+      <c r="T113" s="1"/>
+      <c r="U113" s="1"/>
+      <c r="V113" s="1"/>
+      <c r="W113" s="1"/>
+      <c r="X113" s="1"/>
+      <c r="Y113" s="1"/>
       <c r="Z113" s="1"/>
     </row>
     <row r="114" spans="1:26">
@@ -5539,15 +5541,15 @@
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
-      <c r="F114" s="2"/>
-      <c r="G114" s="3"/>
-      <c r="H114" s="3"/>
-      <c r="I114" s="3"/>
-      <c r="J114" s="3"/>
-      <c r="K114" s="3"/>
-      <c r="L114" s="3"/>
-      <c r="M114" s="3"/>
-      <c r="N114" s="3"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
       <c r="O114" s="1"/>
       <c r="P114" s="1"/>
       <c r="Q114" s="1"/>
@@ -5617,61 +5619,13 @@
       <c r="Y116" s="1"/>
       <c r="Z116" s="1"/>
     </row>
-    <row r="117" spans="1:26">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
-      <c r="G117" s="1"/>
-      <c r="H117" s="1"/>
-      <c r="I117" s="1"/>
-      <c r="J117" s="1"/>
-      <c r="K117" s="1"/>
-      <c r="L117" s="1"/>
-      <c r="M117" s="1"/>
-      <c r="N117" s="1"/>
-      <c r="O117" s="1"/>
-      <c r="P117" s="1"/>
-      <c r="Q117" s="1"/>
-      <c r="R117" s="1"/>
-      <c r="S117" s="1"/>
-      <c r="T117" s="1"/>
-      <c r="U117" s="1"/>
-      <c r="V117" s="1"/>
-      <c r="W117" s="1"/>
-      <c r="X117" s="1"/>
-      <c r="Y117" s="1"/>
-      <c r="Z117" s="1"/>
-    </row>
-    <row r="118" spans="1:26">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="1"/>
-      <c r="J118" s="1"/>
-      <c r="K118" s="1"/>
-      <c r="L118" s="1"/>
-      <c r="M118" s="1"/>
-      <c r="N118" s="1"/>
-      <c r="O118" s="1"/>
-      <c r="P118" s="1"/>
-      <c r="Q118" s="1"/>
-      <c r="R118" s="1"/>
-      <c r="S118" s="1"/>
-      <c r="T118" s="1"/>
-      <c r="U118" s="1"/>
-      <c r="V118" s="1"/>
-      <c r="W118" s="1"/>
-      <c r="X118" s="1"/>
-      <c r="Y118" s="1"/>
-      <c r="Z118" s="1"/>
+    <row r="121" spans="1:26">
+      <c r="M121" s="1"/>
+      <c r="N121" s="1"/>
+    </row>
+    <row r="122" spans="1:26">
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
     </row>
     <row r="123" spans="1:26">
       <c r="M123" s="1"/>
@@ -5690,16 +5644,16 @@
       <c r="N126" s="1"/>
     </row>
     <row r="127" spans="1:26">
-      <c r="M127" s="1"/>
-      <c r="N127" s="1"/>
+      <c r="M127" s="3"/>
+      <c r="N127" s="3"/>
     </row>
     <row r="128" spans="1:26">
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
     </row>
     <row r="129" spans="13:14">
-      <c r="M129" s="3"/>
-      <c r="N129" s="3"/>
+      <c r="M129" s="1"/>
+      <c r="N129" s="1"/>
     </row>
     <row r="130" spans="13:14">
       <c r="M130" s="1"/>
@@ -5726,16 +5680,16 @@
       <c r="N135" s="1"/>
     </row>
     <row r="136" spans="13:14">
-      <c r="M136" s="1"/>
-      <c r="N136" s="1"/>
+      <c r="M136" s="3"/>
+      <c r="N136" s="3"/>
     </row>
     <row r="137" spans="13:14">
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
     </row>
     <row r="138" spans="13:14">
-      <c r="M138" s="3"/>
-      <c r="N138" s="3"/>
+      <c r="M138" s="1"/>
+      <c r="N138" s="1"/>
     </row>
     <row r="139" spans="13:14">
       <c r="M139" s="1"/>
@@ -5778,16 +5732,16 @@
       <c r="N148" s="1"/>
     </row>
     <row r="149" spans="13:14">
-      <c r="M149" s="1"/>
-      <c r="N149" s="1"/>
+      <c r="M149" s="3"/>
+      <c r="N149" s="3"/>
     </row>
     <row r="150" spans="13:14">
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
     </row>
     <row r="151" spans="13:14">
-      <c r="M151" s="3"/>
-      <c r="N151" s="3"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
     </row>
     <row r="152" spans="13:14">
       <c r="M152" s="1"/>
@@ -5838,16 +5792,16 @@
       <c r="N163" s="1"/>
     </row>
     <row r="164" spans="13:14">
-      <c r="M164" s="1"/>
-      <c r="N164" s="1"/>
+      <c r="M164" s="3"/>
+      <c r="N164" s="3"/>
     </row>
     <row r="165" spans="13:14">
       <c r="M165" s="1"/>
       <c r="N165" s="1"/>
     </row>
     <row r="166" spans="13:14">
-      <c r="M166" s="3"/>
-      <c r="N166" s="3"/>
+      <c r="M166" s="1"/>
+      <c r="N166" s="1"/>
     </row>
     <row r="167" spans="13:14">
       <c r="M167" s="1"/>
@@ -5890,16 +5844,16 @@
       <c r="N176" s="1"/>
     </row>
     <row r="177" spans="13:14">
-      <c r="M177" s="1"/>
-      <c r="N177" s="1"/>
+      <c r="M177" s="3"/>
+      <c r="N177" s="3"/>
     </row>
     <row r="178" spans="13:14">
       <c r="M178" s="1"/>
       <c r="N178" s="1"/>
     </row>
     <row r="179" spans="13:14">
-      <c r="M179" s="3"/>
-      <c r="N179" s="3"/>
+      <c r="M179" s="1"/>
+      <c r="N179" s="1"/>
     </row>
     <row r="180" spans="13:14">
       <c r="M180" s="1"/>
@@ -5918,16 +5872,16 @@
       <c r="N183" s="1"/>
     </row>
     <row r="184" spans="13:14">
-      <c r="M184" s="1"/>
-      <c r="N184" s="1"/>
+      <c r="M184" s="3"/>
+      <c r="N184" s="3"/>
     </row>
     <row r="185" spans="13:14">
       <c r="M185" s="1"/>
       <c r="N185" s="1"/>
     </row>
     <row r="186" spans="13:14">
-      <c r="M186" s="3"/>
-      <c r="N186" s="3"/>
+      <c r="M186" s="1"/>
+      <c r="N186" s="1"/>
     </row>
     <row r="187" spans="13:14">
       <c r="M187" s="1"/>
@@ -5954,16 +5908,16 @@
       <c r="N192" s="1"/>
     </row>
     <row r="193" spans="13:14">
-      <c r="M193" s="1"/>
-      <c r="N193" s="1"/>
+      <c r="M193" s="3"/>
+      <c r="N193" s="3"/>
     </row>
     <row r="194" spans="13:14">
       <c r="M194" s="1"/>
       <c r="N194" s="1"/>
     </row>
     <row r="195" spans="13:14">
-      <c r="M195" s="3"/>
-      <c r="N195" s="3"/>
+      <c r="M195" s="1"/>
+      <c r="N195" s="1"/>
     </row>
     <row r="196" spans="13:14">
       <c r="M196" s="1"/>
@@ -5986,24 +5940,24 @@
       <c r="N200" s="1"/>
     </row>
     <row r="201" spans="13:14">
-      <c r="M201" s="1"/>
-      <c r="N201" s="1"/>
+      <c r="M201" s="3"/>
+      <c r="N201" s="3"/>
     </row>
     <row r="202" spans="13:14">
-      <c r="M202" s="1"/>
-      <c r="N202" s="1"/>
+      <c r="M202" s="3"/>
+      <c r="N202" s="3"/>
     </row>
     <row r="203" spans="13:14">
       <c r="M203" s="3"/>
       <c r="N203" s="3"/>
     </row>
     <row r="204" spans="13:14">
-      <c r="M204" s="3"/>
-      <c r="N204" s="3"/>
+      <c r="M204" s="1"/>
+      <c r="N204" s="1"/>
     </row>
     <row r="205" spans="13:14">
-      <c r="M205" s="3"/>
-      <c r="N205" s="3"/>
+      <c r="M205" s="1"/>
+      <c r="N205" s="1"/>
     </row>
     <row r="206" spans="13:14">
       <c r="M206" s="1"/>
@@ -6025,56 +5979,25 @@
       <c r="M210" s="1"/>
       <c r="N210" s="1"/>
     </row>
-    <row r="211" spans="13:14">
-      <c r="M211" s="1"/>
-      <c r="N211" s="1"/>
-    </row>
-    <row r="212" spans="13:14">
-      <c r="M212" s="1"/>
-      <c r="N212" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="82">
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="C73:E74"/>
+  <mergeCells count="81">
+    <mergeCell ref="C97:E98"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="B108:E108"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="B83:E83"/>
     <mergeCell ref="C67:E68"/>
-    <mergeCell ref="C65:E66"/>
-    <mergeCell ref="C77:E78"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="C90:E91"/>
-    <mergeCell ref="C95:E96"/>
-    <mergeCell ref="C104:E105"/>
-    <mergeCell ref="C75:E76"/>
-    <mergeCell ref="C97:E98"/>
+    <mergeCell ref="C69:E70"/>
+    <mergeCell ref="C44:E45"/>
+    <mergeCell ref="C86:E87"/>
+    <mergeCell ref="C56:E57"/>
     <mergeCell ref="C81:E82"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="C79:E80"/>
-    <mergeCell ref="V2:W8"/>
-    <mergeCell ref="X2:Y8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="T2:U8"/>
-    <mergeCell ref="R2:S8"/>
-    <mergeCell ref="B112:D113"/>
-    <mergeCell ref="C108:D109"/>
-    <mergeCell ref="C99:E100"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="C33:E34"/>
-    <mergeCell ref="C60:E61"/>
-    <mergeCell ref="C37:E38"/>
-    <mergeCell ref="C56:E57"/>
-    <mergeCell ref="C35:E36"/>
-    <mergeCell ref="C42:E43"/>
-    <mergeCell ref="C48:E49"/>
     <mergeCell ref="C52:E53"/>
-    <mergeCell ref="C44:E45"/>
-    <mergeCell ref="C106:E107"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="C50:E51"/>
-    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="C106:D107"/>
     <mergeCell ref="B5:C6"/>
     <mergeCell ref="P9:Q9"/>
     <mergeCell ref="F2:G8"/>
@@ -6090,6 +6013,12 @@
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="E3:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C50:E51"/>
+    <mergeCell ref="C42:E43"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="C48:E49"/>
+    <mergeCell ref="B7:C8"/>
     <mergeCell ref="C31:E32"/>
     <mergeCell ref="C24:E25"/>
     <mergeCell ref="C16:E17"/>
@@ -6099,26 +6028,43 @@
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="C12:E13"/>
     <mergeCell ref="C18:E19"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B101:E101"/>
-    <mergeCell ref="B110:E110"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="C69:E70"/>
+    <mergeCell ref="C104:E105"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="V2:W8"/>
+    <mergeCell ref="X2:Y8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="T2:U8"/>
+    <mergeCell ref="R2:S8"/>
+    <mergeCell ref="C33:E34"/>
+    <mergeCell ref="C58:E59"/>
+    <mergeCell ref="C37:E38"/>
+    <mergeCell ref="C54:E55"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="C46:E47"/>
+    <mergeCell ref="E110:E111"/>
     <mergeCell ref="C71:E72"/>
-    <mergeCell ref="C46:E47"/>
+    <mergeCell ref="C65:E66"/>
+    <mergeCell ref="C63:E64"/>
+    <mergeCell ref="C75:E76"/>
+    <mergeCell ref="D92:E92"/>
     <mergeCell ref="C88:E89"/>
-    <mergeCell ref="C58:E59"/>
-    <mergeCell ref="C83:E84"/>
-    <mergeCell ref="C54:E55"/>
+    <mergeCell ref="C93:E94"/>
+    <mergeCell ref="C102:E103"/>
+    <mergeCell ref="C73:E74"/>
+    <mergeCell ref="C95:E96"/>
+    <mergeCell ref="C79:E80"/>
+    <mergeCell ref="B90:E90"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="C77:E78"/>
+    <mergeCell ref="B110:D111"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Dokumentation V0.5 abgeschlossen, Zeitplan angepasst, Skript angefange zu erarbeiten.
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <workbookPr filterPrivacy="1" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="41860" yWindow="6780" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="2140" yWindow="540" windowWidth="34640" windowHeight="22900"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -914,8 +914,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1348,15 +1360,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1405,9 +1408,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1420,6 +1420,36 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1438,24 +1468,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1511,7 +1523,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1588,6 +1600,12 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1664,6 +1682,12 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2306,18 +2330,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="N94" sqref="N94"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="3.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="4.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="5" customWidth="1"/>
-    <col min="6" max="25" width="3.83203125" style="5" customWidth="1"/>
+    <col min="6" max="25" width="3.5" style="5" customWidth="1"/>
     <col min="26" max="26" width="4.6640625" style="5" customWidth="1"/>
     <col min="27" max="16384" width="9.1640625" style="5"/>
   </cols>
@@ -2352,50 +2376,50 @@
     </row>
     <row r="2" spans="1:31" ht="16" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="160"/>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="143" t="s">
+      <c r="B2" s="166"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="152"/>
-      <c r="H2" s="143" t="s">
+      <c r="G2" s="149"/>
+      <c r="H2" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="138"/>
-      <c r="J2" s="152" t="s">
+      <c r="I2" s="135"/>
+      <c r="J2" s="149" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="152"/>
-      <c r="L2" s="143" t="s">
+      <c r="K2" s="149"/>
+      <c r="L2" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="152"/>
-      <c r="N2" s="137" t="s">
+      <c r="M2" s="149"/>
+      <c r="N2" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="138"/>
-      <c r="P2" s="143" t="s">
+      <c r="O2" s="135"/>
+      <c r="P2" s="140" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="138"/>
-      <c r="R2" s="152" t="s">
+      <c r="Q2" s="135"/>
+      <c r="R2" s="149" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="152"/>
-      <c r="T2" s="143" t="s">
+      <c r="S2" s="149"/>
+      <c r="T2" s="140" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="152"/>
-      <c r="V2" s="137" t="s">
+      <c r="U2" s="149"/>
+      <c r="V2" s="134" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="138"/>
-      <c r="X2" s="143" t="s">
+      <c r="W2" s="135"/>
+      <c r="X2" s="140" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="138"/>
+      <c r="Y2" s="135"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:31" ht="14" customHeight="1">
@@ -2405,27 +2429,27 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="145"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="145"/>
-      <c r="N3" s="139"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="144"/>
-      <c r="Q3" s="140"/>
-      <c r="R3" s="145"/>
-      <c r="S3" s="145"/>
-      <c r="T3" s="144"/>
-      <c r="U3" s="145"/>
-      <c r="V3" s="139"/>
-      <c r="W3" s="140"/>
-      <c r="X3" s="144"/>
-      <c r="Y3" s="140"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="136"/>
+      <c r="O3" s="137"/>
+      <c r="P3" s="141"/>
+      <c r="Q3" s="137"/>
+      <c r="R3" s="142"/>
+      <c r="S3" s="142"/>
+      <c r="T3" s="141"/>
+      <c r="U3" s="142"/>
+      <c r="V3" s="136"/>
+      <c r="W3" s="137"/>
+      <c r="X3" s="141"/>
+      <c r="Y3" s="137"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:31" ht="14" customHeight="1">
@@ -2435,143 +2459,143 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="145"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="140"/>
-      <c r="J4" s="145"/>
-      <c r="K4" s="145"/>
-      <c r="L4" s="144"/>
-      <c r="M4" s="145"/>
-      <c r="N4" s="139"/>
-      <c r="O4" s="140"/>
-      <c r="P4" s="144"/>
-      <c r="Q4" s="140"/>
-      <c r="R4" s="145"/>
-      <c r="S4" s="145"/>
-      <c r="T4" s="144"/>
-      <c r="U4" s="145"/>
-      <c r="V4" s="139"/>
-      <c r="W4" s="140"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="140"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="141"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="141"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="137"/>
+      <c r="P4" s="141"/>
+      <c r="Q4" s="137"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="141"/>
+      <c r="U4" s="142"/>
+      <c r="V4" s="136"/>
+      <c r="W4" s="137"/>
+      <c r="X4" s="141"/>
+      <c r="Y4" s="137"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:31" ht="7" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="158" t="s">
+      <c r="B5" s="164" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="159"/>
+      <c r="C5" s="165"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="162"/>
-      <c r="F5" s="144"/>
-      <c r="G5" s="145"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="140"/>
-      <c r="J5" s="145"/>
-      <c r="K5" s="145"/>
-      <c r="L5" s="144"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="139"/>
-      <c r="O5" s="140"/>
-      <c r="P5" s="144"/>
-      <c r="Q5" s="140"/>
-      <c r="R5" s="145"/>
-      <c r="S5" s="145"/>
-      <c r="T5" s="144"/>
-      <c r="U5" s="145"/>
-      <c r="V5" s="139"/>
-      <c r="W5" s="140"/>
-      <c r="X5" s="144"/>
-      <c r="Y5" s="145"/>
+      <c r="E5" s="168"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="142"/>
+      <c r="K5" s="142"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="142"/>
+      <c r="N5" s="136"/>
+      <c r="O5" s="137"/>
+      <c r="P5" s="141"/>
+      <c r="Q5" s="137"/>
+      <c r="R5" s="142"/>
+      <c r="S5" s="142"/>
+      <c r="T5" s="141"/>
+      <c r="U5" s="142"/>
+      <c r="V5" s="136"/>
+      <c r="W5" s="137"/>
+      <c r="X5" s="141"/>
+      <c r="Y5" s="142"/>
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:31" ht="7" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="158"/>
-      <c r="C6" s="159"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="165"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="162"/>
-      <c r="F6" s="144"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="144"/>
-      <c r="I6" s="140"/>
-      <c r="J6" s="145"/>
-      <c r="K6" s="145"/>
-      <c r="L6" s="144"/>
-      <c r="M6" s="145"/>
-      <c r="N6" s="139"/>
-      <c r="O6" s="140"/>
-      <c r="P6" s="144"/>
-      <c r="Q6" s="140"/>
-      <c r="R6" s="145"/>
-      <c r="S6" s="145"/>
-      <c r="T6" s="144"/>
-      <c r="U6" s="145"/>
-      <c r="V6" s="139"/>
-      <c r="W6" s="140"/>
-      <c r="X6" s="144"/>
-      <c r="Y6" s="145"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="141"/>
+      <c r="I6" s="137"/>
+      <c r="J6" s="142"/>
+      <c r="K6" s="142"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="142"/>
+      <c r="N6" s="136"/>
+      <c r="O6" s="137"/>
+      <c r="P6" s="141"/>
+      <c r="Q6" s="137"/>
+      <c r="R6" s="142"/>
+      <c r="S6" s="142"/>
+      <c r="T6" s="141"/>
+      <c r="U6" s="142"/>
+      <c r="V6" s="136"/>
+      <c r="W6" s="137"/>
+      <c r="X6" s="141"/>
+      <c r="Y6" s="142"/>
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:31" ht="7" customHeight="1" thickBot="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="154" t="s">
+      <c r="B7" s="150" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="155"/>
+      <c r="C7" s="151"/>
       <c r="D7" s="108"/>
-      <c r="E7" s="162"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="145"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="145"/>
-      <c r="K7" s="145"/>
-      <c r="L7" s="144"/>
-      <c r="M7" s="145"/>
-      <c r="N7" s="139"/>
-      <c r="O7" s="140"/>
-      <c r="P7" s="144"/>
-      <c r="Q7" s="140"/>
-      <c r="R7" s="145"/>
-      <c r="S7" s="145"/>
-      <c r="T7" s="144"/>
-      <c r="U7" s="145"/>
-      <c r="V7" s="139"/>
-      <c r="W7" s="140"/>
-      <c r="X7" s="144"/>
-      <c r="Y7" s="145"/>
+      <c r="E7" s="168"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="142"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="137"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="136"/>
+      <c r="O7" s="137"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="142"/>
+      <c r="S7" s="142"/>
+      <c r="T7" s="141"/>
+      <c r="U7" s="142"/>
+      <c r="V7" s="136"/>
+      <c r="W7" s="137"/>
+      <c r="X7" s="141"/>
+      <c r="Y7" s="142"/>
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:31" ht="7" customHeight="1" thickTop="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="156"/>
-      <c r="C8" s="157"/>
+      <c r="B8" s="152"/>
+      <c r="C8" s="153"/>
       <c r="D8" s="107"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="147"/>
-      <c r="H8" s="146"/>
-      <c r="I8" s="142"/>
-      <c r="J8" s="147"/>
-      <c r="K8" s="147"/>
-      <c r="L8" s="146"/>
-      <c r="M8" s="147"/>
-      <c r="N8" s="141"/>
-      <c r="O8" s="142"/>
-      <c r="P8" s="146"/>
-      <c r="Q8" s="142"/>
-      <c r="R8" s="147"/>
-      <c r="S8" s="147"/>
-      <c r="T8" s="146"/>
-      <c r="U8" s="147"/>
-      <c r="V8" s="141"/>
-      <c r="W8" s="142"/>
-      <c r="X8" s="146"/>
-      <c r="Y8" s="147"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="144"/>
+      <c r="H8" s="143"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="144"/>
+      <c r="K8" s="144"/>
+      <c r="L8" s="143"/>
+      <c r="M8" s="144"/>
+      <c r="N8" s="138"/>
+      <c r="O8" s="139"/>
+      <c r="P8" s="143"/>
+      <c r="Q8" s="139"/>
+      <c r="R8" s="144"/>
+      <c r="S8" s="144"/>
+      <c r="T8" s="143"/>
+      <c r="U8" s="144"/>
+      <c r="V8" s="138"/>
+      <c r="W8" s="139"/>
+      <c r="X8" s="143"/>
+      <c r="Y8" s="144"/>
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:31" ht="10" customHeight="1">
@@ -2580,30 +2604,30 @@
         <v>13</v>
       </c>
       <c r="C9" s="81"/>
-      <c r="D9" s="150" t="s">
+      <c r="D9" s="147" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="149"/>
-      <c r="F9" s="148"/>
-      <c r="G9" s="149"/>
-      <c r="H9" s="148"/>
-      <c r="I9" s="149"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="149"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="150"/>
-      <c r="N9" s="151"/>
-      <c r="O9" s="149"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="149"/>
-      <c r="R9" s="148"/>
-      <c r="S9" s="149"/>
-      <c r="T9" s="148"/>
-      <c r="U9" s="150"/>
-      <c r="V9" s="151"/>
-      <c r="W9" s="149"/>
-      <c r="X9" s="148"/>
-      <c r="Y9" s="149"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="145"/>
+      <c r="G9" s="146"/>
+      <c r="H9" s="145"/>
+      <c r="I9" s="146"/>
+      <c r="J9" s="145"/>
+      <c r="K9" s="146"/>
+      <c r="L9" s="145"/>
+      <c r="M9" s="147"/>
+      <c r="N9" s="148"/>
+      <c r="O9" s="146"/>
+      <c r="P9" s="145"/>
+      <c r="Q9" s="146"/>
+      <c r="R9" s="145"/>
+      <c r="S9" s="146"/>
+      <c r="T9" s="145"/>
+      <c r="U9" s="147"/>
+      <c r="V9" s="148"/>
+      <c r="W9" s="146"/>
+      <c r="X9" s="145"/>
+      <c r="Y9" s="146"/>
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:31" s="3" customFormat="1" ht="7" customHeight="1">
@@ -2632,10 +2656,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="83"/>
-      <c r="D11" s="168" t="s">
+      <c r="D11" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="169"/>
+      <c r="E11" s="159"/>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
       <c r="H11" s="13"/>
@@ -3069,8 +3093,8 @@
       <c r="A26" s="1"/>
       <c r="B26" s="78"/>
       <c r="C26" s="79"/>
-      <c r="D26" s="166"/>
-      <c r="E26" s="167"/>
+      <c r="D26" s="156"/>
+      <c r="E26" s="157"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
       <c r="H26" s="13"/>
@@ -3118,10 +3142,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="85"/>
-      <c r="D28" s="164" t="s">
+      <c r="D28" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="165"/>
+      <c r="E28" s="155"/>
       <c r="F28" s="33"/>
       <c r="G28" s="34"/>
       <c r="H28" s="33"/>
@@ -4275,7 +4299,7 @@
       <c r="L68" s="43"/>
       <c r="M68" s="42"/>
       <c r="N68" s="102"/>
-      <c r="O68" s="67"/>
+      <c r="O68" s="49"/>
       <c r="P68" s="43"/>
       <c r="Q68" s="40"/>
       <c r="R68" s="41"/>
@@ -5144,10 +5168,10 @@
     </row>
     <row r="99" spans="1:26" ht="10" customHeight="1">
       <c r="A99" s="1"/>
-      <c r="B99" s="134"/>
-      <c r="C99" s="135"/>
-      <c r="D99" s="135"/>
-      <c r="E99" s="136"/>
+      <c r="B99" s="161"/>
+      <c r="C99" s="162"/>
+      <c r="D99" s="162"/>
+      <c r="E99" s="163"/>
       <c r="F99" s="13"/>
       <c r="G99" s="14"/>
       <c r="H99" s="13"/>
@@ -5396,10 +5420,10 @@
       <c r="Z107" s="2"/>
     </row>
     <row r="108" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B108" s="134"/>
-      <c r="C108" s="135"/>
-      <c r="D108" s="135"/>
-      <c r="E108" s="136"/>
+      <c r="B108" s="161"/>
+      <c r="C108" s="162"/>
+      <c r="D108" s="162"/>
+      <c r="E108" s="163"/>
       <c r="F108" s="13"/>
       <c r="G108" s="14"/>
       <c r="H108" s="13"/>
@@ -5423,9 +5447,9 @@
       <c r="Z108" s="2"/>
     </row>
     <row r="109" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
-      <c r="B109" s="153"/>
-      <c r="C109" s="153"/>
-      <c r="D109" s="153"/>
+      <c r="B109" s="160"/>
+      <c r="C109" s="160"/>
+      <c r="D109" s="160"/>
       <c r="E109" s="32"/>
       <c r="F109" s="2"/>
       <c r="H109" s="2"/>
@@ -5981,23 +6005,8 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C97:E98"/>
-    <mergeCell ref="C29:E30"/>
-    <mergeCell ref="B108:E108"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="C67:E68"/>
-    <mergeCell ref="C69:E70"/>
-    <mergeCell ref="C44:E45"/>
-    <mergeCell ref="C86:E87"/>
-    <mergeCell ref="C56:E57"/>
     <mergeCell ref="C81:E82"/>
     <mergeCell ref="C52:E53"/>
-    <mergeCell ref="C106:D107"/>
     <mergeCell ref="B5:C6"/>
     <mergeCell ref="P9:Q9"/>
     <mergeCell ref="F2:G8"/>
@@ -6013,11 +6022,32 @@
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="E3:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C33:E34"/>
+    <mergeCell ref="C58:E59"/>
+    <mergeCell ref="C37:E38"/>
+    <mergeCell ref="C54:E55"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="C46:E47"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="C44:E45"/>
+    <mergeCell ref="C56:E57"/>
     <mergeCell ref="C50:E51"/>
     <mergeCell ref="C42:E43"/>
     <mergeCell ref="B109:D109"/>
     <mergeCell ref="C48:E49"/>
+    <mergeCell ref="C104:E105"/>
+    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="C106:D107"/>
+    <mergeCell ref="C97:E98"/>
+    <mergeCell ref="B108:E108"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="C67:E68"/>
+    <mergeCell ref="C69:E70"/>
+    <mergeCell ref="C86:E87"/>
     <mergeCell ref="B7:C8"/>
     <mergeCell ref="C31:E32"/>
     <mergeCell ref="C24:E25"/>
@@ -6030,8 +6060,8 @@
     <mergeCell ref="C18:E19"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="C104:E105"/>
-    <mergeCell ref="B99:E99"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C29:E30"/>
     <mergeCell ref="V2:W8"/>
     <mergeCell ref="X2:Y8"/>
     <mergeCell ref="R9:S9"/>
@@ -6040,12 +6070,6 @@
     <mergeCell ref="X9:Y9"/>
     <mergeCell ref="T2:U8"/>
     <mergeCell ref="R2:S8"/>
-    <mergeCell ref="C33:E34"/>
-    <mergeCell ref="C58:E59"/>
-    <mergeCell ref="C37:E38"/>
-    <mergeCell ref="C54:E55"/>
-    <mergeCell ref="C35:E36"/>
-    <mergeCell ref="C46:E47"/>
     <mergeCell ref="E110:E111"/>
     <mergeCell ref="C71:E72"/>
     <mergeCell ref="C65:E66"/>
@@ -6065,6 +6089,7 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="8" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6082,6 +6107,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6099,6 +6125,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Version 0.6 abgeschlossen und verschiedene Bilder und grafiken der Struktur hinzugefügt.
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="540" windowWidth="34640" windowHeight="22900"/>
+    <workbookView xWindow="1060" yWindow="0" windowWidth="34640" windowHeight="24560"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Zeitplan erstellen</t>
   </si>
@@ -288,14 +288,36 @@
     <t>Systemstruktur</t>
   </si>
   <si>
-    <t>Profil definieren in einem Branch des Pakest "eGov"</t>
-  </si>
-  <si>
     <t>Installationsskript erstellen</t>
   </si>
   <si>
     <t>Runskript erarbeiten in einem Branch
  des Pakets "teamraum-buildout"</t>
+  </si>
+  <si>
+    <r>
+      <t>18.5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>16.5</t>
+    </r>
+  </si>
+  <si>
+    <t>Profil definieren in einem Branch des Pakets "eGov"</t>
   </si>
 </sst>
 </file>
@@ -1408,6 +1430,96 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1420,36 +1532,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1461,66 +1543,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="165">
@@ -2330,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="AA19" sqref="AA19"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -2376,10 +2398,10 @@
     </row>
     <row r="2" spans="1:31" ht="16" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="166"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
       <c r="F2" s="140" t="s">
         <v>14</v>
       </c>
@@ -2429,7 +2451,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="168"/>
+      <c r="E3" s="173"/>
       <c r="F3" s="141"/>
       <c r="G3" s="142"/>
       <c r="H3" s="141"/>
@@ -2459,7 +2481,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="168"/>
+      <c r="E4" s="173"/>
       <c r="F4" s="141"/>
       <c r="G4" s="142"/>
       <c r="H4" s="141"/>
@@ -2484,12 +2506,12 @@
     </row>
     <row r="5" spans="1:31" ht="7" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="164" t="s">
+      <c r="B5" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="165"/>
+      <c r="C5" s="185"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="168"/>
+      <c r="E5" s="173"/>
       <c r="F5" s="141"/>
       <c r="G5" s="142"/>
       <c r="H5" s="141"/>
@@ -2514,10 +2536,10 @@
     </row>
     <row r="6" spans="1:31" ht="7" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="164"/>
-      <c r="C6" s="165"/>
+      <c r="B6" s="184"/>
+      <c r="C6" s="185"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="168"/>
+      <c r="E6" s="173"/>
       <c r="F6" s="141"/>
       <c r="G6" s="142"/>
       <c r="H6" s="141"/>
@@ -2542,12 +2564,12 @@
     </row>
     <row r="7" spans="1:31" ht="7" customHeight="1" thickBot="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="180" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="151"/>
+      <c r="C7" s="181"/>
       <c r="D7" s="108"/>
-      <c r="E7" s="168"/>
+      <c r="E7" s="173"/>
       <c r="F7" s="141"/>
       <c r="G7" s="142"/>
       <c r="H7" s="141"/>
@@ -2572,10 +2594,10 @@
     </row>
     <row r="8" spans="1:31" ht="7" customHeight="1" thickTop="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="152"/>
-      <c r="C8" s="153"/>
+      <c r="B8" s="182"/>
+      <c r="C8" s="183"/>
       <c r="D8" s="107"/>
-      <c r="E8" s="169"/>
+      <c r="E8" s="174"/>
       <c r="F8" s="143"/>
       <c r="G8" s="144"/>
       <c r="H8" s="143"/>
@@ -2656,10 +2678,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="83"/>
-      <c r="D11" s="158" t="s">
+      <c r="D11" s="152" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="159"/>
+      <c r="E11" s="153"/>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
       <c r="H11" s="13"/>
@@ -3093,8 +3115,8 @@
       <c r="A26" s="1"/>
       <c r="B26" s="78"/>
       <c r="C26" s="79"/>
-      <c r="D26" s="156"/>
-      <c r="E26" s="157"/>
+      <c r="D26" s="150"/>
+      <c r="E26" s="151"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
       <c r="H26" s="13"/>
@@ -3460,10 +3482,10 @@
     </row>
     <row r="39" spans="1:26" ht="10" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="172"/>
-      <c r="C39" s="173"/>
-      <c r="D39" s="173"/>
-      <c r="E39" s="174"/>
+      <c r="B39" s="175"/>
+      <c r="C39" s="176"/>
+      <c r="D39" s="176"/>
+      <c r="E39" s="177"/>
       <c r="F39" s="33"/>
       <c r="G39" s="34"/>
       <c r="H39" s="33"/>
@@ -3511,10 +3533,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="87"/>
-      <c r="D41" s="175">
-        <v>12</v>
-      </c>
-      <c r="E41" s="176"/>
+      <c r="D41" s="178" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="179"/>
       <c r="F41" s="52"/>
       <c r="G41" s="53"/>
       <c r="H41" s="52"/>
@@ -4061,10 +4083,10 @@
     </row>
     <row r="60" spans="1:26" ht="10" customHeight="1">
       <c r="A60" s="1"/>
-      <c r="B60" s="177"/>
-      <c r="C60" s="178"/>
-      <c r="D60" s="178"/>
-      <c r="E60" s="179"/>
+      <c r="B60" s="162"/>
+      <c r="C60" s="163"/>
+      <c r="D60" s="163"/>
+      <c r="E60" s="164"/>
       <c r="F60" s="52"/>
       <c r="G60" s="53"/>
       <c r="H60" s="52"/>
@@ -4112,10 +4134,10 @@
         <v>5</v>
       </c>
       <c r="C62" s="89"/>
-      <c r="D62" s="180">
-        <v>28</v>
-      </c>
-      <c r="E62" s="181"/>
+      <c r="D62" s="165">
+        <v>25.5</v>
+      </c>
+      <c r="E62" s="166"/>
       <c r="F62" s="69"/>
       <c r="G62" s="70"/>
       <c r="H62" s="69"/>
@@ -4258,7 +4280,7 @@
       <c r="A67" s="1"/>
       <c r="B67" s="72"/>
       <c r="C67" s="114" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D67" s="115"/>
       <c r="E67" s="116"/>
@@ -4287,9 +4309,9 @@
     <row r="68" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A68" s="1"/>
       <c r="B68" s="72"/>
-      <c r="C68" s="185"/>
-      <c r="D68" s="186"/>
-      <c r="E68" s="187"/>
+      <c r="C68" s="170"/>
+      <c r="D68" s="171"/>
+      <c r="E68" s="172"/>
       <c r="F68" s="43"/>
       <c r="G68" s="56"/>
       <c r="H68" s="43"/>
@@ -4300,8 +4322,8 @@
       <c r="M68" s="42"/>
       <c r="N68" s="102"/>
       <c r="O68" s="49"/>
-      <c r="P68" s="43"/>
-      <c r="Q68" s="40"/>
+      <c r="P68" s="45"/>
+      <c r="Q68" s="49"/>
       <c r="R68" s="41"/>
       <c r="S68" s="42"/>
       <c r="T68" s="43"/>
@@ -4316,7 +4338,7 @@
       <c r="A69" s="1"/>
       <c r="B69" s="72"/>
       <c r="C69" s="114" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D69" s="115"/>
       <c r="E69" s="116"/>
@@ -4374,7 +4396,7 @@
       <c r="A71" s="1"/>
       <c r="B71" s="72"/>
       <c r="C71" s="114" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D71" s="115"/>
       <c r="E71" s="116"/>
@@ -4720,10 +4742,10 @@
     </row>
     <row r="83" spans="1:26" ht="10" customHeight="1">
       <c r="A83" s="1"/>
-      <c r="B83" s="182"/>
-      <c r="C83" s="183"/>
-      <c r="D83" s="183"/>
-      <c r="E83" s="184"/>
+      <c r="B83" s="167"/>
+      <c r="C83" s="168"/>
+      <c r="D83" s="168"/>
+      <c r="E83" s="169"/>
       <c r="F83" s="69"/>
       <c r="G83" s="70"/>
       <c r="H83" s="69"/>
@@ -4772,7 +4794,7 @@
       </c>
       <c r="C85" s="91"/>
       <c r="D85" s="126">
-        <v>12</v>
+        <v>9.5</v>
       </c>
       <c r="E85" s="127"/>
       <c r="F85" s="60"/>
@@ -4967,7 +4989,7 @@
       </c>
       <c r="C92" s="93"/>
       <c r="D92" s="121">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="E92" s="122"/>
       <c r="F92" s="13"/>
@@ -5038,8 +5060,8 @@
       <c r="M94" s="42"/>
       <c r="N94" s="110"/>
       <c r="O94" s="40"/>
-      <c r="P94" s="43"/>
-      <c r="Q94" s="40"/>
+      <c r="P94" s="45"/>
+      <c r="Q94" s="49"/>
       <c r="R94" s="41"/>
       <c r="S94" s="42"/>
       <c r="T94" s="43"/>
@@ -5168,10 +5190,10 @@
     </row>
     <row r="99" spans="1:26" ht="10" customHeight="1">
       <c r="A99" s="1"/>
-      <c r="B99" s="161"/>
-      <c r="C99" s="162"/>
-      <c r="D99" s="162"/>
-      <c r="E99" s="163"/>
+      <c r="B99" s="157"/>
+      <c r="C99" s="158"/>
+      <c r="D99" s="158"/>
+      <c r="E99" s="159"/>
       <c r="F99" s="13"/>
       <c r="G99" s="14"/>
       <c r="H99" s="13"/>
@@ -5219,8 +5241,8 @@
         <v>26</v>
       </c>
       <c r="C101" s="93"/>
-      <c r="D101" s="170"/>
-      <c r="E101" s="171"/>
+      <c r="D101" s="160"/>
+      <c r="E101" s="161"/>
       <c r="F101" s="13"/>
       <c r="G101" s="14"/>
       <c r="H101" s="13"/>
@@ -5407,8 +5429,8 @@
       <c r="M107" s="66"/>
       <c r="N107" s="102"/>
       <c r="O107" s="67"/>
-      <c r="P107" s="47"/>
-      <c r="Q107" s="67"/>
+      <c r="P107" s="45"/>
+      <c r="Q107" s="49"/>
       <c r="R107" s="65"/>
       <c r="S107" s="66"/>
       <c r="T107" s="47"/>
@@ -5420,10 +5442,10 @@
       <c r="Z107" s="2"/>
     </row>
     <row r="108" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B108" s="161"/>
-      <c r="C108" s="162"/>
-      <c r="D108" s="162"/>
-      <c r="E108" s="163"/>
+      <c r="B108" s="157"/>
+      <c r="C108" s="158"/>
+      <c r="D108" s="158"/>
+      <c r="E108" s="159"/>
       <c r="F108" s="13"/>
       <c r="G108" s="14"/>
       <c r="H108" s="13"/>
@@ -5447,9 +5469,9 @@
       <c r="Z108" s="2"/>
     </row>
     <row r="109" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
-      <c r="B109" s="160"/>
-      <c r="C109" s="160"/>
-      <c r="D109" s="160"/>
+      <c r="B109" s="156"/>
+      <c r="C109" s="156"/>
+      <c r="D109" s="156"/>
       <c r="E109" s="32"/>
       <c r="F109" s="2"/>
       <c r="H109" s="2"/>
@@ -6005,6 +6027,8 @@
     </row>
   </sheetData>
   <mergeCells count="81">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C24:E25"/>
     <mergeCell ref="C81:E82"/>
     <mergeCell ref="C52:E53"/>
     <mergeCell ref="B5:C6"/>
@@ -6020,7 +6044,7 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C86:E87"/>
     <mergeCell ref="E3:E8"/>
     <mergeCell ref="C33:E34"/>
     <mergeCell ref="C58:E59"/>
@@ -6034,6 +6058,11 @@
     <mergeCell ref="C56:E57"/>
     <mergeCell ref="C50:E51"/>
     <mergeCell ref="C42:E43"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="C31:E32"/>
+    <mergeCell ref="C20:E21"/>
+    <mergeCell ref="C22:E23"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="B109:D109"/>
     <mergeCell ref="C48:E49"/>
     <mergeCell ref="C104:E105"/>
@@ -6047,20 +6076,6 @@
     <mergeCell ref="B83:E83"/>
     <mergeCell ref="C67:E68"/>
     <mergeCell ref="C69:E70"/>
-    <mergeCell ref="C86:E87"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="C31:E32"/>
-    <mergeCell ref="C24:E25"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C14:E15"/>
-    <mergeCell ref="C20:E21"/>
-    <mergeCell ref="C22:E23"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="C12:E13"/>
-    <mergeCell ref="C18:E19"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="C29:E30"/>
     <mergeCell ref="V2:W8"/>
     <mergeCell ref="X2:Y8"/>
@@ -6070,6 +6085,13 @@
     <mergeCell ref="X9:Y9"/>
     <mergeCell ref="T2:U8"/>
     <mergeCell ref="R2:S8"/>
+    <mergeCell ref="C12:E13"/>
+    <mergeCell ref="C18:E19"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C14:E15"/>
     <mergeCell ref="E110:E111"/>
     <mergeCell ref="C71:E72"/>
     <mergeCell ref="C65:E66"/>
@@ -6089,7 +6111,6 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup paperSize="8" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Bilder hinzugefügt und Dokumentation 0.7 angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="0" windowWidth="34640" windowHeight="24560"/>
+    <workbookView xWindow="4160" yWindow="4640" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -291,10 +291,6 @@
     <t>Installationsskript erstellen</t>
   </si>
   <si>
-    <t>Runskript erarbeiten in einem Branch
- des Pakets "teamraum-buildout"</t>
-  </si>
-  <si>
     <r>
       <t>18.5</t>
     </r>
@@ -318,6 +314,10 @@
   </si>
   <si>
     <t>Profil definieren in einem Branch des Pakets "eGov"</t>
+  </si>
+  <si>
+    <t>Runskript erarbeiten in einem Branch
+ des Pakets buildout-base"</t>
   </si>
 </sst>
 </file>
@@ -1430,24 +1430,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1532,17 +1514,35 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="165">
@@ -2352,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="Z62" sqref="Z62"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="S74" sqref="S74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -2398,10 +2398,10 @@
     </row>
     <row r="2" spans="1:31" ht="16" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="186"/>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="187"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
       <c r="F2" s="140" t="s">
         <v>14</v>
       </c>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="173"/>
+      <c r="E3" s="167"/>
       <c r="F3" s="141"/>
       <c r="G3" s="142"/>
       <c r="H3" s="141"/>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="173"/>
+      <c r="E4" s="167"/>
       <c r="F4" s="141"/>
       <c r="G4" s="142"/>
       <c r="H4" s="141"/>
@@ -2506,12 +2506,12 @@
     </row>
     <row r="5" spans="1:31" ht="7" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="184" t="s">
+      <c r="B5" s="180" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="185"/>
+      <c r="C5" s="181"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="173"/>
+      <c r="E5" s="167"/>
       <c r="F5" s="141"/>
       <c r="G5" s="142"/>
       <c r="H5" s="141"/>
@@ -2536,10 +2536,10 @@
     </row>
     <row r="6" spans="1:31" ht="7" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="185"/>
+      <c r="B6" s="180"/>
+      <c r="C6" s="181"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="173"/>
+      <c r="E6" s="167"/>
       <c r="F6" s="141"/>
       <c r="G6" s="142"/>
       <c r="H6" s="141"/>
@@ -2564,12 +2564,12 @@
     </row>
     <row r="7" spans="1:31" ht="7" customHeight="1" thickBot="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="180" t="s">
+      <c r="B7" s="174" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="181"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="108"/>
-      <c r="E7" s="173"/>
+      <c r="E7" s="167"/>
       <c r="F7" s="141"/>
       <c r="G7" s="142"/>
       <c r="H7" s="141"/>
@@ -2594,10 +2594,10 @@
     </row>
     <row r="8" spans="1:31" ht="7" customHeight="1" thickTop="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="182"/>
-      <c r="C8" s="183"/>
+      <c r="B8" s="176"/>
+      <c r="C8" s="177"/>
       <c r="D8" s="107"/>
-      <c r="E8" s="174"/>
+      <c r="E8" s="168"/>
       <c r="F8" s="143"/>
       <c r="G8" s="144"/>
       <c r="H8" s="143"/>
@@ -2678,10 +2678,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="83"/>
-      <c r="D11" s="152" t="s">
+      <c r="D11" s="186" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="153"/>
+      <c r="E11" s="187"/>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
       <c r="H11" s="13"/>
@@ -3115,8 +3115,8 @@
       <c r="A26" s="1"/>
       <c r="B26" s="78"/>
       <c r="C26" s="79"/>
-      <c r="D26" s="150"/>
-      <c r="E26" s="151"/>
+      <c r="D26" s="184"/>
+      <c r="E26" s="185"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
       <c r="H26" s="13"/>
@@ -3164,10 +3164,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="85"/>
-      <c r="D28" s="154" t="s">
+      <c r="D28" s="182" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="155"/>
+      <c r="E28" s="183"/>
       <c r="F28" s="33"/>
       <c r="G28" s="34"/>
       <c r="H28" s="33"/>
@@ -3482,10 +3482,10 @@
     </row>
     <row r="39" spans="1:26" ht="10" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="175"/>
-      <c r="C39" s="176"/>
-      <c r="D39" s="176"/>
-      <c r="E39" s="177"/>
+      <c r="B39" s="169"/>
+      <c r="C39" s="170"/>
+      <c r="D39" s="170"/>
+      <c r="E39" s="171"/>
       <c r="F39" s="33"/>
       <c r="G39" s="34"/>
       <c r="H39" s="33"/>
@@ -3533,10 +3533,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="87"/>
-      <c r="D41" s="178" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="179"/>
+      <c r="D41" s="172" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="173"/>
       <c r="F41" s="52"/>
       <c r="G41" s="53"/>
       <c r="H41" s="52"/>
@@ -4083,10 +4083,10 @@
     </row>
     <row r="60" spans="1:26" ht="10" customHeight="1">
       <c r="A60" s="1"/>
-      <c r="B60" s="162"/>
-      <c r="C60" s="163"/>
-      <c r="D60" s="163"/>
-      <c r="E60" s="164"/>
+      <c r="B60" s="156"/>
+      <c r="C60" s="157"/>
+      <c r="D60" s="157"/>
+      <c r="E60" s="158"/>
       <c r="F60" s="52"/>
       <c r="G60" s="53"/>
       <c r="H60" s="52"/>
@@ -4134,10 +4134,10 @@
         <v>5</v>
       </c>
       <c r="C62" s="89"/>
-      <c r="D62" s="165">
+      <c r="D62" s="159">
         <v>25.5</v>
       </c>
-      <c r="E62" s="166"/>
+      <c r="E62" s="160"/>
       <c r="F62" s="69"/>
       <c r="G62" s="70"/>
       <c r="H62" s="69"/>
@@ -4309,9 +4309,9 @@
     <row r="68" spans="1:26" ht="10" customHeight="1" thickBot="1">
       <c r="A68" s="1"/>
       <c r="B68" s="72"/>
-      <c r="C68" s="170"/>
-      <c r="D68" s="171"/>
-      <c r="E68" s="172"/>
+      <c r="C68" s="164"/>
+      <c r="D68" s="165"/>
+      <c r="E68" s="166"/>
       <c r="F68" s="43"/>
       <c r="G68" s="56"/>
       <c r="H68" s="43"/>
@@ -4338,7 +4338,7 @@
       <c r="A69" s="1"/>
       <c r="B69" s="72"/>
       <c r="C69" s="114" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D69" s="115"/>
       <c r="E69" s="116"/>
@@ -4382,7 +4382,7 @@
       <c r="O70" s="40"/>
       <c r="P70" s="43"/>
       <c r="Q70" s="40"/>
-      <c r="R70" s="41"/>
+      <c r="R70" s="76"/>
       <c r="S70" s="42"/>
       <c r="T70" s="43"/>
       <c r="U70" s="42"/>
@@ -4396,7 +4396,7 @@
       <c r="A71" s="1"/>
       <c r="B71" s="72"/>
       <c r="C71" s="114" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D71" s="115"/>
       <c r="E71" s="116"/>
@@ -4440,8 +4440,8 @@
       <c r="O72" s="40"/>
       <c r="P72" s="43"/>
       <c r="Q72" s="40"/>
-      <c r="R72" s="41"/>
-      <c r="S72" s="42"/>
+      <c r="R72" s="65"/>
+      <c r="S72" s="77"/>
       <c r="T72" s="43"/>
       <c r="U72" s="42"/>
       <c r="V72" s="100"/>
@@ -4499,7 +4499,7 @@
       <c r="P74" s="43"/>
       <c r="Q74" s="40"/>
       <c r="R74" s="41"/>
-      <c r="S74" s="42"/>
+      <c r="S74" s="66"/>
       <c r="T74" s="43"/>
       <c r="U74" s="42"/>
       <c r="V74" s="100"/>
@@ -4742,10 +4742,10 @@
     </row>
     <row r="83" spans="1:26" ht="10" customHeight="1">
       <c r="A83" s="1"/>
-      <c r="B83" s="167"/>
-      <c r="C83" s="168"/>
-      <c r="D83" s="168"/>
-      <c r="E83" s="169"/>
+      <c r="B83" s="161"/>
+      <c r="C83" s="162"/>
+      <c r="D83" s="162"/>
+      <c r="E83" s="163"/>
       <c r="F83" s="69"/>
       <c r="G83" s="70"/>
       <c r="H83" s="69"/>
@@ -5190,10 +5190,10 @@
     </row>
     <row r="99" spans="1:26" ht="10" customHeight="1">
       <c r="A99" s="1"/>
-      <c r="B99" s="157"/>
-      <c r="C99" s="158"/>
-      <c r="D99" s="158"/>
-      <c r="E99" s="159"/>
+      <c r="B99" s="151"/>
+      <c r="C99" s="152"/>
+      <c r="D99" s="152"/>
+      <c r="E99" s="153"/>
       <c r="F99" s="13"/>
       <c r="G99" s="14"/>
       <c r="H99" s="13"/>
@@ -5241,8 +5241,8 @@
         <v>26</v>
       </c>
       <c r="C101" s="93"/>
-      <c r="D101" s="160"/>
-      <c r="E101" s="161"/>
+      <c r="D101" s="154"/>
+      <c r="E101" s="155"/>
       <c r="F101" s="13"/>
       <c r="G101" s="14"/>
       <c r="H101" s="13"/>
@@ -5442,10 +5442,10 @@
       <c r="Z107" s="2"/>
     </row>
     <row r="108" spans="1:26" s="3" customFormat="1" ht="10" customHeight="1">
-      <c r="B108" s="157"/>
-      <c r="C108" s="158"/>
-      <c r="D108" s="158"/>
-      <c r="E108" s="159"/>
+      <c r="B108" s="151"/>
+      <c r="C108" s="152"/>
+      <c r="D108" s="152"/>
+      <c r="E108" s="153"/>
       <c r="F108" s="13"/>
       <c r="G108" s="14"/>
       <c r="H108" s="13"/>
@@ -5469,9 +5469,9 @@
       <c r="Z108" s="2"/>
     </row>
     <row r="109" spans="1:26" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
-      <c r="B109" s="156"/>
-      <c r="C109" s="156"/>
-      <c r="D109" s="156"/>
+      <c r="B109" s="150"/>
+      <c r="C109" s="150"/>
+      <c r="D109" s="150"/>
       <c r="E109" s="32"/>
       <c r="F109" s="2"/>
       <c r="H109" s="2"/>
@@ -6032,6 +6032,17 @@
     <mergeCell ref="C81:E82"/>
     <mergeCell ref="C52:E53"/>
     <mergeCell ref="B5:C6"/>
+    <mergeCell ref="C20:E21"/>
+    <mergeCell ref="C22:E23"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="C12:E13"/>
+    <mergeCell ref="C18:E19"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C14:E15"/>
     <mergeCell ref="P9:Q9"/>
     <mergeCell ref="F2:G8"/>
     <mergeCell ref="H2:I8"/>
@@ -6044,7 +6055,6 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="C86:E87"/>
     <mergeCell ref="E3:E8"/>
     <mergeCell ref="C33:E34"/>
     <mergeCell ref="C58:E59"/>
@@ -6060,9 +6070,6 @@
     <mergeCell ref="C42:E43"/>
     <mergeCell ref="B7:C8"/>
     <mergeCell ref="C31:E32"/>
-    <mergeCell ref="C20:E21"/>
-    <mergeCell ref="C22:E23"/>
-    <mergeCell ref="D28:E28"/>
     <mergeCell ref="B109:D109"/>
     <mergeCell ref="C48:E49"/>
     <mergeCell ref="C104:E105"/>
@@ -6076,7 +6083,7 @@
     <mergeCell ref="B83:E83"/>
     <mergeCell ref="C67:E68"/>
     <mergeCell ref="C69:E70"/>
-    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="C86:E87"/>
     <mergeCell ref="V2:W8"/>
     <mergeCell ref="X2:Y8"/>
     <mergeCell ref="R9:S9"/>
@@ -6085,13 +6092,6 @@
     <mergeCell ref="X9:Y9"/>
     <mergeCell ref="T2:U8"/>
     <mergeCell ref="R2:S8"/>
-    <mergeCell ref="C12:E13"/>
-    <mergeCell ref="C18:E19"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C14:E15"/>
     <mergeCell ref="E110:E111"/>
     <mergeCell ref="C71:E72"/>
     <mergeCell ref="C65:E66"/>
@@ -6111,6 +6111,7 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>